<commit_message>
Added Combat Calendar to displays
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6B7801E-2E8A-4672-BF03-6C2CB3E61A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{670F6BD4-F22D-4727-90D3-B700D7EA3113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,14 @@
   </si>
   <si>
     <t>&lt;Bold&gt;e001 Fourth Armor Division Campaign&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r1.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The campaign game of &lt;Bold&gt;Patton' Best&lt;/Bold&gt; recreates the actions of the 4th Armored Division from late July 1944 through April 1945. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Each day begins with a check of the Combat Calendar &lt;InlineUIContainer&gt;&lt;Button Content='cc' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; to see what the Division was doing on that day. The four possibilities are Refitting &lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, an Advance scenario &lt;InlineUIContainer&gt;&lt;Button Content='r20.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, a Battle scenario &lt;InlineUIContainer&gt;&lt;Button Content='r20.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, or a Counterattack scenario &lt;InlineUIContainer&gt;&lt;Button Content='r20.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The campaign game of &lt;Bold&gt;Patton' Best&lt;/Bold&gt; recreates the actions of the 4th Armored Division from late July 1944 through April 1945. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Each day begins with a check of the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; to see
+ what the Division was doing on that day. The four possibilities are Refitting &lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
+an Advance scenario &lt;InlineUIContainer&gt;&lt;Button Content='r20.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
+a Battle scenario &lt;InlineUIContainer&gt;&lt;Button Content='r20.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
+or a Counterattack scenario &lt;InlineUIContainer&gt;&lt;Button Content='r20.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Nothing' Source='../images/Nothing.gif' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
@@ -471,16 +476,16 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="152" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="181.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -488,7 +493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +501,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -504,7 +509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -512,7 +517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="128.44999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -520,7 +525,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -528,7 +533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Fix issue with die roll not showing up. Worked on initial combat calendar check.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1320D12-6C3F-403D-BC50-F2921C2F00C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F509C595-C9E8-4749-8A03-18BA36DDFEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -165,14 +165,19 @@
                                    &lt;InlineUIContainer&gt;&lt;Image Name='MapMovement'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e006 Combat Calendar Check&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Date from Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;: DATE&lt;LineBreak/&gt;
+    <t xml:space="preserve">&lt;Bold&gt;e006 Combat Calendar Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll for possible combat today. If die &amp;lt;= probability, start morning briefing per 
+&lt;InlineUIContainer&gt;&lt;Button Content='e007' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  
+Otherwise continue with next day check.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Date from Combat Calendar: DATE&lt;LineBreak/&gt;
 Expected Resistance: RESISTANCE&lt;LineBreak/&gt;
-Probablility of Combat: PROBABILITY &gt; &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-&lt;LineBreak/&gt;
-If the roll is equal or less than the probability, start morning briefing &lt;InlineUIContainer&gt;&lt;Button Content='e007' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the roll is greater than the probability, move to the next day.</t>
+Probablility of Combat: PROBABILITY &amp;gt;= &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+</t>
   </si>
 </sst>
 </file>
@@ -596,7 +601,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Got initial combat caledar check loop working
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F509C595-C9E8-4749-8A03-18BA36DDFEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9A378F5C-CA17-4690-9F21-6AA868469587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -145,16 +145,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Name='Read_Rules' Content='Read Rules' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt; or &lt;InlineUIContainer&gt;&lt;Button Name='Begin' Content='Begin Game' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>e008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e008 Morning Briefing - Weather Roll&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Consult weather table &lt;InlineUIContainer&gt;&lt;Button Content='tWeather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; after rolling to determine weather for today:
-&lt;InlineUIContainer&gt;&lt;Image Name='DiceRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e002 Movement Board&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The movement board is a depiction fo typical European countryside and is used to show the "big picture" for the day. The movement board is divided into white lines into areas. Click image to continue.
@@ -165,7 +155,19 @@
                                    &lt;InlineUIContainer&gt;&lt;Image Name='MapMovement'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;e006 Combat Calendar Check&lt;/Bold&gt; 
+    <t>e007</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Consult weather table 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+after rolling to determine weather for today:
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e006 Combat Calendar Check&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -175,9 +177,9 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Date from Combat Calendar: DATE&lt;LineBreak/&gt;
 Expected Resistance: RESISTANCE&lt;LineBreak/&gt;
-Probablility of Combat: PROBABILITY &amp;gt;= &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-</t>
+Probablility of Combat: PROBABILITY &amp;gt;= 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -543,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -574,7 +576,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -609,12 +611,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
starting to develop crew ratings
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{770F9648-4F0A-4E77-9EC0-1F0FFD4C0776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3B0C271A-CFE9-42A7-B20C-E32AED6DE54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -111,20 +111,6 @@
                                    &lt;InlineUIContainer&gt;&lt;Image Name='MapBattle'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e004 Tank Card&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The upper right image is the Tank Card. The game starts with the basic M4 Sherman tank, i.e., Tank Card #1. The Tank Card shows the tank model and other important information regarding the tank. The use of the Tank Card is described in &lt;InlineUIContainer&gt;&lt;Button Content='r5.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                 &lt;InlineUIContainer&gt;&lt;Image Name='m001M4'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e005 After Action Report (AAR)&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The events of each engagement or day of battle are recorded as they unfold on the After Action Report. At this time, you may elect to change the name of the tank or the names of your crew by clicking on the appropriate location on the form. When ready, click image below to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue005' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e000 Welcome to Patton's Best Solo Tank Battle Game&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The game starts with a tutorial how to play. However, before starting, it is important to know that Active events are shown with a green background. The game may only advance when a green background is displayed. Most often, the game advances by rolling dice or clicking an image. 
@@ -185,6 +171,24 @@
  Table determines weather for today:  
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e005 After Action Report (AAR)&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The events of each engagement or day of battle are recorded as they unfold on the After Action Report. At this time, you may elect to change the name of the tank or the names of your crew by clicking on the appropriate location on the form. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When ready, click image below to assign crew ratings to your new crew per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r7.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue005' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e004 Tank Card&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The upper right image is the Tank Card. The game starts with the basic M4 Sherman tank, i.e., Tank Card #1. 
+The Tank Card shows the tank model and other important information regarding the tank. The use of the Tank Card is described in 
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                 &lt;InlineUIContainer&gt;&lt;Image Name='m001M4'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -550,14 +554,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="175.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="175.25" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -565,15 +569,15 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="210.1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -581,10 +585,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="104.95" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -592,39 +596,39 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -632,7 +636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -640,7 +644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="128.44999999999999" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,7 +652,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -656,7 +660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
checkpointing - ready rack work
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C6CC4CFA-1D72-4CF0-8219-BB2B2A200B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6D81B2C7-BFD1-4F59-B5F3-A4676B1D42A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>e001</t>
   </si>
@@ -204,22 +204,6 @@
  Table:  
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e009a</t>
-  </si>
-  <si>
-    <t>e009b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e009a Loading Normal Ammo&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e009b Loading Extra Ammo&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r16.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e008 Ammo Loading Limits&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r16.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
@@ -233,6 +217,17 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 -- &lt;Bold&gt;AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
 -- &lt;Bold&gt;HE:&lt;/Bold&gt; Unlimited</t>
+  </si>
+  <si>
+    <t>e010</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. The same die roll is used to determine the ammo expended:
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
 </sst>
 </file>
@@ -596,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -685,62 +680,54 @@
         <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started Time Check work
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6D81B2C7-BFD1-4F59-B5F3-A4676B1D42A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{513C74B4-0296-498E-958C-1724768713DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -224,10 +224,11 @@
   <si>
     <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. The same die roll is used to determine the ammo expended:
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;.</t>
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Roll 1D/2  on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -594,7 +595,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -683,7 +684,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Finished the Time Track.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{513C74B4-0296-498E-958C-1724768713DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{676D5944-F9E7-4D16-94E3-17E18EFF587E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>e001</t>
   </si>
@@ -227,6 +227,18 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Roll 1D/2  on the 
 &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e011</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine your tank&amp;apos;s deployment from the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table:  
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
@@ -592,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -692,43 +704,51 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moved to hatches in prep
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ECA22B-ECBD-4738-967D-3065630F16BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0162EC4F-03D6-416D-AC0E-BCDCAEB24351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>e001</t>
   </si>
@@ -234,13 +234,25 @@
     <t>e011</t>
   </si>
   <si>
+    <t>e012</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Determine your tank&amp;apos;s deployment from the 
 &lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table:  
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e012 Hatches&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Left click on hatches on the Tank Card to toggle adding counter. Click image below to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                     &lt;InlineUIContainer&gt;&lt;Image Name='c15OpenHatch'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -604,16 +616,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="175.25" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="175.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -640,7 +652,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="104.95" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -648,7 +660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="99.95" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -656,7 +668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="114.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -672,7 +684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="99.95" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -680,7 +692,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="99.95" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -688,7 +700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="156.94999999999999" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -696,7 +708,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="114.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -704,51 +716,59 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:2" ht="128.44999999999999" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update for TankCard regions
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ECA22B-ECBD-4738-967D-3065630F16BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7534968B-D0EB-4E34-9FE5-834234E7230C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>e001</t>
   </si>
@@ -241,6 +241,17 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table:  
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e012</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e012 Hatches&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Left click on hatches on the Tank Card to toggle adding counter. Click image below to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                               &lt;InlineUIContainer&gt;&lt;Image Name='c15OpenHatch'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;"</t>
   </si>
 </sst>
 </file>
@@ -604,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -712,43 +723,51 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Continue to work Preparations
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7534968B-D0EB-4E34-9FE5-834234E7230C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{385A300D-FB1D-42CC-B588-09B3ECBEE582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>e001</t>
   </si>
@@ -246,12 +246,63 @@
     <t>e012</t>
   </si>
   <si>
+    <t>e013</t>
+  </si>
+  <si>
+    <t>e014</t>
+  </si>
+  <si>
+    <t>e015</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e013 Gun Load&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Mark the type of round you want loaded in the main gun before any action begins by clicking the highlighted box on the Tank Card in the correct ammo type box. Click image below to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c17GunLoad'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e012 Hatches&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Left click on hatches on the Tank Card to toggle adding counter. Click image below to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                               &lt;InlineUIContainer&gt;&lt;Image Name='c15OpenHatch'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;"</t>
+Left click on hatches on the Tank Card to toggle adding counter. If already open, click button to remove open hatch. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c15OpenHatch'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image in this text box when satisfied and want to continue.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e014 Tank &amp;amp; Turret Orientation&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Sherman tank counter is placed at the center of the battle board. If you want the turret to face a different sector, click tank counter on center of Battle Board. 
+Alternatively, select buttons here:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                   &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Image Name='c16Turret'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When you are satisfied with the current turret orientation, click turret image between buttons to continue.</t>
+  </si>
+  <si>
+    <t>e016</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e015 Loader Spotting&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.45' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the loader is buttoned up or does not have a hatch, mark the sector he will be searching by left clicking on dot just outside the long range zone of the sector. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e016 Commander Spotting&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.45' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the Commander is buttoned up or does not have a vision cupola, mark the sector he will be searching by right clicking on dot just outside the long range zone of the sector. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -615,16 +666,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="175.25" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="175.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -651,7 +702,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="104.95" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -659,7 +710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="99.95" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -667,7 +718,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="114.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -683,7 +734,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="99.95" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -691,7 +742,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="99.95" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -699,7 +750,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="156.94999999999999" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -707,7 +758,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="114.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -715,7 +766,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="99.95" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -723,51 +774,83 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="114.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finish the final prep
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{385A300D-FB1D-42CC-B588-09B3ECBEE582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D480AF4C-7A38-474E-A06E-43FCCCF34EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>e001</t>
   </si>
@@ -303,6 +303,17 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 If the Commander is buttoned up or does not have a vision cupola, mark the sector he will be searching by right clicking on dot just outside the long range zone of the sector. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e017</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e017 Preparations Final&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+US Control markers are placed on sectors 1, 2, and 3. The Weather is displayed on top left of Battle Board.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue017' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -666,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="99.95" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -718,7 +729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="114.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -814,43 +825,51 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started working on Movement Phase
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D480AF4C-7A38-474E-A06E-43FCCCF34EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF3A9890-7879-4B3B-A243-F4C0627DA72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>e001</t>
   </si>
@@ -314,6 +314,62 @@
 US Control markers are placed on sectors 1, 2, and 3. The Weather is displayed on top left of Battle Board.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue017' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e018</t>
+  </si>
+  <si>
+    <t>e019</t>
+  </si>
+  <si>
+    <t>e020</t>
+  </si>
+  <si>
+    <t>e021</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e020 Enemy Strenth Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Check any one adjacent area to your task force for estimating enemy strength. Click on one of the adjacent regions highlighted blue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table. The area is marked with a Light, Medium, or Heavy marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e019 Set Exit Area&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.52' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+On the &lt;InlineUIContainer&gt;&lt;Button Content='Exit Areas' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table, roll 1D and cross reference the number with the Start Area marker 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e018 Set Start Area&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Around the edge of the Movement Board, there are 10 areas number 1-10. The area is marked with the Start Area and Task Force markers. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e021 Choose Operations&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Choose one of following options:&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='Additional' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Area Check&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='Artillery' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Support &lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='Air' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Strike  &lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='Attempt' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Resupply &lt;LineBreak/&gt;
+Alternatively, click on an adjacent highlighted area on the Movement Board to enter that area.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -677,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +833,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="99.95" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -785,7 +841,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="114.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -833,43 +889,75 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding start and exit areas
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF3A9890-7879-4B3B-A243-F4C0627DA72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7D79BC78-46A1-48B3-B3A4-E7C6283A5247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -328,18 +328,6 @@
     <t>e021</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e020 Enemy Strenth Check&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Check any one adjacent area to your task force for estimating enemy strength. Click on one of the adjacent regions highlighted blue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table. The area is marked with a Light, Medium, or Heavy marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e019 Set Exit Area&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.52' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -360,15 +348,35 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;e020 Enemy Strength Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Check any one adjacent area to your task force for estimating enemy strength. Click on one of the adjacent regions highlighted blue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table. The area is marked with a Light, Medium, or Heavy marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e021 Choose Operations&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Choose one of following options:&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='Additional' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Area Check&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='Artillery' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Support &lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='Air' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Strike  &lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='Attempt' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Resupply &lt;LineBreak/&gt;
-Alternatively, click on an adjacent highlighted area on the Movement Board to enter that area.
+Choose one of following options. To see the options, select the &amp;apos;e###&amp;apos; button. To choose the option, select the other buttons. Each option uses up time per the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e022' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ Perform an additional &lt;InlineUIContainer&gt;&lt;Button Content='Area Check' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e023' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Call for Artillery 
+&lt;InlineUIContainer&gt;&lt;Button Content='Support' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e024' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Call for Air 
+&lt;InlineUIContainer&gt;&lt;Button Content='Strike' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e025' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attempt to &lt;InlineUIContainer&gt;&lt;Button Content='Resupply' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Alternatively, click on an adjacent highlighted area on the Movement Board to enter that area per 
+&lt;InlineUIContainer&gt;&lt;Button Content='e026' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -735,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +902,7 @@
         <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -902,7 +910,7 @@
         <v>47</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -910,10 +918,10 @@
         <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Fixed Turret showing up improperly. Started working the Verify Dialog
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7D79BC78-46A1-48B3-B3A4-E7C6283A5247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0B069D-1C5C-4EB6-A0F0-B6CE8A9F23E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Working on start area setup
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0B069D-1C5C-4EB6-A0F0-B6CE8A9F23E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA6E9579-C19E-4581-BDE0-BBD1507BE599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>e001</t>
   </si>
@@ -348,16 +348,36 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e020 Enemy Strength Check&lt;/Bold&gt; 
+    <t>e022</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e020 Enemy Strength Check - Choose Area&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Check any one adjacent area to your task force for estimating enemy strength. Click on one of the adjacent regions highlighted blue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e020 Enemy Strength Check Roll&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 Table. The area is marked with a Light, Medium, or Heavy marker.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e023</t>
+  </si>
+  <si>
+    <t>e024</t>
+  </si>
+  <si>
+    <t>e025</t>
+  </si>
+  <si>
+    <t>e026</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e021 Choose Operations&lt;/Bold&gt; 
@@ -367,17 +387,55 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 Table.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e022' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e023' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
  Perform an additional &lt;InlineUIContainer&gt;&lt;Button Content='Area Check' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e023' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Call for Artillery 
+&lt;InlineUIContainer&gt;&lt;Button Content='e024' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Call for Artillery 
 &lt;InlineUIContainer&gt;&lt;Button Content='Support' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e024' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Call for Air 
+&lt;InlineUIContainer&gt;&lt;Button Content='e025' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Call for Air 
 &lt;InlineUIContainer&gt;&lt;Button Content='Strike' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e025' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attempt to &lt;InlineUIContainer&gt;&lt;Button Content='Resupply' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Alternatively, click on an adjacent highlighted area on the Movement Board to enter that area per 
-&lt;InlineUIContainer&gt;&lt;Button Content='e026' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+&lt;InlineUIContainer&gt;&lt;Button Content='e026' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attempt to 
+&lt;InlineUIContainer&gt;&lt;Button Content='Resupply' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e027' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Click on highlighted area to Enter
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e027</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e027 Enter Adjacent Area&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e023 Area Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Check any one additional adjacent area for estimated enemy strength by rolling on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Click on one of the adjacent regions highlighted blue.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e025 Call for Air Strike&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Call to hit an area adjacent to your task force. Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to see if Air Strike arrives. If successful, an Air Strike marker is placed on the area.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e024 Call for Artillery Support&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Call to hit an area adjacent to your task force. Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to see if Artillery Support arrives. If successful, an Artillery Support marker on the area. Click on one of the adjacent regions highlighted blue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e026 Attempt to Resupply&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to see if resupply occurs. If successful, you may relead your tank with ammo. </t>
   </si>
 </sst>
 </file>
@@ -741,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,59 +971,107 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Trying to incorporatate stacks in the game.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66309992-762D-458A-BC08-B91D6062D86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3741D586-A46C-4CA0-8E3E-4226662F70A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>e001</t>
   </si>
@@ -380,33 +380,60 @@
     <t>e027</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e027 Enter Adjacent Area&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+    <t>e026</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e027 Attempt to Resupply&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to see if resupply occurs. If successful, you may relead your tank with ammo. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e028</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e026 Air Strike Roll&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to see if Air Strike arrives. If successful, an Air Strike marker is placed on the area. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e024 Artillery Support Roll&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to see if Artillery Support arrives. If successful, an Artillery Support marker is placed on the area. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e025 Call for Air Strike&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r23.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Call to hit an area adjacent to your task force. Consult the 
+Call to hit an area adjacent to your task force. Only two Air Strike markers can exist on the board at one time. 
+An additional 15 minute action can be selected while waiting for an air strike. Consult the 
 &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-to see if Air Strike arrives. If successful, an Air Strike marker is placed on the area.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e024 Call for Artillery Support&lt;/Bold&gt; 
+to see if Air Strike arrives. If successful, an Air Strike marker is placed on the area. Click on one of the adjacent regions highlighted blue.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e023 Call for Artillery Support&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Call to hit an area adjacent to your task force. Consult the 
+Call to hit an area adjacent to your task force. Only three Artillery Support markers can exist on the board at one time. Consult the 
 &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 to see if Artillery Support arrives. If successful, an Artillery Support marker on the area. Click on one of the adjacent regions highlighted blue.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e026 Attempt to Resupply&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Consult the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-to see if resupply occurs. If successful, you may relead your tank with ammo. </t>
   </si>
   <si>
     <t>&lt;Bold&gt;e021 Choose Operations&lt;/Bold&gt; 
@@ -420,12 +447,22 @@
  Perform an additional Enemy &lt;InlineUIContainer&gt;&lt;Button Content='Strength Check' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='e023' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Call for Artillery 
 &lt;InlineUIContainer&gt;&lt;Button Content='Support' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e024' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Call for Air 
+&lt;InlineUIContainer&gt;&lt;Button Content='e025' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Call for Air 
 &lt;InlineUIContainer&gt;&lt;Button Content='Strike' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e025' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attempt to 
+&lt;InlineUIContainer&gt;&lt;Button Content='e027' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attempt to 
 &lt;InlineUIContainer&gt;&lt;Button Content='Resupply' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e026' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Click on highlighted area to Enter
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+&lt;InlineUIContainer&gt;&lt;Button Content='e028' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; An adjacent area is 
+&lt;InlineUIContainer&gt;&lt;Button Content='Entered' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e028 Enter Adjacent Area&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click on one of the adjacent highlighted areas. Artillery Support or Air Strike Counters are moved to the battle board as a reminder. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Choose 
+&lt;InlineUIContainer&gt;&lt;Button Content='Advancing Fire' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. </t>
   </si>
 </sst>
 </file>
@@ -789,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +902,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="99.95" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -977,83 +1014,99 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fleshing out end of movement phase
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3741D586-A46C-4CA0-8E3E-4226662F70A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{ACA436FD-7687-491E-B5E1-7B6D52714706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>e001</t>
   </si>
@@ -162,15 +162,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r20.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue001' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The 
-&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- Table determines weather for today:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>e008</t>
@@ -358,16 +349,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e020 Enemy Strength Check Roll&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table. The area is marked with a Light, Medium, or Heavy marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>e023</t>
   </si>
   <si>
@@ -381,6 +362,9 @@
   </si>
   <si>
     <t>e026</t>
+  </si>
+  <si>
+    <t>e029</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e027 Attempt to Resupply&lt;/Bold&gt; 
@@ -436,7 +420,26 @@
 to see if Artillery Support arrives. If successful, an Artillery Support marker on the area. Click on one of the adjacent regions highlighted blue.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e021 Choose Operations&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;e021 Enemy Strength Check Roll&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table. The area is marked with a Light, Medium, or Heavy marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ Table determines weather for today:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;B24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e021 Choose Operations&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Choose one of following options. To see the options, select the &amp;apos;e###&amp;apos; button. To choose the option, select the other buttons. Each option uses up time per the 
@@ -451,18 +454,27 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Strike' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='e027' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attempt to 
 &lt;InlineUIContainer&gt;&lt;Button Content='Resupply' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e028' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; An adjacent area is 
-&lt;InlineUIContainer&gt;&lt;Button Content='Entered' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e028 Enter Adjacent Area&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='e028' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Choose adjacent area to 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enter' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e028 Enter Adjacent Area&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Click on one of the adjacent highlighted areas. Artillery Support or Air Strike Counters are moved to the battle board as a reminder. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Choose 
-&lt;InlineUIContainer&gt;&lt;Button Content='Advancing Fire' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r22.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. </t>
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                &lt;InlineUIContainer&gt;&lt;Image Name='Combat' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e029 Advancing Fire Choice&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Choose one of the following images for Advancing Fire option per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFire' Height='60' Width='60'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; to perform advancing fire. &lt;LineBreak/&gt; &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFireDeny' Height='60' Width='60'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; to skip advancing fire.  </t>
   </si>
 </sst>
 </file>
@@ -826,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,7 +887,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -883,10 +895,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -894,219 +906,227 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="99.95" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="156.94999999999999" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="114.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B30" s="2" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working entering an area
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{ACA436FD-7687-491E-B5E1-7B6D52714706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F7AC9D6-20AD-447B-B573-5C3652D6B78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>e001</t>
   </si>
@@ -475,6 +475,28 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFire' Height='60' Width='60'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; to perform advancing fire. &lt;LineBreak/&gt; &lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFireDeny' Height='60' Width='60'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; to skip advancing fire.  </t>
+  </si>
+  <si>
+    <t>e030</t>
+  </si>
+  <si>
+    <t>e031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e030 Enemy Strength Roll Entering Battle Board&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table for enemy strength: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e031 Resistance Table&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to determine if combat occurs in this area: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
 </sst>
 </file>
@@ -838,10 +860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,43 +1112,59 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="35" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="36" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update victory points when advancing.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F7AC9D6-20AD-447B-B573-5C3652D6B78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B772DB0E-D30C-4A68-9149-259449797EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>e001</t>
   </si>
@@ -197,29 +197,7 @@
 &lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e008 Ammo Loading Limits&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r16.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-See 
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-for ammo types. See 
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-for loading ammo. The Tank Card limits the number of normal main gun ammo allowed to AMMO_NORMAL_LOAD. Extra ammo is added in a later step 
-&lt;InlineUIContainer&gt;&lt;Button Content='e009b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
--- &lt;Bold&gt;AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
--- &lt;Bold&gt;HE:&lt;/Bold&gt; Unlimited</t>
-  </si>
-  <si>
     <t>e010</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Roll 1D/2  on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>e011</t>
@@ -428,15 +406,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The 
-&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- Table determines weather for today:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;B24</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;Bold&gt;e021 Choose Operations&lt;/Bold&gt; 
@@ -491,12 +460,56 @@
 Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;e031 Resistance Table&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ Table determines weather for today:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e031 Battle Check&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 Table to determine if combat occurs in this area: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>e032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e032 No Combat&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+No combat. Victory points added to the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Image Name='AAR' Height='60' Width='60'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+to reflect area under US Control. Continue with </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
+Roll 1D/2  on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. 
+The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e009 Ammo Loading Limits&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r16.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+for ammo types. See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+for loading ammo. The Tank Card limits the number of normal main gun ammo allowed to AMMO_NORMAL_LOAD. Extra ammo is added in a later step 
+&lt;InlineUIContainer&gt;&lt;Button Content='e009b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;Bold&gt;--AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
+ &lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
   </si>
 </sst>
 </file>
@@ -860,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,7 +946,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -949,222 +962,230 @@
         <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Movement through movement map nearly done
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B772DB0E-D30C-4A68-9149-259449797EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2FC59FE-2111-4FEC-BA72-3C67A5C966B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -460,15 +460,6 @@
 Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The 
-&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- Table determines weather for today:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;Bold&gt;e031 Battle Check&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -478,14 +469,6 @@
   </si>
   <si>
     <t>e032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e032 No Combat&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-No combat. Victory points added to the After Action Report 
-&lt;InlineUIContainer&gt;&lt;Image Name='AAR' Height='60' Width='60'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-to reflect area under US Control. Continue with </t>
   </si>
   <si>
     <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
@@ -510,6 +493,23 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
  &lt;Bold&gt;--AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
  &lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;B29
+The 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ Table determines weather for today:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e032 No Combat&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+No combat. Victory points added to the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to reflect area under US Control. </t>
   </si>
 </sst>
 </file>
@@ -875,7 +875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -946,7 +946,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -962,7 +962,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -970,7 +970,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1138,15 +1138,15 @@
         <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add Debriefing rules, Promotion Rules, Decoration Rules
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2FC59FE-2111-4FEC-BA72-3C67A5C966B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071BA1FA-685F-4DA4-B5B3-1D3BFD4BD6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -408,7 +408,91 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;e021 Choose Operations&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;e028 Enter Adjacent Area&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click on one of the adjacent highlighted areas. Artillery Support or Air Strike Counters are moved to the battle board as a reminder. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                &lt;InlineUIContainer&gt;&lt;Image Name='Combat' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e029 Advancing Fire Choice&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Choose one of the following images for Advancing Fire option per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFire' Height='60' Width='60'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; to perform advancing fire. &lt;LineBreak/&gt; &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFireDeny' Height='60' Width='60'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; to skip advancing fire.  </t>
+  </si>
+  <si>
+    <t>e030</t>
+  </si>
+  <si>
+    <t>e031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e030 Enemy Strength Roll Entering Battle Board&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table for enemy strength: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e031 Battle Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to determine if combat occurs in this area: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>e032</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
+Roll 1D/2  on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. 
+The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e009 Ammo Loading Limits&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r16.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+for ammo types. See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+for loading ammo. The Tank Card limits the number of normal main gun ammo allowed to AMMO_NORMAL_LOAD. Extra ammo is added in a later step 
+&lt;InlineUIContainer&gt;&lt;Button Content='e009b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;Bold&gt;--AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
+ &lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;B29
+The 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ Table determines weather for today:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e032 No Combat&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+No combat. Victory points added to the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to reflect area under US Control. </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e022 Choose Operations&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Choose one of following options. To see the options, select the &amp;apos;e###&amp;apos; button. To choose the option, select the other buttons. Each option uses up time per the 
@@ -424,92 +508,7 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='e027' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attempt to 
 &lt;InlineUIContainer&gt;&lt;Button Content='Resupply' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='e028' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Choose adjacent area to 
-&lt;InlineUIContainer&gt;&lt;Button Content='Enter' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e028 Enter Adjacent Area&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click on one of the adjacent highlighted areas. Artillery Support or Air Strike Counters are moved to the battle board as a reminder. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                &lt;InlineUIContainer&gt;&lt;Image Name='Combat' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e029 Advancing Fire Choice&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Choose one of the following images for Advancing Fire option per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r22.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFire' Height='60' Width='60'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; to perform advancing fire. &lt;LineBreak/&gt; &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFireDeny' Height='60' Width='60'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; to skip advancing fire.  </t>
-  </si>
-  <si>
-    <t>e030</t>
-  </si>
-  <si>
-    <t>e031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e030 Enemy Strength Roll Entering Battle Board&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table for enemy strength: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e031 Battle Check&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table to determine if combat occurs in this area: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-  </si>
-  <si>
-    <t>e032</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
-Roll 1D/2  on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. 
-The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e009 Ammo Loading Limits&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r16.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-See 
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-for ammo types. See 
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-for loading ammo. The Tank Card limits the number of normal main gun ammo allowed to AMMO_NORMAL_LOAD. Extra ammo is added in a later step 
-&lt;InlineUIContainer&gt;&lt;Button Content='e009b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;Bold&gt;--AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
- &lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;B29
-The 
-&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- Table determines weather for today:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e032 No Combat&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-No combat. Victory points added to the After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-to reflect area under US Control. </t>
+&lt;InlineUIContainer&gt;&lt;Button Content='Enter' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -875,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,7 +945,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -962,7 +961,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -970,7 +969,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1061,12 +1060,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1114,7 +1113,7 @@
         <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1122,31 +1121,31 @@
         <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added rules section 6
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071BA1FA-685F-4DA4-B5B3-1D3BFD4BD6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE79259-B51A-4928-A999-E8AB98DE945F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -462,28 +462,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e009 Ammo Loading Limits&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r16.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-See 
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-for ammo types. See 
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-for loading ammo. The Tank Card limits the number of normal main gun ammo allowed to AMMO_NORMAL_LOAD. Extra ammo is added in a later step 
-&lt;InlineUIContainer&gt;&lt;Button Content='e009b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;Bold&gt;--AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
- &lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;B29
-The 
-&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- Table determines weather for today:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;Bold&gt;e032 No Combat&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -509,6 +487,28 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Resupply' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='e028' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Choose adjacent area to 
 &lt;InlineUIContainer&gt;&lt;Button Content='Enter' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ Table determines weather for today:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e009 Ammo Loading Limits&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r16.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+for ammo types. See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+for loading ammo. The Tank Card limits the number of normal main gun ammo allowed to AMMO_NORMAL_LOAD. Extra ammo is added in a later step 
+&lt;InlineUIContainer&gt;&lt;Button Content='e009b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Bold&gt;--AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
+&lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
   </si>
 </sst>
 </file>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +945,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -1065,7 +1065,7 @@
         <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1145,7 +1145,7 @@
         <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add rule section 5
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE79259-B51A-4928-A999-E8AB98DE945F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{255E3FAA-719B-4228-8A0D-A865A9825122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -408,14 +408,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e028 Enter Adjacent Area&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click on one of the adjacent highlighted areas. Artillery Support or Air Strike Counters are moved to the battle board as a reminder. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                &lt;InlineUIContainer&gt;&lt;Image Name='Combat' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;Bold&gt;e029 Advancing Fire Choice&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -504,11 +496,18 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r16.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 for ammo types. See 
 &lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-for loading ammo. The Tank Card limits the number of normal main gun ammo allowed to AMMO_NORMAL_LOAD. Extra ammo is added in a later step 
-&lt;InlineUIContainer&gt;&lt;Button Content='e009b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;Bold&gt;--AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
+for loading ammo. The Tank Card limits the number of normal main gun ammo allowed to AMMO_NORMAL_LOAD. Extra ammo is added in a later step after assigning normal load.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Bold&gt;-- AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
 &lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e028 Enter Adjacent Area&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click on one of the adjacent highlighted areas. Artillery Support or Air Strike Counters are moved to the battle board as a reminder. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                        &lt;InlineUIContainer&gt;&lt;Image Name='Sherman1' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -874,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +944,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -956,12 +955,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -969,7 +968,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1065,7 +1064,7 @@
         <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1113,7 +1112,7 @@
         <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1121,31 +1120,31 @@
         <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added 10 sided die roll icons
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{255E3FAA-719B-4228-8A0D-A865A9825122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{13171856-F851-43F6-A5AC-060DF04C7C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -135,21 +135,6 @@
     <t>e007</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e006 Combat Calendar Check&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll for possible combat today. If die &amp;lt;= probability, start morning briefing per 
-&lt;InlineUIContainer&gt;&lt;Button Content='e007' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  
-Otherwise continue with next day check.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Date from Combat Calendar: DATE&lt;LineBreak/&gt;
-Expected Resistance: RESISTANCE&lt;LineBreak/&gt;
-Probablility of Combat: PROBABILITY &amp;gt;= 
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e001 Fourth Armor Division Campaign&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r1.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -188,28 +173,10 @@
     <t>e009</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e008 Type of Snow&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Snow is in the forecast. Roll for type of snow on the
-&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- Table:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>e010</t>
   </si>
   <si>
     <t>e011</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine your tank&amp;apos;s deployment from the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>e012</t>
@@ -297,26 +264,6 @@
     <t>e021</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e019 Set Exit Area&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.52' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-On the &lt;InlineUIContainer&gt;&lt;Button Content='Exit Areas' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table, roll 1D and cross reference the number with the Start Area marker 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e018 Set Start Area&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Around the edge of the Movement Board, there are 10 areas number 1-10. The area is marked with the Start Area and Task Force markers. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>e022</t>
   </si>
   <si>
@@ -345,38 +292,7 @@
     <t>e029</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e027 Attempt to Resupply&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Consult the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-to see if resupply occurs. If successful, you may relead your tank with ammo. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>e028</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e026 Air Strike Roll&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table to see if Air Strike arrives. If successful, an Air Strike marker is placed on the area. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e024 Artillery Support Roll&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table to see if Artillery Support arrives. If successful, an Artillery Support marker is placed on the area. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e025 Call for Air Strike&lt;/Bold&gt; 
@@ -398,16 +314,6 @@
 to see if Artillery Support arrives. If successful, an Artillery Support marker on the area. Click on one of the adjacent regions highlighted blue.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e021 Enemy Strength Check Roll&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table. The area is marked with a Light, Medium, or Heavy marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;Bold&gt;e029 Advancing Fire Choice&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -424,34 +330,7 @@
     <t>e031</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;e030 Enemy Strength Roll Entering Battle Board&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table for enemy strength: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e031 Battle Check&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table to determine if combat occurs in this area: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-  </si>
-  <si>
     <t>e032</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
-Roll 1D/2  on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. 
-The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;Bold&gt;e032 No Combat&lt;/Bold&gt; 
@@ -481,15 +360,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Enter' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The 
-&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- Table determines weather for today:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e009 Ammo Loading Limits&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r16.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 See 
@@ -508,6 +378,136 @@
 Click on one of the adjacent highlighted areas. Artillery Support or Air Strike Counters are moved to the battle board as a reminder. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                         &lt;InlineUIContainer&gt;&lt;Image Name='Sherman1' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e006 Combat Calendar Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll for possible combat today. If die &amp;lt;= probability, start morning briefing per 
+&lt;InlineUIContainer&gt;&lt;Button Content='e007' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  
+Otherwise continue with next day check.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Date from Combat Calendar: DATE&lt;LineBreak/&gt;
+Expected Resistance: RESISTANCE&lt;LineBreak/&gt;
+Probablility of Combat: PROBABILITY &amp;gt;= 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e008 Type of Snow&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Snow is in the forecast. Roll for type of snow on the
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ Table:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
+Roll 1D/2  on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. 
+The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e018 Set Start Area&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Around the edge of the Movement Board, there are 10 areas number 1-10. The area is marked with the Start Area and Task Force markers. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e019 Set Exit Area&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.52' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+On the &lt;InlineUIContainer&gt;&lt;Button Content='Exit Areas' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table, roll 1D and cross reference the number with the Start Area marker 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e021 Enemy Strength Check Roll&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table. The area is marked with a Light, Medium, or Heavy marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e024 Artillery Support Roll&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to see if Artillery Support arrives. If successful, an Artillery Support marker is placed on the area. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e026 Air Strike Roll&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to see if Air Strike arrives. If successful, an Air Strike marker is placed on the area. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e027 Attempt to Resupply&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to see if resupply occurs. If successful, you may relead your tank with ammo. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e030 Enemy Strength Roll Entering Battle Board&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table for enemy strength: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e031 Battle Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to determine if combat occurs in this area: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ Table determines weather for today:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine your tank&amp;apos;s deployment from the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -873,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -920,7 +920,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -928,7 +928,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -936,7 +936,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -944,207 +944,207 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Started Battle Board mechanics
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{144E2B57-6926-4385-8E99-71C3BB6CAC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D2EDBB7-A1A1-426A-BF7B-9F578E45C5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>e001</t>
   </si>
@@ -508,6 +508,50 @@
 The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e033</t>
+  </si>
+  <si>
+    <t>e034</t>
+  </si>
+  <si>
+    <t>e035</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e034 Activation of Enemy Units&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.62' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Activation' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table for the number and general type of enemy units appearing per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The specific types of tanks, SPGs, and AT guns are not known until identified during the Spotting Phase of the Battle Round Sequence per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 2D (x2 for Light, x3 for Medium, and x4 for Heavy resistance).
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e035 Placement of Enemy Units&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.63' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Place enemy units according to Battle Board 
+&lt;InlineUIContainer&gt;&lt;Button Content='Placement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e033 Placing Advancing Fire Markers&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.61' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Place Advancing Fire Markers available to you per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click one of highlighted regions where Advancing Fire Marker is placed. You place up to six minus one marker for every three friendly tank losses (rounded up) . 
+You may place more than one in a zone. The status bar on the bottom tracks how many you have placed.</t>
   </si>
 </sst>
 </file>
@@ -871,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,43 +1191,67 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="39" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="40" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Show Advancing Fire Markers in Status Bar
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D2EDBB7-A1A1-426A-BF7B-9F578E45C5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A85B2B63-00F9-45EF-8FDE-BB6F60E76D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -548,10 +548,12 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.61' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Place Advancing Fire Markers available to you per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r22.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click one of highlighted regions where Advancing Fire Marker is placed. You place up to six minus one marker for every three friendly tank losses (rounded up) . 
-You may place more than one in a zone. The status bar on the bottom tracks how many you have placed.</t>
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Click one of highlighted regions to place. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You place up to six minus one marker for every three friendly tank losses (rounded up) . You may place more than one in a zone. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The status bar on the bottom shows how many are remaining to place.</t>
   </si>
 </sst>
 </file>
@@ -918,7 +920,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1193,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Finished show weather and snow
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A85B2B63-00F9-45EF-8FDE-BB6F60E76D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E196D9D6-EBB1-4C47-BB75-5659843B8C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -395,15 +395,6 @@
 &lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e008 Type of Snow&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Snow is in the forecast. Roll for type of snow on the
-&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- Table:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e018 Set Start Area&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -479,15 +470,6 @@
 Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 Table to determine if combat occurs in this area: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The 
-&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- Table determines weather for today:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
@@ -554,6 +536,24 @@
 You place up to six minus one marker for every three friendly tank losses (rounded up) . You may place more than one in a zone. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The status bar on the bottom shows how many are remaining to place.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ Table determines weather for today:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e008 Type of Snow&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Snow is in the forecast. Roll for type of snow on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ Table:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -919,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,7 +990,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -998,7 +998,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1022,7 +1022,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1078,7 +1078,7 @@
         <v>40</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -1102,7 +1102,7 @@
         <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
         <v>47</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1142,7 +1142,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
         <v>49</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
         <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
         <v>57</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1195,26 +1195,26 @@
     </row>
     <row r="34" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix movement and strength checks
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F130875-2C33-4A2C-A507-4B661BEA3583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DC33B66-5525-4B4D-A8B4-9C35544C1B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>e001</t>
   </si>
@@ -554,6 +553,16 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
  Table:  
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e036</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e036 Re-enter Friendly Control&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+No combat. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -918,19 +927,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="175.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="175.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -938,7 +947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,7 +955,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -954,7 +963,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -962,7 +971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -970,7 +979,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -978,7 +987,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -986,7 +995,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -994,7 +1003,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1002,7 +1011,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1010,7 +1019,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -1018,7 +1027,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1026,7 +1035,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1034,7 +1043,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -1042,7 +1051,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1050,7 +1059,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1058,7 +1067,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1066,7 +1075,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1074,7 +1083,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
@@ -1082,7 +1091,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1090,7 +1099,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -1098,7 +1107,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -1114,7 +1123,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -1122,7 +1131,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
@@ -1130,7 +1139,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -1138,7 +1147,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -1146,7 +1155,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
@@ -1154,7 +1163,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
@@ -1162,7 +1171,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -1170,7 +1179,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>56</v>
       </c>
@@ -1178,7 +1187,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>57</v>
       </c>
@@ -1186,7 +1195,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>58</v>
       </c>
@@ -1194,7 +1203,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>74</v>
       </c>
@@ -1202,7 +1211,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>75</v>
       </c>
@@ -1210,7 +1219,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>76</v>
       </c>
@@ -1218,43 +1227,51 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Rule section 24 and 27
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DC33B66-5525-4B4D-A8B4-9C35544C1B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0EC1F0B6-E96E-48DD-A241-49C6B7A26B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added start of Evening Briefing
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0EC1F0B6-E96E-48DD-A241-49C6B7A26B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA537710-1639-49C1-BC44-506B0494D769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -333,14 +333,6 @@
     <t>e032</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;e032 No Combat&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-No combat. Victory points added to the After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-to reflect area under US Control. </t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e022 Choose Operations&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -564,6 +556,13 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 No combat. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e032 No Combat&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If converting territory to US Control, Victory points are added to the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
 </sst>
 </file>
@@ -930,16 +929,16 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="175.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="175.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -947,7 +946,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,7 +954,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -963,7 +962,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -971,7 +970,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -979,7 +978,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -987,55 +986,55 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1043,7 +1042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1059,7 +1058,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1075,7 +1074,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1083,23 +1082,23 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -1107,23 +1106,23 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -1131,15 +1130,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -1147,31 +1146,31 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -1179,63 +1178,63 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>2</v>
       </c>
@@ -1243,7 +1242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
@@ -1251,7 +1250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
@@ -1259,7 +1258,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>8</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
added capability for advance fire ammo use. Added some functionality for debrief
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90EE1C52-1B7E-4CED-856F-E4DF2E87906D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7255D79C-5ECF-4F00-ACFD-E5C398F804FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>e001</t>
   </si>
@@ -448,22 +448,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;e030 Enemy Strength Roll Entering Battle Board&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table for enemy strength: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e031 Battle Check&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table to determine if combat occurs in this area: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -493,43 +477,6 @@
     <t>e035</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e034 Activation of Enemy Units&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.62' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Consult the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Activation' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table for the number and general type of enemy units appearing per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r12.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
- &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The specific types of tanks, SPGs, and AT guns are not known until identified during the Spotting Phase of the Battle Round Sequence per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r17.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
- &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 2D (x2 for Light, x3 for Medium, and x4 for Heavy resistance).
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e035 Placement of Enemy Units&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.63' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Place enemy units according to Battle Board 
-&lt;InlineUIContainer&gt;&lt;Button Content='Placement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r12.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e033 Placing Advancing Fire Markers&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.61' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Place Advancing Fire Markers available to you per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r22.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-Click one of highlighted regions to place. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You place up to six minus one marker for every three friendly tank losses (rounded up) . You may place more than one in a zone. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The status bar on the bottom shows how many are remaining to place.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e007 Morning Briefing - Weather Roll&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The 
@@ -551,27 +498,51 @@
     <t>e036</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e036 Re-enter Friendly Control&lt;/Bold&gt; 
+    <t xml:space="preserve">&lt;Bold&gt;e031 Enemy Strength Roll Entering Battle Board&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table for enemy strength: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e032 Battle Check&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-No combat. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e032 No Combat&lt;/Bold&gt; 
+Roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to determine if combat occurs in this area: &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e033 No Combat&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 If converting territory to US Control, Victory points are added to the After Action Report 
 &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
   <si>
-    <t>e037</t>
-  </si>
-  <si>
-    <t>e038</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e037 Ambush Check&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;e034 Placing Advancing Fire Markers&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.61' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Place Advancing Fire Markers available to you per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Click one of highlighted regions to place. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You place up to six minus one marker for every three friendly tank losses (rounded up) . You may place more than one in a zone. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The status bar on the bottom shows how many are remaining to place.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e030 Advancing Fire Ammo Use&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Mark off 1D/2 (round down) HE rounds and .30 caliber MG ammo boxes regardless of whether the battle occurs or not. Mark off on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e035 Ambush Check&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.65' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Roll 1D for possible Ambush: 
@@ -579,7 +550,18 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e038 Battle Board Empty&lt;/Bold&gt; 
+    <t>e050</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050 Evening Debriefing&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                     &lt;InlineUIContainer&gt;&lt;Image Name='Sherman4' Height='168' Width='275'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e036 Battle Board Empty&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Since the Battle Board is now empty of enemy units, the battle for this area is over. 
@@ -597,7 +579,7 @@
 &lt;LineBreak/&gt;
 5.) Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                               &lt;InlineUIContainer&gt;&lt;Image Name='Sherman4' Height='168' Width='275'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+          &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='225' Width='450'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -961,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,7 +1016,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1042,7 +1024,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1058,7 +1040,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1066,7 +1048,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1213,12 +1195,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1226,102 +1208,94 @@
         <v>57</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="B37" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix some images. Added skip of battle setup
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7255D79C-5ECF-4F00-ACFD-E5C398F804FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AA7A77E-D379-43F2-B9D0-50E92E51DED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -945,7 +945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Moving forward with Enemy Actions
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AA7A77E-D379-43F2-B9D0-50E92E51DED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD3A9A72-5B81-4075-BD72-030EB56F1F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>e001</t>
   </si>
@@ -580,6 +580,19 @@
 5.) Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
           &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='225' Width='450'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e037</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e037 Smoke Depletion Phase&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.71' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Deplete smoke in each zone by converting one white full strength Smoke marker to a gray 1/2 strength Smoke marker. Alternatively, remove 1/2 strength Smoke marker. Refer to 
+&lt;InlineUIContainer&gt;&lt;Button Content='r18.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for the smoke rules. Click image to continue with 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                              &lt;InlineUIContainer&gt;&lt;Image Name='c111Smoke1' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -943,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +984,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1251,51 +1264,59 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on spotting behavior
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D012156-4852-42A0-9C40-C4C56876996F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB3D38D9-3143-444B-BBD2-5E3038431E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -601,16 +601,16 @@
     <t>&lt;Bold&gt;e038 Orders Phase&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click on closed hatches to open and open hatches to close.
+Click on blue squares to open hatches. Click on Open Hatch marker to close.
  &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click crew member boxes on the Tank Card to select from a pull down of options for each crew member per 
+Click crew member action boxes to select from a pull down to assign crew actions for each crew member per 
 &lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click on the appropriate Tank Card location to place the Gun Reload marker per 
+Click on the appropriate Gun Load box to set the Gun Reload marker per 
 &lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click on the ready rack boxes on the Tank Card to select the Ready Rack Ammo Reload marker and the Gun Reload marker per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+Click the Gun Reload marker/button if you want the reload to come from the ready rack. A Ready Rack Ammo Reload marker is added per  
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Determine the specific unit type for any units identified per 
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
@@ -981,7 +981,7 @@
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
started working out kinks in run up to battle
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB3D38D9-3143-444B-BBD2-5E3038431E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FA89551-65EA-4678-9420-923C47F5357C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>e001</t>
   </si>
@@ -454,17 +454,6 @@
 Determine your tank&amp;apos;s deployment from the 
 &lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table:  
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
-Roll 1D on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. 
-The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
@@ -614,6 +603,190 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Determine the specific unit type for any units identified per 
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e039</t>
+  </si>
+  <si>
+    <t>e040</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r21.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
+Roll 1D on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. 
+The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e040 Time Passes&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r21.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Fifteen minutes pass on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                   &lt;InlineUIContainer&gt;&lt;Image Name='MilitaryWatch' Height='100' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e041</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e041 Friendly Artillery&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Friendly artillery support arrives. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='c39ArtillerySupport'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e042</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e042 Enemy Artillery&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy artillery arrives. Roll 1D to knock out (KO) friendly units: 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1 KO for 1-6&lt;LineBreak/&gt;
+2 KO for 7-9&lt;LineBreak/&gt;
+3 KO for 10
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e043</t>
+  </si>
+  <si>
+    <t>e044</t>
+  </si>
+  <si>
+    <t>e045</t>
+  </si>
+  <si>
+    <t>e046</t>
+  </si>
+  <si>
+    <t>e047</t>
+  </si>
+  <si>
+    <t>e048</t>
+  </si>
+  <si>
+    <t>e049</t>
+  </si>
+  <si>
+    <t>e043a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e043 Mine Attack&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Minefield' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attack Table: 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e043a Mine Attack Ignored&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+No effect since Sherman is not moving. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue043' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e047 Enemy Reinformement&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e044 Panzerfaust Attack&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine from which sector of the Battle Board attack is originating by rolling 1D according to 
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; :  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the sector rolled is US controlled, no attack is made. If the sector is not US Controlled, a Panzerfaust marker is placed in the sector's close range.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If an attack occurs, roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Attack Table to hit Sherman:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite1' Height='21' Width='21' Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If hits, roll again to see if your tank is knocked out (KO):  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite2' Height='21' Width='21' Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e045 Harrassing Fire&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Your tank is sprayed with small weapons fire. Roll 1D on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Collateral' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Damage Table:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e046 Friendly Advance&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Place a US Controlled marker in a sector of your choice that is empty of enemy units and adjacent to a sector already US Controlled.</t>
+  </si>
+  <si>
+    <t>e046a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e046a Friendly Advance Ignored&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since there is no sector adjacent to a US Controlled sector that is empty of enemy units, this event is ignored. Click image to continue.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e048 Enemy Advance&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Remove one US Control marker from sector adjacent to an enemy unit. If two sectors are eligible, it is chosen randomly</t>
+  </si>
+  <si>
+    <t>e048a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e048a Enemy Advance Ignored&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since no sector is adjacent to an enemy unit, this event is ignored. Click image to continue.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e049 Flanking Fire&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll against each enemy unit on the Friendly Action Table with a die roll modifer of -10. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e039 Random Events for Ambush&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.65' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e040' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Time Passes&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e041' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Friendly Artillery&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e042' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Artillery&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e043' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Mine Attack&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e044' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Panzerfaust Attack&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e045' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Harrassing Fire&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e046' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Friendly Advance&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e047' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Reinforcment&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e048' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Advance&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e049' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Flanking Fire&lt;LineBreak/&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -978,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1224,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1059,7 +1232,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1070,12 +1243,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1235,7 +1408,7 @@
         <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1243,7 +1416,7 @@
         <v>57</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1251,102 +1424,214 @@
         <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="2" t="s">
+    </row>
+    <row r="40" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="B40" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cehckpointing - adding explosion
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FA89551-65EA-4678-9420-923C47F5357C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3911EB7-28CB-4369-B187-03C5A5850882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -787,7 +787,7 @@
   &lt;InlineUIContainer&gt;&lt;Button Content='e047' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Reinforcment&lt;LineBreak/&gt;
   &lt;InlineUIContainer&gt;&lt;Button Content='e048' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Advance&lt;LineBreak/&gt;
   &lt;InlineUIContainer&gt;&lt;Button Content='e049' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Flanking Fire&lt;LineBreak/&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +1154,7 @@
   <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
checkpointing - about to add identification of enemy units
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3911EB7-28CB-4369-B187-03C5A5850882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB09B2B1-C350-497D-840F-EB63E4402A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>e001</t>
   </si>
@@ -587,25 +587,6 @@
     <t>e038</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e038 Orders Phase&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click on blue squares to open hatches. Click on Open Hatch marker to close.
- &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click crew member action boxes to select from a pull down to assign crew actions for each crew member per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click on the appropriate Gun Load box to set the Gun Reload marker per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click the Gun Reload marker/button if you want the reload to come from the ready rack. A Ready Rack Ammo Reload marker is added per  
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine the specific unit type for any units identified per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r17.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>e039</t>
   </si>
   <si>
@@ -788,6 +769,28 @@
   &lt;InlineUIContainer&gt;&lt;Button Content='e048' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Advance&lt;LineBreak/&gt;
   &lt;InlineUIContainer&gt;&lt;Button Content='e049' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Flanking Fire&lt;LineBreak/&gt;
 &lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e051</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e038 Orders Phase&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click on blue squares to open hatches. Click on Open Hatch marker to close.
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Right click crew member action boxes to select from a pull down to assign crew actions for each crew member.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e051 Ammo Reload Order&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1151,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,7 +1251,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1467,124 +1470,124 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1595,43 +1598,51 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
making progress on killed tank
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB09B2B1-C350-497D-840F-EB63E4402A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{17CDEA3A-F6A6-423F-8FD8-07191E81AFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -673,14 +673,6 @@
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e043a Mine Attack Ignored&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-No effect since Sherman is not moving. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue043' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e047 Enemy Reinformement&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
@@ -791,6 +783,14 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e043a Mine Attack Ignored&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+No effect since Sherman is not moving. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue43' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1156,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,7 +1475,7 @@
         <v>87</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -1483,7 +1483,7 @@
         <v>88</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -1523,7 +1523,7 @@
         <v>103</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -1531,7 +1531,7 @@
         <v>97</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1539,7 +1539,7 @@
         <v>98</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1547,15 +1547,15 @@
         <v>99</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1563,7 +1563,7 @@
         <v>100</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1571,15 +1571,15 @@
         <v>101</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -1587,7 +1587,7 @@
         <v>102</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1600,10 +1600,10 @@
     </row>
     <row r="55" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
making progress on bail out - finished minefield attack
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25292A0F-1525-49E0-851A-3335BCC4BD0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED0FEAF4-ACF3-4E1D-B3CC-088615E1524A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>e001</t>
   </si>
@@ -796,16 +796,38 @@
     <t>e043b</t>
   </si>
   <si>
+    <t>e043c</t>
+  </si>
+  <si>
+    <t>e043d</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e043b Mine Attack Destroyed Tank&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Tank is disabled for today. Place a Thrown Track marker. Roll 1D to determine crew effect as shown on 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Tank is disabled for today. Roll 1D to determine crew effect as shown on 
 &lt;InlineUIContainer&gt;&lt;Button Content='Minefield' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attack Table: 
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 1-8 = No Effect&lt;LineBreak/&gt;
 9 = Driver possibly wounded&lt;LineBreak/&gt;
 10 = Assistant possibly wounded
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e043c Driver Possibly Wounded from Minefield Attack&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Driver possibly wounded by minefield attack. Roll 2D and look at 
+&lt;InlineUIContainer&gt;&lt;Button Content='Wounds' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table: 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e043d Assistant Possibly Wounded from Minefield Attack&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Assistant Driver possibly wounded by minefield attack. Roll 2D and look at 
+&lt;InlineUIContainer&gt;&lt;Button Content='Wounds' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table: 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -1170,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,131 +1564,147 @@
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="B47" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="50" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="51" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="55" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="56" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="61" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="62" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started working panzerfaust attack
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED0FEAF4-ACF3-4E1D-B3CC-088615E1524A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{477F36B4-90B5-4CCD-9A1A-C162C87CF100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t>e001</t>
   </si>
@@ -678,24 +678,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e044 Panzerfaust Attack&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine from which sector of the Battle Board attack is originating by rolling 1D according to 
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; :  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the sector rolled is US controlled, no attack is made. If the sector is not US Controlled, a Panzerfaust marker is placed in the sector's close range.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If an attack occurs, roll on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Attack Table to hit Sherman:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite1' Height='21' Width='21' Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If hits, roll again to see if your tank is knocked out (KO):  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite2' Height='21' Width='21' Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e045 Harrassing Fire&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -829,6 +811,75 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Wounds' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table: 
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e044a</t>
+  </si>
+  <si>
+    <t>e044b</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e044 Panzerfaust Attack - Sector&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine from which sector of the Battle Board attack is originating by rolling 1D according to 
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; :  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the sector rolled is US controlled, no attack is made. If the sector is not US Controlled, a Panzerfaust marker is placed in the sector's close range.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e044c Panzerfaust Attack - To Kill&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since there was a hit, roll again to see if your tank is knocked out (KO):  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  1 to 8  is KO&lt;LineBreak/&gt;
+  9 to 10 is No Effect&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e044b Panzerfaust Attack - To Hit&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since an attack occurred, roll to hit:   
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  1 to 7 is Hit&lt;LineBreak/&gt;
+  8 to 10 is Miss&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;
+  Sherman moving = +2&lt;LineBreak/&gt;
+  Advancing Fire in zone = +3&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e044a Panzerfaust Attack - To Attack&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine if attack occurs based on scenario type, roll one die: 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  1 to 3 for Advance&lt;LineBreak/&gt;
+  1 to 5 for Battle&lt;LineBreak/&gt;
+  1 to 2 for Counterattack&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;
+  December 1944 or later = -1&lt;LineBreak/&gt;
+  Sherman moving = -1&lt;LineBreak/&gt;
+  Lead tank = -1&lt;LineBreak/&gt;
+  Advancing Fire in zone = +3&lt;LineBreak/&gt;
+  Attack from sector 1,2, or3 = -1&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e044c</t>
   </si>
 </sst>
 </file>
@@ -1192,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,7 +1564,7 @@
         <v>87</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -1521,7 +1572,7 @@
         <v>88</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -1561,150 +1612,174 @@
         <v>103</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B55" s="2" t="s">
+    </row>
+    <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="64" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="65" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
worked on panzerfaust attack
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{477F36B4-90B5-4CCD-9A1A-C162C87CF100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A14C6B62-2224-4BB9-8338-58AC7BA1D5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>e001</t>
   </si>
@@ -540,14 +540,6 @@
   </si>
   <si>
     <t>e050</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050 Evening Debriefing&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                     &lt;InlineUIContainer&gt;&lt;Image Name='Sherman4' Height='168' Width='275'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e036 Battle Board Empty&lt;/Bold&gt; 
@@ -745,9 +737,6 @@
 &lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>e051</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e038 Orders Phase&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
@@ -755,15 +744,6 @@
 Click on blue squares to open hatches. Click on Open Hatch marker to close.
  &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Right click crew member action boxes to select from a pull down to assign crew actions for each crew member.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e051 Ammo Reload Order&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
@@ -843,6 +823,50 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
+    <t>e044c</t>
+  </si>
+  <si>
+    <t>e100</t>
+  </si>
+  <si>
+    <t>e0101</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e101 Evening Debriefing&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e100 Evening Debriefing&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                     &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='168' Width='275'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e044a Panzerfaust Attack - To Attack&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine if attack occurs based on scenario type, roll one die: 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  1 to 3 for Advance&lt;LineBreak/&gt;
+  1 to 5 for Battle&lt;LineBreak/&gt;
+  1 to 2 for Counterattack
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e044b Panzerfaust Attack - To Hit&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
@@ -853,33 +877,7 @@
   1 to 7 is Hit&lt;LineBreak/&gt;
   8 to 10 is Miss&lt;LineBreak/&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;
-  Sherman moving = +2&lt;LineBreak/&gt;
-  Advancing Fire in zone = +3&lt;LineBreak/&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e044a Panzerfaust Attack - To Attack&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine if attack occurs based on scenario type, roll one die: 
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-  1 to 3 for Advance&lt;LineBreak/&gt;
-  1 to 5 for Battle&lt;LineBreak/&gt;
-  1 to 2 for Counterattack&lt;LineBreak/&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;
-  December 1944 or later = -1&lt;LineBreak/&gt;
-  Sherman moving = -1&lt;LineBreak/&gt;
-  Lead tank = -1&lt;LineBreak/&gt;
-  Advancing Fire in zone = +3&lt;LineBreak/&gt;
-  Attack from sector 1,2, or3 = -1&lt;LineBreak/&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e044c</t>
+&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1241,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
@@ -1340,7 +1338,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1548,238 +1546,246 @@
         <v>75</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>4</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cleaned up exploding tank image
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A14C6B62-2224-4BB9-8338-58AC7BA1D5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD927AF7-C866-487A-BC95-0CF7B8C103D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -665,39 +665,7 @@
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e047 Enemy Reinformement&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e045 Harrassing Fire&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Your tank is sprayed with small weapons fire. Roll 1D on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Collateral' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Damage Table:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e046 Friendly Advance&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Place a US Controlled marker in a sector of your choice that is empty of enemy units and adjacent to a sector already US Controlled.</t>
-  </si>
-  <si>
     <t>e046a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e046a Friendly Advance Ignored&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since there is no sector adjacent to a US Controlled sector that is empty of enemy units, this event is ignored. Click image to continue.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e048 Enemy Advance&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Remove one US Control marker from sector adjacent to an enemy unit. If two sectors are eligible, it is chosen randomly</t>
   </si>
   <si>
     <t>e048a</t>
@@ -799,20 +767,38 @@
     <t>e044b</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e044 Panzerfaust Attack - Sector&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine from which sector of the Battle Board attack is originating by rolling 1D according to 
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; :  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the sector rolled is US controlled, no attack is made. If the sector is not US Controlled, a Panzerfaust marker is placed in the sector's close range.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+    <t>e044c</t>
+  </si>
+  <si>
+    <t>e100</t>
+  </si>
+  <si>
+    <t>e0101</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e101 Evening Debriefing&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e100 Evening Debriefing&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                     &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='168' Width='275'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e044c Panzerfaust Attack - To Kill&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
  &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Since there was a hit, roll again to see if your tank is knocked out (KO):  
@@ -823,38 +809,33 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>e044c</t>
-  </si>
-  <si>
-    <t>e100</t>
-  </si>
-  <si>
-    <t>e0101</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e101 Evening Debriefing&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e100 Evening Debriefing&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                     &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='168' Width='275'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    <t>&lt;Bold&gt;e044b Panzerfaust Attack - To Hit&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since an attack occurred, roll to hit:   
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  1 to 7 is Hit&lt;LineBreak/&gt;
+  8 to 10 is Miss&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e044 Panzerfaust Attack - Sector&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine from which sector of the Battle Board attack is originating by rolling 1D according to 
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; :  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the sector rolled is US controlled, no attack is made. If the sector is not US Controlled, a Panzerfaust marker is placed in the sector's close range.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e044a Panzerfaust Attack - To Attack&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Determine if attack occurs based on scenario type, roll one die: 
@@ -867,17 +848,38 @@
 &lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e044b Panzerfaust Attack - To Hit&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since an attack occurred, roll to hit:   
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-  1 to 7 is Hit&lt;LineBreak/&gt;
-  8 to 10 is Miss&lt;LineBreak/&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
+    <t>&lt;Bold&gt;e046 Friendly Advance&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Place a US Controlled marker in a sector of your choice that is empty of enemy units and adjacent to a sector already US Controlled.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e046a Friendly Advance Ignored&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.8' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since there is no sector adjacent to a US Controlled sector that is empty of enemy units, this event is ignored. Click image to continue.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e047 Enemy Reinforcement&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e048 Enemy Advance&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.10' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Remove one US Control marker from sector adjacent to an enemy unit. If two sectors are eligible, it is chosen randomly</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e045 Harrassing Fire&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Your tank is sprayed with small weapons fire. Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Collateral' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Damage Table. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                        &lt;InlineUIContainer&gt;&lt;Image Name='CollateralDamage' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1243,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,7 +1564,7 @@
         <v>86</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -1570,7 +1572,7 @@
         <v>87</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -1610,31 +1612,31 @@
         <v>102</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1642,39 +1644,39 @@
         <v>96</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1682,15 +1684,15 @@
         <v>98</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1698,7 +1700,7 @@
         <v>99</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1706,15 +1708,15 @@
         <v>100</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -1722,7 +1724,7 @@
         <v>101</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1730,23 +1732,23 @@
         <v>82</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated evening debriefing events
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD927AF7-C866-487A-BC95-0CF7B8C103D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{999F0B67-7BB9-451F-AD04-F87E27EB5EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>e001</t>
   </si>
@@ -773,9 +773,6 @@
     <t>e100</t>
   </si>
   <si>
-    <t>e0101</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
@@ -783,18 +780,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e101 Evening Debriefing&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e100 Evening Debriefing&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                     &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='168' Width='275'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e044c Panzerfaust Attack - To Kill&lt;/Bold&gt; 
@@ -880,6 +865,53 @@
 Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                         &lt;InlineUIContainer&gt;&lt;Image Name='CollateralDamage' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e100 Evening Debriefing&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Click image to continue to continue to Crew Rating Improvements per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                     &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='168' Width='275'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e101 Evening Debriefing - Victory Point Total&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+is updated to reflect victory points for both yoru tank and friendly forces. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the combined victory points from both your tank and friendly forces is positive, you have won the engagement.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e101</t>
+  </si>
+  <si>
+    <t>e102</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e102 Evening Debriefing - Promotions&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r25.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+is updated to reflect promotions.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e103</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e103 Evening Debriefing - Decorations&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r26.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll for possible decorations on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Decorations' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+Medals received are recorded on the  per After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1243,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,7 +1676,7 @@
         <v>96</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -1652,7 +1684,7 @@
         <v>117</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -1660,7 +1692,7 @@
         <v>118</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1668,7 +1700,7 @@
         <v>119</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -1676,7 +1708,7 @@
         <v>97</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1684,7 +1716,7 @@
         <v>98</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1692,7 +1724,7 @@
         <v>104</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1700,7 +1732,7 @@
         <v>99</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1708,7 +1740,7 @@
         <v>100</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1732,62 +1764,78 @@
         <v>82</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="68" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started working evening debriefing
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{999F0B67-7BB9-451F-AD04-F87E27EB5EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15F15E19-A4C0-4F32-B31D-E679CEF1D7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -867,50 +867,58 @@
                         &lt;InlineUIContainer&gt;&lt;Image Name='CollateralDamage' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
+    <t>e101</t>
+  </si>
+  <si>
+    <t>e102</t>
+  </si>
+  <si>
+    <t>e103</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e100 Evening Debriefing&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
 Click image to continue to continue to Crew Rating Improvements per 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                     &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='168' Width='275'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+             &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e101 Evening Debriefing - Victory Point Total&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.92' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The After Action Report 
 &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-is updated to reflect victory points for both yoru tank and friendly forces. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the combined victory points from both your tank and friendly forces is positive, you have won the engagement.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e101</t>
-  </si>
-  <si>
-    <t>e102</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e102 Evening Debriefing - Promotions&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r25.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-is updated to reflect promotions.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e103</t>
+is updated to reflect victory points for both your tank and friendly forces. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e103 Evening Debriefing - Decorations&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r26.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Roll for possible decorations on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Decorations' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
-Medals received are recorded on the  per After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
+&lt;InlineUIContainer&gt;&lt;Button Content='Decorations' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
+Medals received are recorded on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Must roll at least 200 after modifications with 2D.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e102 Evening Debriefing - Promotions&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.93' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r25.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You are promoted when promotion points reach these values. However, cannot be promoted faster than once per month:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+100 = Staff Sergeant&lt;LineBreak/&gt;
+200 = 2nd Lieutenant&lt;LineBreak/&gt;
+300 = 1st Lieutenant&lt;LineBreak/&gt;
+400 = Captian
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Promotion Points:  PROMOTION_POINTS&lt;LineBreak/&gt;
+Promotion Date:     PROMOTION_DATE&lt;LineBreak/&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -1277,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
@@ -1772,31 +1780,31 @@
         <v>120</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="B64" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
checkpointing - added decorations
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15F15E19-A4C0-4F32-B31D-E679CEF1D7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{832975CE-6C1A-415F-B092-BE2A34BB9FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -876,15 +876,6 @@
     <t>e103</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e100 Evening Debriefing&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-Click image to continue to continue to Crew Rating Improvements per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-             &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e101 Evening Debriefing - Victory Point Total&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.92' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -920,6 +911,15 @@
 Promotion Points:  PROMOTION_POINTS&lt;LineBreak/&gt;
 Promotion Date:     PROMOTION_DATE&lt;LineBreak/&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e100 Evening Debriefing&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Click image to continue to continue to Crew Rating Improvements per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                  &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1285,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,7 +1780,7 @@
         <v>120</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1788,7 +1788,7 @@
         <v>131</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -1796,7 +1796,7 @@
         <v>132</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -1804,7 +1804,7 @@
         <v>133</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working through brew up
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{832975CE-6C1A-415F-B092-BE2A34BB9FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6A26E75-2DBC-44D2-AA56-CA57B4D72441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>e001</t>
   </si>
@@ -207,19 +207,6 @@
                                                   &lt;InlineUIContainer&gt;&lt;Image Name='c15OpenHatch'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Click image in this text box when satisfied and want to continue.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e014 Tank &amp;amp; Turret Orientation&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The Sherman tank counter is placed at the center of the battle board. If you want the turret to face a different sector, click tank counter on center of Battle Board. 
-Alternatively, select buttons here:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                   &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Image Name='c16Turret'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When you are satisfied with the current turret orientation, click turret image between buttons to continue.</t>
   </si>
   <si>
     <t>e016</t>
@@ -920,6 +907,32 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                   &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e104</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e104 Evening Debriefing - Purple Heart&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r26.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The purple heart is awarded for receiving a wound in combat. You have acumulated NUMBER_PURPLE_HEARTS in this campaign.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                              &lt;InlineUIContainer&gt;&lt;Image Name='DecorationPurpleHeart' Height='210' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to continue.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e014 Tank &amp;amp; Turret Orientation&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Sherman tank counter is placed at the center of the battle board. If you want the turret to face a different sector, click tank counter on center of Battle Board. 
+Alternatively, select buttons here:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                   &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Image Name='c16TurretSherman75'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When you are satisfied with the current turret orientation, click turret image between buttons to continue.</t>
   </si>
 </sst>
 </file>
@@ -1283,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,7 +1361,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1356,7 +1369,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1364,7 +1377,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1372,7 +1385,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1380,7 +1393,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1388,7 +1401,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1412,7 +1425,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1420,430 +1433,438 @@
         <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>2</v>
+        <v>137</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>4</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished with Tank Destroyed conops
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6A26E75-2DBC-44D2-AA56-CA57B4D72441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9626E792-B070-45A0-A94E-8FC127C5503A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -884,6 +885,41 @@
 &lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;e100 Evening Debriefing&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Click image to continue to continue to Crew Rating Improvements per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                  &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e104</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e104 Evening Debriefing - Purple Heart&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r26.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The purple heart is awarded for receiving a wound in combat. You have acumulated NUMBER_PURPLE_HEARTS in this campaign.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                              &lt;InlineUIContainer&gt;&lt;Image Name='DecorationPurpleHeart' Height='210' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to continue.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e014 Tank &amp;amp; Turret Orientation&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Sherman tank counter is placed at the center of the battle board. If you want the turret to face a different sector, click tank counter on center of Battle Board. 
+Alternatively, select buttons here:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                   &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Image Name='c16TurretSherman75'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When you are satisfied with the current turret orientation, click turret image between buttons to continue.</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e102 Evening Debriefing - Promotions&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.93' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Content='r25.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -894,45 +930,7 @@
 200 = 2nd Lieutenant&lt;LineBreak/&gt;
 300 = 1st Lieutenant&lt;LineBreak/&gt;
 400 = Captian
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Promotion Points:  PROMOTION_POINTS&lt;LineBreak/&gt;
-Promotion Date:     PROMOTION_DATE&lt;LineBreak/&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e100 Evening Debriefing&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-Click image to continue to continue to Crew Rating Improvements per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                  &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>e104</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e104 Evening Debriefing - Purple Heart&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r26.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The purple heart is awarded for receiving a wound in combat. You have acumulated NUMBER_PURPLE_HEARTS in this campaign.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                              &lt;InlineUIContainer&gt;&lt;Image Name='DecorationPurpleHeart' Height='210' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click image to continue.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e014 Tank &amp;amp; Turret Orientation&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The Sherman tank counter is placed at the center of the battle board. If you want the turret to face a different sector, click tank counter on center of Battle Board. 
-Alternatively, select buttons here:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                   &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Image Name='c16TurretSherman75'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When you are satisfied with the current turret orientation, click turret image between buttons to continue.</t>
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1298,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,7 +1423,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1793,7 +1791,7 @@
         <v>119</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1804,12 +1802,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -1822,10 +1820,10 @@
     </row>
     <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
change name of order
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9626E792-B070-45A0-A94E-8FC127C5503A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{096ECD68-88E0-4E72-820E-1A19B13FBE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -761,15 +760,6 @@
     <t>e100</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e044c Panzerfaust Attack - To Kill&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r15.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -931,6 +921,16 @@
 300 = 1st Lieutenant&lt;LineBreak/&gt;
 400 = Captian
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1296,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,7 +1423,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1695,7 +1695,7 @@
         <v>95</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -1703,7 +1703,7 @@
         <v>116</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -1711,7 +1711,7 @@
         <v>117</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1719,7 +1719,7 @@
         <v>118</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -1727,7 +1727,7 @@
         <v>96</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1735,7 +1735,7 @@
         <v>97</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1743,7 +1743,7 @@
         <v>103</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>98</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1759,7 +1759,7 @@
         <v>99</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1778,12 +1778,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1791,39 +1791,39 @@
         <v>119</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
started doing sherman movement
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{096ECD68-88E0-4E72-820E-1A19B13FBE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D046FD4-D593-49B1-857D-AA81EE95E9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
   <si>
     <t>e001</t>
   </si>
@@ -931,6 +931,19 @@
 Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue50' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e051</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e051 Crew Actions - Tank Movement&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Resolve movement per the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Movement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Tables.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1294,10 +1307,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,83 +1799,91 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished updating rules. Started implementing Sherman Movement rules and Firing rules
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D046FD4-D593-49B1-857D-AA81EE95E9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FA182EDE-B15B-4D30-B0CC-5A8AD3A87A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t>e001</t>
   </si>
@@ -944,6 +944,34 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Movement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Tables.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e052</t>
+  </si>
+  <si>
+    <t>e053</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053 Main Gun Firing&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Select a target by clicking the enemy unit. Consult the &lt;InlineUIContainer&gt;&lt;Button Content='To Hit Target' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table to determine if target is hit.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e052 Pivot Tank&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Select the plus or minus buttons to rotate.  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                   &lt;InlineUIContainer&gt;&lt;Button Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Image Name='ShermanPivot'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When you are satisfied with the current orientation, click Sherman image between buttons to continue.</t>
   </si>
 </sst>
 </file>
@@ -1307,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1807,83 +1835,99 @@
         <v>141</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="66" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="71" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="72" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started to work on firing Sherman
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CD18C87-4D9B-468D-A1E3-4D8D977D2743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5734C1D2-9331-4518-AD8B-76D8934FF91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>e001</t>
   </si>
@@ -865,15 +865,6 @@
     <t>e053</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e053 Main Gun Firing&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Select a target by clicking the enemy unit. Consult the &lt;InlineUIContainer&gt;&lt;Button Content='To Hit Target' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table to determine if target is hit.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e052 Pivot Tank&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r8.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -980,6 +971,37 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Roll against each enemy unit on the Friendly Action Table with a die roll modifer of -10. Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e053a</t>
+  </si>
+  <si>
+    <t>e053b</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053b Main Gun Firing&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Select a target by clicking the enemy unit on the Battle Board. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053 Main Gun Firing - Select Target&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Select a target by clicking the enemy unit on the Battle Board. Only enemy units that have been spotted may be selected. The main gun may only fire at a target in the turret&amp;apos;s sector unless the &lt;Bold&gt;Rotate Turret - Fire Main Gun&lt;/Bold&gt; action was taken.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053a Main Gun Firing - No Target Available&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+There is no target that is selectable. Only enemy units that have been spotted may be selected. The main gun may only fire at a target in the turret&amp;apos;s front sector unless the &lt;Bold&gt;Rotate Turret - Fire Main Gun&lt;/Bold&gt; action was taken. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1343,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,7 +1694,7 @@
         <v>86</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1680,7 +1702,7 @@
         <v>87</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1688,7 +1710,7 @@
         <v>89</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1696,7 +1718,7 @@
         <v>90</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1784,7 +1806,7 @@
         <v>94</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1792,7 +1814,7 @@
         <v>100</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1800,7 +1822,7 @@
         <v>95</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1808,7 +1830,7 @@
         <v>96</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1816,7 +1838,7 @@
         <v>101</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -1824,7 +1846,7 @@
         <v>97</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1848,94 +1870,110 @@
         <v>132</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="67" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="68" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="70" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="73" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="75" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on direct vs area fire
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5734C1D2-9331-4518-AD8B-76D8934FF91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{250D8A6E-BC37-4040-9D8C-17999CC86B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -529,27 +529,6 @@
     <t>e050</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e036 Battle Board Empty&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since the Battle Board is now empty of enemy units, the battle for this area is over. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-1.) Flip Resistance marker to US Controlled on Movement Board.
-&lt;LineBreak/&gt;
-2.) Victory points for control of the area added to the 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;
-3.) If daylight remains, return to Prepare for Battle per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;
-4.) No daylight, perform the Evening Debriefing per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;
-5.) Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-          &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='225' Width='450'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>e037</t>
   </si>
   <si>
@@ -979,29 +958,53 @@
     <t>e053b</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e053b Main Gun Firing&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;e053a Main Gun Firing - No Target Available&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Select a target by clicking the enemy unit on the Battle Board. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+There is no target that is selectable. Only enemy units that have been spotted may be selected. The main gun may only fire at a target in the turret&amp;apos;s front sector unless the &lt;Bold&gt;Rotate Turret - Fire Main Gun&lt;/Bold&gt; action was taken. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e036 Battle Board Empty&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since the Battle Board is now empty of enemy units, the battle for this area is over. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1.) Flip Resistance marker to US Controlled on Movement Board.
+&lt;LineBreak/&gt;
+2.) Victory points for control of the area added to the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;
+3.) If daylight remains, return to Prepare for Battle per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;
+4.) No daylight, perform the Evening Debriefing per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;
+5.) Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+          &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='225' Width='450'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e053 Main Gun Firing - Select Target&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The appropriate type of ammo is marked off the After Action Report &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Select a target by clicking the enemy unit on the Battle Board. Only enemy units that have been spotted may be selected. The main gun may only fire at a target in the turret&amp;apos;s sector unless the &lt;Bold&gt;Rotate Turret - Fire Main Gun&lt;/Bold&gt; action was taken.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e053a Main Gun Firing - No Target Available&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;e053b Main Gun Firing - Target Selected&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-There is no target that is selectable. Only enemy units that have been spotted may be selected. The main gun may only fire at a target in the turret&amp;apos;s front sector unless the &lt;Bold&gt;Rotate Turret - Fire Main Gun&lt;/Bold&gt; action was taken. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+Choose  &lt;InlineUIContainer&gt;&lt;Button Content='Direct' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   or    
+&lt;InlineUIContainer&gt;&lt;Button Content=' Area ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   fire.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
@@ -1462,7 +1465,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1494,7 +1497,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1670,183 +1673,183 @@
         <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1854,28 +1857,28 @@
         <v>81</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>148</v>
@@ -1883,58 +1886,58 @@
     </row>
     <row r="64" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working crew conducting actions
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{250D8A6E-BC37-4040-9D8C-17999CC86B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DC2D800-49B2-4F09-957C-0A4272305046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>e001</t>
   </si>
@@ -956,15 +956,6 @@
   </si>
   <si>
     <t>e053b</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053a Main Gun Firing - No Target Available&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-There is no target that is selectable. Only enemy units that have been spotted may be selected. The main gun may only fire at a target in the turret&amp;apos;s front sector unless the &lt;Bold&gt;Rotate Turret - Fire Main Gun&lt;/Bold&gt; action was taken. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e036 Battle Board Empty&lt;/Bold&gt; 
@@ -988,22 +979,49 @@
           &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='225' Width='450'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
+    <t>e053c</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053b Main Gun Firing - Target Selected&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The appropriate type of ammo is marked off the After Action Report &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Choose  &lt;InlineUIContainer&gt;&lt;Button Content='Direct' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   or    
+&lt;InlineUIContainer&gt;&lt;Button Content=' Area ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    fire.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053c MG Gun Firing - Select Target&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click either the highlighted zone or an spotted target or &lt;InlineUIContainer&gt;&lt;Button Content='Skip MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; . 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53c' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053a Main Gun Firing - No Target Available&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+There is no target that is selectable. Only enemy units that have been spotted may be selected.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The main gun may only fire at a target in the turret&amp;apos;s front sector unless the &amp;quot;Rotate Turret - Fire Main Gun&amp;quot; action was taken. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e053 Main Gun Firing - Select Target&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The appropriate type of ammo is marked off the After Action Report &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Select a target by clicking the enemy unit on the Battle Board. Only enemy units that have been spotted may be selected. The main gun may only fire at a target in the turret&amp;apos;s sector unless the &lt;Bold&gt;Rotate Turret - Fire Main Gun&lt;/Bold&gt; action was taken.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053b Main Gun Firing - Target Selected&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Choose  &lt;InlineUIContainer&gt;&lt;Button Content='Direct' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   or    
-&lt;InlineUIContainer&gt;&lt;Button Content=' Area ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   fire.
+Select a target by clicking the enemy unit on the Battle Board or &lt;InlineUIContainer&gt;&lt;Button Content=' Skip ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; firing. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Only enemy units that have been spotted may be selected. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The main gun may only fire at a target in the turret&amp;apos;s front sector unless the &amp;quot;Rotate Turret - Fire Main Gun&amp;quot; action was taken.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -1368,10 +1386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A62" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,7 +1691,7 @@
         <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1876,107 +1894,115 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>145</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working rate of fire
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86856AD7-A040-4683-AD50-41658F40F1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AF8DBA3C-1EE5-410A-AD7C-6A769C2C20C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <t>e001</t>
   </si>
@@ -1018,6 +1018,41 @@
     <t>e053d</t>
   </si>
   <si>
+    <t>e053e</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053e MG Gun Firing - Select Target&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click either the highlighted zone or an spotted target or &lt;InlineUIContainer&gt;&lt;Button Content='Skip MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; . 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53c' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053d Main Gun Fire - Resolution&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For each hit scored against a target, consult the correct To Kill Table to determine if the target is knocked out (KO'ed).</t>
+  </si>
+  <si>
+    <t>e052a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e052 Pivot Turret&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Select the plus or minus buttons to rotate.  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                   &lt;InlineUIContainer&gt;&lt;Button Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Image Name='ShermanPivot'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When you are satisfied with the current orientation, click Sherman image between buttons to continue.</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e053c Main Gun Firing - Rate of Fire&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -1027,26 +1062,8 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
  Choose 
  &lt;InlineUIContainer&gt;&lt;Button Content='Fire' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   or  
- &lt;InlineUIContainer&gt;&lt;Button Content='Skip' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   to continue.</t>
-  </si>
-  <si>
-    <t>e053e</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053e MG Gun Firing - Select Target&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click either the highlighted zone or an spotted target or &lt;InlineUIContainer&gt;&lt;Button Content='Skip MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; . 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53c' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053d Main Gun Fire - Resolution&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-For each hit scored against a target, consult the correct To Kill Table to determine if the target is knocked out (KO'ed).</t>
+ &lt;InlineUIContainer&gt;&lt;Button Content='Skip' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1410,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="B64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1918,49 +1935,49 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+      <c r="B67" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>154</v>
@@ -1968,81 +1985,89 @@
     </row>
     <row r="69" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started resolving TO KILL rolls
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFB15AF1-E7D9-40EE-8BA8-6A599113ADD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{665AD5EE-A695-4038-BBE7-1C62CE6BF878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t>e001</t>
   </si>
@@ -1021,13 +1021,6 @@
     <t>e053e</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e053d Main Gun Fire - Resolution&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-For each hit scored against a target, consult the correct To Kill Table to determine if the target is knocked out (KO'ed).</t>
-  </si>
-  <si>
     <t>e052a</t>
   </si>
   <si>
@@ -1043,21 +1036,41 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 When you are satisfied with the current turret orientation, click turret image between buttons to continue.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053e Machine Gun (MG) Firing - Select Target&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click either the highlighted zone or an spotted target or &lt;InlineUIContainer&gt;&lt;Button Content='Skip MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; . 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53c' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e053c Main Gun Firing - Rate of Fire&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='Rate of Fire' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e053f</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053f Machine Gun (MG) Firing - Select Target&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click either the highlighted zone or an spotted target or &lt;InlineUIContainer&gt;&lt;Button Content='Skip MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; . 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53c' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053e Main Gun Fire Against Vehicle - Resolution&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For each hit scored against a target, consult the correct To Kill Table to determine if the target is knocked out (KO'ed).</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053d Main Gun Fire Against Infantry - Resolution&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For each hit scored against a target, consult the  
+&lt;InlineUIContainer&gt;&lt;Button Content='To Kill Infantry' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ Table to determine if the target is knocked out (KO'ed) using these modifier:
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -1422,10 +1435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1932,10 +1945,10 @@
     </row>
     <row r="63" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -1967,102 +1980,110 @@
         <v>147</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>151</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>152</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started MG conops. Also finished Infantry To Kill
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{665AD5EE-A695-4038-BBE7-1C62CE6BF878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41B99503-1597-4C3F-9449-558D0CD1E7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -815,16 +815,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>e051</t>
   </si>
   <si>
@@ -1057,14 +1047,16 @@
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue53c' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e053e Main Gun Fire Against Vehicle - Resolution&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-For each hit scored against a target, consult the correct To Kill Table to determine if the target is knocked out (KO'ed).</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053d Main Gun Fire Against Infantry - Resolution&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053d Main Gun Against Infantry&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1072,6 +1064,13 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='To Kill Infantry' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
  Table to determine if the target is knocked out (KO'ed) using these modifier:
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053e Main Gun Against Vehicle&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For each hit scored against a target, consult the correct To Kill Table to determine if the target is knocked out (KO'ed).</t>
   </si>
 </sst>
 </file>
@@ -1437,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1740,7 +1739,7 @@
         <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -1764,7 +1763,7 @@
         <v>85</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -1772,7 +1771,7 @@
         <v>86</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -1780,7 +1779,7 @@
         <v>88</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -1788,7 +1787,7 @@
         <v>89</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -1876,7 +1875,7 @@
         <v>93</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -1884,7 +1883,7 @@
         <v>99</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -1892,7 +1891,7 @@
         <v>94</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -1900,7 +1899,7 @@
         <v>95</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -1908,7 +1907,7 @@
         <v>100</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -1916,95 +1915,95 @@
         <v>96</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
good progress on MGs
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41B99503-1597-4C3F-9449-558D0CD1E7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CF30292-7140-4FEC-926E-444F0D529AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
   <si>
     <t>e001</t>
   </si>
@@ -845,26 +845,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 When you are satisfied with the current orientation, click Sherman image between buttons to continue.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e039 Random Events for Ambush&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.65' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e040' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Time Passes&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e041' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Friendly Artillery&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e042' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Artillery&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e043' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Mine Attack&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e044' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Panzerfaust Attack&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e045' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Harrassing Fire&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e046' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Friendly Advance&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e047' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Reinforcement&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e048' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Advance&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e049' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Flanking Fire
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e040 Time Passes&lt;/Bold&gt; 
@@ -1014,39 +994,6 @@
     <t>e052a</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e052 Pivot Turret&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If you want the turret to face a different sector, click tank counter on center of Battle Board. 
-Alternatively, select buttons here:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                   &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Image Name='c16TurretSherman75'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When you are satisfied with the current turret orientation, click turret image between buttons to continue.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053c Main Gun Firing - Rate of Fire&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='Rate of Fire' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e053f</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053f Machine Gun (MG) Firing - Select Target&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click either the highlighted zone or an spotted target or &lt;InlineUIContainer&gt;&lt;Button Content='Skip MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; . 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53c' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
@@ -1066,11 +1013,81 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e053e Main Gun Against Vehicle&lt;/Bold&gt; 
+    <t xml:space="preserve">&lt;Bold&gt;e053e Main Gun Against Vehicle&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-For each hit scored against a target, consult the correct To Kill Table to determine if the target is knocked out (KO'ed).</t>
+For each hit scored against a target, consult the  </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e052a Pivot Turret&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you want the turret to face a different sector, click tank counter on center of Battle Board. 
+Alternatively, select buttons here:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                   &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Image Name='c16TurretSherman75'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When you are satisfied with the current turret orientation, click turret image between buttons to continue.</t>
+  </si>
+  <si>
+    <t>e054</t>
+  </si>
+  <si>
+    <t>e054a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e054 MG Firing - Select Target&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r10.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Choose a MG to fire or select skip: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='   Skip   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+  &lt;InlineUIContainer&gt;&lt;Button Content='  AA MG   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+  &lt;InlineUIContainer&gt;&lt;Button Content='  Bow MG  '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+  &lt;InlineUIContainer&gt;&lt;Button Content='Coaxial MG'  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+  &lt;InlineUIContainer&gt;&lt;Button Content='  Sub MG  '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053c Main Gun Firing - Rate of Fire&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='Rate of Fire' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e054a MG Firing - Target Selected&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r10.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The MG ammo is marked off the After Action Report &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Roll for results on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Sherman MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e039 Random Events&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.65' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e040' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Time Passes&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e041' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Friendly Artillery&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e042' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Artillery&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e043' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Mine Attack&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e044' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Panzerfaust Attack&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e045' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Harrassing Fire&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e046' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Friendly Advance&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e047' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Reinforcement&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e048' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Advance&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e049' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Flanking Fire
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1434,19 +1451,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="175.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="175.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1454,7 +1471,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1462,7 +1479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1470,7 +1487,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1478,7 +1495,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1486,7 +1503,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1494,7 +1511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1502,7 +1519,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1510,7 +1527,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1518,7 +1535,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1526,7 +1543,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -1534,7 +1551,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1542,7 +1559,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1550,7 +1567,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -1558,7 +1575,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1566,7 +1583,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1574,7 +1591,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1582,7 +1599,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
@@ -1590,7 +1607,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
@@ -1598,7 +1615,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
@@ -1606,7 +1623,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -1614,7 +1631,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -1622,7 +1639,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
@@ -1630,7 +1647,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
@@ -1638,7 +1655,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -1646,7 +1663,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -1654,7 +1671,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -1662,7 +1679,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>48</v>
       </c>
@@ -1670,7 +1687,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>51</v>
       </c>
@@ -1678,7 +1695,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>50</v>
       </c>
@@ -1686,7 +1703,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
@@ -1694,7 +1711,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>56</v>
       </c>
@@ -1702,7 +1719,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>57</v>
       </c>
@@ -1710,7 +1727,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>69</v>
       </c>
@@ -1718,7 +1735,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>70</v>
       </c>
@@ -1726,7 +1743,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>71</v>
       </c>
@@ -1734,15 +1751,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>82</v>
       </c>
@@ -1750,7 +1767,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>84</v>
       </c>
@@ -1758,39 +1775,39 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>90</v>
       </c>
@@ -1798,7 +1815,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>97</v>
       </c>
@@ -1806,7 +1823,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>103</v>
       </c>
@@ -1814,7 +1831,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>104</v>
       </c>
@@ -1822,7 +1839,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>105</v>
       </c>
@@ -1830,7 +1847,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>91</v>
       </c>
@@ -1838,7 +1855,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>109</v>
       </c>
@@ -1846,7 +1863,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>110</v>
       </c>
@@ -1854,7 +1871,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>111</v>
       </c>
@@ -1862,7 +1879,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>92</v>
       </c>
@@ -1870,63 +1887,63 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>128</v>
       </c>
@@ -1934,7 +1951,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>130</v>
       </c>
@@ -1942,147 +1959,155 @@
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B66" s="2" t="s">
+    <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B68" s="2" t="s">
+    <row r="70" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix regions on battle map. Added new ReturnToSpotting territory
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CF30292-7140-4FEC-926E-444F0D529AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3E081688-B2EE-4B34-8772-8CF0D7A5D70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>e001</t>
   </si>
@@ -1061,6 +1061,9 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
+    <t>e060</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e054a MG Firing - Target Selected&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r10.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -1088,6 +1091,14 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 Table:  
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e060 Reset Round&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since the round did not end, reset and return back to Spotting Round.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue60' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1451,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,7 +1791,7 @@
         <v>85</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2028,86 +2039,94 @@
         <v>157</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="B72" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working through battle round
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3E081688-B2EE-4B34-8772-8CF0D7A5D70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0CED90D-C58B-4488-A028-25F9C468E871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t>e001</t>
   </si>
@@ -545,9 +545,6 @@
     <t>e038</t>
   </si>
   <si>
-    <t>e039</t>
-  </si>
-  <si>
     <t>e040</t>
   </si>
   <si>
@@ -926,6 +923,207 @@
   </si>
   <si>
     <t>e053b</t>
+  </si>
+  <si>
+    <t>e053c</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053a Main Gun Firing - No Target Available&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+There is no target that is selectable. Only enemy units that have been spotted may be selected.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The main gun may only fire at a target in the turret&amp;apos;s front sector unless the &amp;quot;Rotate Turret - Fire Main Gun&amp;quot; action was taken. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053 Main Gun Firing - Select Target&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Select a target by clicking the enemy unit on the Battle Board or &lt;InlineUIContainer&gt;&lt;Button Content=' Skip ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; firing. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Only enemy units that have been spotted may be selected. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The main gun may only fire at a target in the turret&amp;apos;s front sector unless the &amp;quot;Rotate Turret - Fire Main Gun&amp;quot; action was taken.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053b Main Gun Firing - Target Selected&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The appropriate type of ammo is marked off the After Action Report &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Choose  &lt;InlineUIContainer&gt;&lt;Button Content='Direct' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   or    
+&lt;InlineUIContainer&gt;&lt;Button Content=' Area ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    fire.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e053d</t>
+  </si>
+  <si>
+    <t>e053e</t>
+  </si>
+  <si>
+    <t>e052a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053d Main Gun Against Infantry&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For each hit scored against a target, consult the  
+&lt;InlineUIContainer&gt;&lt;Button Content='To Kill Infantry' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ Table to determine if the target is knocked out (KO'ed) using these modifier:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e053e Main Gun Against Vehicle&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For each hit scored against a target, consult the  </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e052a Pivot Turret&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you want the turret to face a different sector, click tank counter on center of Battle Board. 
+Alternatively, select buttons here:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                   &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Image Name='c16TurretSherman75'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When you are satisfied with the current turret orientation, click turret image between buttons to continue.</t>
+  </si>
+  <si>
+    <t>e054</t>
+  </si>
+  <si>
+    <t>e054a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e054 MG Firing - Select Target&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r10.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Choose a MG to fire or select skip: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='   Skip   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+  &lt;InlineUIContainer&gt;&lt;Button Content='  AA MG   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+  &lt;InlineUIContainer&gt;&lt;Button Content='  Bow MG  '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+  &lt;InlineUIContainer&gt;&lt;Button Content='Coaxial MG'  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+  &lt;InlineUIContainer&gt;&lt;Button Content='  Sub MG  '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053c Main Gun Firing - Rate of Fire&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='Rate of Fire' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e060</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e054a MG Firing - Target Selected&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r10.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The MG ammo is marked off the After Action Report &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Roll for results on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Sherman MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e039a</t>
+  </si>
+  <si>
+    <t>e039b</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e039a Advance Scenario - Random Events&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.65' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e040' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 01-05   Time Passes&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e041' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 06-15    Friendly Artillery&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e042' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 16-20    Enemy Artillery&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e043' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 21-25    Mine Attack&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e044' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 26-30    Panzerfaust Attack&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e045' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 31-35    Harrassing Fire&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e046' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 36-60    Friendly Advance&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e047' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 61-80    Enemy Reinforcement&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e048' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; --------     Enemy Advance&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e049' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 81-100+ Flanking Fire
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e039b Battle Scenario - Random Events&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.65' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e040' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 01-05   Time Passes&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e041' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 06-20    Friendly Artillery&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e042' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 21-30    Enemy Artillery&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e043' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 31-35    Mine Attack&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e044' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 36-40    Panzerfaust Attack&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e045' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 41-45    Harrassing Fire&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e046' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 46-60    Friendly Advance&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e047' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 61-80    Enemy Reinforcement&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e048' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 81-85     Enemy Advance&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e049' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 86-100+ Flanking Fire
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e039c Counterattack Scenario - Random Events&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.65' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e040' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 01-05   Time Passes&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e041' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 06-25    Friendly Artillery&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e042' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 25-35    Enemy Artillery&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e043' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; --------     Mine Attack&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e044' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 36-40    Panzerfaust Attack&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e045' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 41-45    Harrassing Fire&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e046' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 46-50    Friendly Advance&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e047' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 51-75    Enemy Reinforcement&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e048' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 76-90     Enemy Advance&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e049' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 91-100+ Flanking Fire
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table:  
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e039c</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e060 Reset Round&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since the round did not end, reset and return back to Spotting Round. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue60' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e036 Battle Board Empty&lt;/Bold&gt; 
@@ -946,159 +1144,7 @@
 &lt;LineBreak/&gt;
 5.) Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-          &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='225' Width='450'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>e053c</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053a Main Gun Firing - No Target Available&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-There is no target that is selectable. Only enemy units that have been spotted may be selected.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The main gun may only fire at a target in the turret&amp;apos;s front sector unless the &amp;quot;Rotate Turret - Fire Main Gun&amp;quot; action was taken. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053 Main Gun Firing - Select Target&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Select a target by clicking the enemy unit on the Battle Board or &lt;InlineUIContainer&gt;&lt;Button Content=' Skip ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; firing. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Only enemy units that have been spotted may be selected. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The main gun may only fire at a target in the turret&amp;apos;s front sector unless the &amp;quot;Rotate Turret - Fire Main Gun&amp;quot; action was taken.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053b Main Gun Firing - Target Selected&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The appropriate type of ammo is marked off the After Action Report &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-Choose  &lt;InlineUIContainer&gt;&lt;Button Content='Direct' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   or    
-&lt;InlineUIContainer&gt;&lt;Button Content=' Area ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    fire.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e053d</t>
-  </si>
-  <si>
-    <t>e053e</t>
-  </si>
-  <si>
-    <t>e052a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053d Main Gun Against Infantry&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-For each hit scored against a target, consult the  
-&lt;InlineUIContainer&gt;&lt;Button Content='To Kill Infantry' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- Table to determine if the target is knocked out (KO'ed) using these modifier:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;e053e Main Gun Against Vehicle&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-For each hit scored against a target, consult the  </t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e052a Pivot Turret&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If you want the turret to face a different sector, click tank counter on center of Battle Board. 
-Alternatively, select buttons here:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                   &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Image Name='c16TurretSherman75'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When you are satisfied with the current turret orientation, click turret image between buttons to continue.</t>
-  </si>
-  <si>
-    <t>e054</t>
-  </si>
-  <si>
-    <t>e054a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e054 MG Firing - Select Target&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r10.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Choose a MG to fire or select skip: 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='   Skip   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-  &lt;InlineUIContainer&gt;&lt;Button Content='  AA MG   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-  &lt;InlineUIContainer&gt;&lt;Button Content='  Bow MG  '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-  &lt;InlineUIContainer&gt;&lt;Button Content='Coaxial MG'  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-  &lt;InlineUIContainer&gt;&lt;Button Content='  Sub MG  '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053c Main Gun Firing - Rate of Fire&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='Rate of Fire' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e060</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e054a MG Firing - Target Selected&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r10.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The MG ammo is marked off the After Action Report &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Roll for results on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Sherman MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e039 Random Events&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.65' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e040' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Time Passes&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e041' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Friendly Artillery&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e042' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Artillery&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e043' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Mine Attack&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e044' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Panzerfaust Attack&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e045' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Harrassing Fire&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e046' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Friendly Advance&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e047' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Reinforcement&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e048' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Advance&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e049' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Flanking Fire
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e060 Reset Round&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since the round did not end, reset and return back to Spotting Round.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue60' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue36' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1462,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,7 +1605,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1591,7 +1637,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1767,7 +1813,7 @@
         <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1783,350 +1829,366 @@
         <v>84</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>86</v>
+        <v>161</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>88</v>
+        <v>165</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="B46" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="B56" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B58" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B59" s="2" t="s">
+    <row r="62" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="B67" s="2" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="B72" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>112</v>
+        <v>155</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="B79" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    </row>
+    <row r="80" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="81" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="83" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented the bogged down status
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0CED90D-C58B-4488-A028-25F9C468E871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{06F278D5-7858-4943-9DFE-EA070BF038CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t>e001</t>
   </si>
@@ -1145,6 +1146,18 @@
 5.) Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue36' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e051a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e051a Bogged Down&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+A bogged down tank may not move or pivot until it has freed itself by using reverse movement on the
+ &lt;InlineUIContainer&gt;&lt;Button Content='Bogged Down' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1508,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B84"/>
+  <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,171 +2037,179 @@
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cleaning p some stuff related to pivoting
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06F278D5-7858-4943-9DFE-EA070BF038CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3CA9A5F-9F04-4B89-9792-4066C815DF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -832,19 +832,6 @@
     <t>e053</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e052 Pivot Tank&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Select the plus or minus buttons to rotate.  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                   &lt;InlineUIContainer&gt;&lt;Button Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Image Name='ShermanPivot'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When you are satisfied with the current orientation, click Sherman image between buttons to continue.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e040 Time Passes&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r15.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Content='r21.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
@@ -949,16 +936,6 @@
 Only enemy units that have been spotted may be selected. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The main gun may only fire at a target in the turret&amp;apos;s front sector unless the &amp;quot;Rotate Turret - Fire Main Gun&amp;quot; action was taken.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053b Main Gun Firing - Target Selected&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The appropriate type of ammo is marked off the After Action Report &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-Choose  &lt;InlineUIContainer&gt;&lt;Button Content='Direct' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   or    
-&lt;InlineUIContainer&gt;&lt;Button Content=' Area ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    fire.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
@@ -995,20 +972,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 For each hit scored against a target, consult the  </t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e052a Pivot Turret&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If you want the turret to face a different sector, click tank counter on center of Battle Board. 
-Alternatively, select buttons here:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                   &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Image Name='c16TurretSherman75'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When you are satisfied with the current turret orientation, click turret image between buttons to continue.</t>
   </si>
   <si>
     <t>e054</t>
@@ -1158,6 +1121,34 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='Bogged Down' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053b Main Gun Firing - Target Selected&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e052a Pivot Turret&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you want the turret to face a different sector, select buttons here: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                             &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
+&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e052 Pivot Tank&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you want the Sherman to face a different sector, select buttons here:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                           &lt;InlineUIContainer&gt;&lt;Button Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;      
+&lt;InlineUIContainer&gt;&lt;Button Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1523,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,7 +1817,7 @@
         <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1847,26 +1838,26 @@
     </row>
     <row r="40" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1874,7 +1865,7 @@
         <v>85</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1882,7 +1873,7 @@
         <v>87</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1890,7 +1881,7 @@
         <v>88</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1978,7 +1969,7 @@
         <v>92</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1986,7 +1977,7 @@
         <v>98</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1994,7 +1985,7 @@
         <v>93</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2002,7 +1993,7 @@
         <v>94</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2010,7 +2001,7 @@
         <v>99</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2018,7 +2009,7 @@
         <v>95</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2026,7 +2017,7 @@
         <v>81</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2039,26 +2030,26 @@
     </row>
     <row r="64" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2066,71 +2057,71 @@
         <v>130</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="B69" s="2" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="105" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tyring to fix issues with gun loads
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3CA9A5F-9F04-4B89-9792-4066C815DF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF3D3EC7-332B-4511-9706-EE940FB03E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t>e001</t>
   </si>
@@ -946,15 +946,6 @@
   </si>
   <si>
     <t>e052a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Right click marker or one of blue boxes to to select from pull down menu where to set Gun Reload marker and/or Ready Rack Ammo Reload marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e053d Main Gun Against Infantry&lt;/Bold&gt; 
@@ -1149,6 +1140,36 @@
                                            &lt;InlineUIContainer&gt;&lt;Button Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;      
 &lt;InlineUIContainer&gt;&lt;Button Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e050a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050a No Gun Round Loaded&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since the gun is unloaded at the start of the round, choose one of the highlighted boxes to load the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e050b</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Right click marker or one of blue boxes to to select from pull down menu where to set the Gun Reload marker and/or Ready Rack Ammo Reload marker. Alternative, right click on the Gun Load marker and choose from pull down menu.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050b Out of Main Gun Ammunition&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since the gun is unloaded at the start of the round, choose one of the highlighted boxes to load the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50b' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1512,10 +1533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B85"/>
+  <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1817,7 +1838,7 @@
         <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1838,26 +1859,26 @@
     </row>
     <row r="40" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2012,195 +2033,211 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="66" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    </row>
+    <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="71" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="B71" s="2" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B74" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="B75" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="79" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="80" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="81" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="82" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="83" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="84" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="85" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="86" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="87" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed some issues Check Facing if only have one AFV that has track thrown. Add VP when killing stuff, Do not show ammo orders in prep if no gun loads,
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{872666C0-10DB-448C-9DCD-FBFD0D755646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10868A5A-DF55-49EC-B1E5-DAEAD254F0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
   <si>
     <t>e001</t>
   </si>
@@ -958,13 +958,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;e053e Main Gun Against Vehicle&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-For each hit scored against a target, consult the  </t>
-  </si>
-  <si>
     <t>e054</t>
   </si>
   <si>
@@ -1071,14 +1064,6 @@
   </si>
   <si>
     <t>e039c</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e060 Reset Round&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since the round did not end, reset and return back to Spotting Round. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue60' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e036 Battle Board Empty&lt;/Bold&gt; 
@@ -1155,43 +1140,86 @@
     <t>e050b</t>
   </si>
   <si>
+    <t>e050c</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050b Out of Main Gun Rounds&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Main Gun is empty, and there are no rounds to load. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50b' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050c No Gun Rounds to Load&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Only one gun round exists in the main gun. There is nothing else to load. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50c' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e050d</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050c No Gun Rounds to Load&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The tank is empty of all main gun rounds. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50d' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e053f</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053e Main Gun Against Vehicle&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053f Smoke Round Hits&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When a hit is scored with a smoke round, place Smoke marker(s) in the zone. HBCI ammo generates two Smoke Markers for each hit.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53f' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Right click marker or one of blue boxes to to select from pull down menu where to set the Gun Reload marker and/or Ready Rack Ammo Reload marker. Alternatively, right click on the Gun Load marker and choose from pull down menu.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e050c</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050b Out of Main Gun Rounds&lt;/Bold&gt; 
+Right click marker or one of blue boxes to show the ammo reload context menu.  Alternatively, or if no blue box is shown, right click on the Gun Load marker to show the context menu.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The context menu allows setting the Ammo Reload marker. When no ammo can be reloaded, this marker disappears.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The selection of Ready Rack Ammo Reload marker over the Ammo Reload marker supports higher chance of performing rate of fire. &lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Gun Load marker shows the round in the main gun. The Gun Load marker changes to the Ammo Reload location when the gun is fired. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e060 Reset Round&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since the battle did not end, reset and return back to Spotting Round. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue60' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e013a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e013a Out of Main Gun Rounds&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Main Gun is empty, and there are no rounds to load. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50b' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050c No Gun Rounds to Load&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Only one gun round exists in the main gun. There is nothing else to load. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50c' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>e050d</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050c No Gun Rounds to Load&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The tank is empty of all main gun rounds. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50d' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+Main Gun is empty, and there are no rounds to load. Tehrefore, the main gun cannot be loaded. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue13a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1555,10 +1583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B89"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,603 +1707,619 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="B38" s="2" t="s">
-        <v>83</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="B43" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="B63" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="B71" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="B74" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="B75" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="B77" s="2" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="83" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="84" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="85" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="86" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="88" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="89" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="91" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Main Gun Working with KIAs and NO CHANCES and Thrown tracks
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10868A5A-DF55-49EC-B1E5-DAEAD254F0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C89EF4E-8F8C-44FB-8E22-FBAD69E7745D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -787,19 +787,6 @@
 Click image to continue.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e014 Tank &amp;amp; Turret Orientation&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The Sherman tank counter is placed at the center of the battle board. If you want the turret to face a different sector, click tank counter on center of Battle Board. 
-Alternatively, select buttons here:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                   &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Image Name='c16TurretSherman75'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When you are satisfied with the current turret orientation, click turret image between buttons to continue.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e102 Evening Debriefing - Promotions&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.93' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Content='r25.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -1105,17 +1092,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e052a Pivot Turret&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If you want the turret to face a different sector, select buttons here: 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                             &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
-&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e052 Pivot Tank&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r8.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -1220,6 +1196,22 @@
 Main Gun is empty, and there are no rounds to load. Tehrefore, the main gun cannot be loaded. Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue13a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e014 Tank &amp;amp; Turret Orientation&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Sherman tank counter is placed at the center of the battle board. If you want the turret to face a different sector, select buttons here: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                             &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
+&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e052a Pivot Turret&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
++B13</t>
   </si>
 </sst>
 </file>
@@ -1585,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,18 +1701,18 @@
     </row>
     <row r="15" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>125</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1896,7 +1888,7 @@
         <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1917,26 +1909,26 @@
     </row>
     <row r="41" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1944,7 +1936,7 @@
         <v>85</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1952,7 +1944,7 @@
         <v>87</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1960,7 +1952,7 @@
         <v>88</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2048,7 +2040,7 @@
         <v>92</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2056,7 +2048,7 @@
         <v>98</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -2064,7 +2056,7 @@
         <v>93</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2072,7 +2064,7 @@
         <v>94</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2080,7 +2072,7 @@
         <v>99</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2088,7 +2080,7 @@
         <v>95</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2096,151 +2088,151 @@
         <v>81</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2264,7 +2256,7 @@
         <v>118</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="135" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished up MG mechanics except for Enemy Movement
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C92A24D-019D-4368-A154-AB16CB40529D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F17A4FCF-AA73-4D48-9383-32F94B518221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>e001</t>
   </si>
@@ -1217,6 +1216,23 @@
                                              &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
 &lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e054b</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e054b MG Firing - Advancing Fire&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Advancing fire attacks infantry targets that move into the zone. It also help protect against Panzerfaust attacks. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 2D for ammo expected:&lt;LineBreak/&gt;
+01 - 30 = 1 box expended&lt;LineBreak/&gt;
+31 - 97 = no effect&lt;LineBreak/&gt;
+98 - 100 = MG malfunctions
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll = &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1580,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,91 +2248,99 @@
         <v>153</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started working in broken scopes
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F17A4FCF-AA73-4D48-9383-32F94B518221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{071FDEB4-29ED-4CDA-9E22-EF5CB8E719D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>e001</t>
   </si>
@@ -1233,6 +1233,18 @@
 98 - 100 = MG malfunctions
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Die Roll = &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e055</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e055 Replace Periscopes&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Replacing PERISCOPE_REPLACEMENT out of PERISCOPE_REPLACEMENT_TOTAL left as shown on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; out of PERISCOPE_REPLACEMENT. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='BrokenPeriscope' Height='350' Width='222'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1596,7 +1608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B81" sqref="B81"/>
@@ -2256,91 +2268,99 @@
         <v>183</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started testing broken scops
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{071FDEB4-29ED-4CDA-9E22-EF5CB8E719D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C3F9281-9E51-4900-BEDE-CE405B1D30E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
   <si>
     <t>e001</t>
   </si>
@@ -1238,11 +1238,21 @@
     <t>e055</t>
   </si>
   <si>
+    <t>e056</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e056 Repair Gun&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content=Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e055 Replace Periscopes&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Replacing PERISCOPE_REPLACEMENT out of PERISCOPE_REPLACEMENT_TOTAL left as shown on the After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; out of PERISCOPE_REPLACEMENT. Click image to continue.
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='BrokenPeriscope' Height='350' Width='222'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
@@ -1608,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,94 +2283,102 @@
         <v>184</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="B83" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement spotting changes due to crew actions
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FADA6CB-4878-4F1D-973E-A3D56EABB6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAF28001-7721-4A27-BF44-11070CD7A498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -1252,9 +1252,11 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Replacing PERISCOPE_REPLACEMENT out of PERISCOPE_REPLACEMENT_TOTAL left as shown on the After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='BrokenPeriscope' Height='222' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                        &lt;InlineUIContainer&gt;&lt;Image Name='BrokenPeriscope' Height='222' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to continue.</t>
   </si>
 </sst>
 </file>
@@ -1621,7 +1623,7 @@
   <dimension ref="A1:B94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,7 +2280,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>184</v>
       </c>

</xml_diff>

<commit_message>
Fix two issues: 1.) Animated Rectangle needs to disappear 2.) Empty Battle board sticks when Collateral Damage returns.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAF28001-7721-4A27-BF44-11070CD7A498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AC1CB8F-12D8-41B5-A2C1-E992EF16AE8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -1052,10 +1052,196 @@
     <t>e039c</t>
   </si>
   <si>
+    <t>e051a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e051a Bogged Down&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+A bogged down tank may not move or pivot until it has freed itself by using reverse movement on the
+ &lt;InlineUIContainer&gt;&lt;Button Content='Bogged Down' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053b Main Gun Firing - Target Selected&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e052a Pivot Turret&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you want the turret to face a different sector, select buttons here: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                             &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
+&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e052 Pivot Tank&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you want the Sherman to face a different sector, select buttons here:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                           &lt;InlineUIContainer&gt;&lt;Button Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;      
+&lt;InlineUIContainer&gt;&lt;Button Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e050a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050a No Gun Round Loaded&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since the gun is unloaded at the start of the round, choose one of the highlighted boxes to load the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e050b</t>
+  </si>
+  <si>
+    <t>e050c</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050b Out of Main Gun Rounds&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Main Gun is empty, and there are no rounds to load. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50b' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050c No Gun Rounds to Load&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Only one gun round exists in the main gun. There is nothing else to load. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50c' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e050d</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050c No Gun Rounds to Load&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The tank is empty of all main gun rounds. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50d' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e053f</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053e Main Gun Against Vehicle&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053f Smoke Round Hits&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When a hit is scored with a smoke round, place Smoke marker(s) in the zone. HBCI ammo generates two Smoke Markers for each hit.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53f' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Right click marker or one of blue boxes to show the ammo reload context menu.  Alternatively, or if no blue box is shown, right click on the Gun Load marker to show the context menu.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The context menu allows setting the Ammo Reload marker. When no ammo can be reloaded, this marker disappears.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The selection of Ready Rack Ammo Reload marker over the Ammo Reload marker supports higher chance of performing rate of fire. &lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Gun Load marker shows the round in the main gun. The Gun Load marker changes to the Ammo Reload location when the gun is fired. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e060 Reset Round&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since the battle did not end, reset and return back to Spotting Round. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue60' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e013a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e013a Out of Main Gun Rounds&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Main Gun is empty, and there are no rounds to load. Tehrefore, the main gun cannot be loaded. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue13a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e014 Tank &amp;amp; Turret Orientation&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Sherman tank counter is placed at the center of the battle board. If you want the turret to face a different sector, select buttons here: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                             &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
+&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e054b</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e054b MG Firing - Advancing Fire&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Advancing fire attacks infantry targets that move into the zone. It also help protect against Panzerfaust attacks. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 2D for ammo expected:&lt;LineBreak/&gt;
+01 - 30 = 1 box expended&lt;LineBreak/&gt;
+31 - 97 = no effect&lt;LineBreak/&gt;
+98 - 100 = MG malfunctions
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll = &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e055</t>
+  </si>
+  <si>
+    <t>e056</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e056 Repair Gun&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content=Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e055 Replace Periscopes&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Replacing PERISCOPE_REPLACEMENT out of PERISCOPE_REPLACEMENT_TOTAL left as shown on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                        &lt;InlineUIContainer&gt;&lt;Image Name='BrokenPeriscope' Height='222' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to continue.</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e036 Battle Board Empty&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since the Battle Board is now empty of enemy units, the battle for this area is over. 
+Since the Battle Board is now empty of enemy units, the battle for this area is finished. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 1.) Flip Resistance marker to US Controlled on Movement Board.
 &lt;LineBreak/&gt;
@@ -1071,192 +1257,6 @@
 5.) Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue36' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>e051a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e051a Bogged Down&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r11.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-A bogged down tank may not move or pivot until it has freed itself by using reverse movement on the
- &lt;InlineUIContainer&gt;&lt;Button Content='Bogged Down' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053b Main Gun Firing - Target Selected&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e052a Pivot Turret&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If you want the turret to face a different sector, select buttons here: 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                             &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
-&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e052 Pivot Tank&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If you want the Sherman to face a different sector, select buttons here:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                           &lt;InlineUIContainer&gt;&lt;Button Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;      
-&lt;InlineUIContainer&gt;&lt;Button Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e050a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050a No Gun Round Loaded&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since the gun is unloaded at the start of the round, choose one of the highlighted boxes to load the gun.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e050b</t>
-  </si>
-  <si>
-    <t>e050c</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050b Out of Main Gun Rounds&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Main Gun is empty, and there are no rounds to load. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50b' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050c No Gun Rounds to Load&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Only one gun round exists in the main gun. There is nothing else to load. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50c' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>e050d</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050c No Gun Rounds to Load&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The tank is empty of all main gun rounds. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50d' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>e053f</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053e Main Gun Against Vehicle&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053f Smoke Round Hits&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When a hit is scored with a smoke round, place Smoke marker(s) in the zone. HBCI ammo generates two Smoke Markers for each hit.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53f' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Right click marker or one of blue boxes to show the ammo reload context menu.  Alternatively, or if no blue box is shown, right click on the Gun Load marker to show the context menu.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The context menu allows setting the Ammo Reload marker. When no ammo can be reloaded, this marker disappears.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The selection of Ready Rack Ammo Reload marker over the Ammo Reload marker supports higher chance of performing rate of fire. &lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The Gun Load marker shows the round in the main gun. The Gun Load marker changes to the Ammo Reload location when the gun is fired. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e060 Reset Round&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since the battle did not end, reset and return back to Spotting Round. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue60' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>e013a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e013a Out of Main Gun Rounds&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Main Gun is empty, and there are no rounds to load. Tehrefore, the main gun cannot be loaded. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue13a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e014 Tank &amp;amp; Turret Orientation&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The Sherman tank counter is placed at the center of the battle board. If you want the turret to face a different sector, select buttons here: 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                             &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
-&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e054b</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e054b MG Firing - Advancing Fire&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Advancing fire attacks infantry targets that move into the zone. It also help protect against Panzerfaust attacks. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 2D for ammo expected:&lt;LineBreak/&gt;
-01 - 30 = 1 box expended&lt;LineBreak/&gt;
-31 - 97 = no effect&lt;LineBreak/&gt;
-98 - 100 = MG malfunctions
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll = &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>e055</t>
-  </si>
-  <si>
-    <t>e056</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e056 Repair Gun&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content=Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e055 Replace Periscopes&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Replacing PERISCOPE_REPLACEMENT out of PERISCOPE_REPLACEMENT_TOTAL left as shown on the After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                        &lt;InlineUIContainer&gt;&lt;Image Name='BrokenPeriscope' Height='222' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click image to continue.</t>
   </si>
 </sst>
 </file>
@@ -1622,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,10 +1746,10 @@
     </row>
     <row r="15" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1757,7 +1757,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1933,7 +1933,7 @@
         <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>160</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2133,39 +2133,39 @@
         <v>81</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2178,10 +2178,10 @@
     </row>
     <row r="69" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2189,7 +2189,7 @@
         <v>128</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2197,7 +2197,7 @@
         <v>146</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2221,7 +2221,7 @@
         <v>140</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2245,15 +2245,15 @@
         <v>145</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2274,26 +2274,26 @@
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2301,7 +2301,7 @@
         <v>152</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
started working on gun malfunction
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAF28001-7721-4A27-BF44-11070CD7A498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F57F13E4-36A0-483C-BA64-6433D6E5571E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -902,17 +902,6 @@
     <t>e053c</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e053a Main Gun Firing - No Target Available&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-There is no target that is selectable. Only enemy units that have been spotted may be selected.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The main gun may only fire at a target in the turret&amp;apos;s front sector unless the &amp;quot;Rotate Turret - Fire Main Gun&amp;quot; action was taken. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue53a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e053 Main Gun Firing - Select Target&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -1257,6 +1246,18 @@
                         &lt;InlineUIContainer&gt;&lt;Image Name='BrokenPeriscope' Height='222' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Click image to continue.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053a Main Gun Firing - No Target Available&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+There is no target that is selectable. Only enemy units that have been spotted may be selected.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The main gun may only fire at a target in the turret&amp;apos;s front sector. 
+Since that is not possible, the gun fires at no target.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll for malfunctioning gun (98, 99, or 100): &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1622,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,10 +1747,10 @@
     </row>
     <row r="15" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1757,7 +1758,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1933,7 +1934,7 @@
         <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1954,26 +1955,26 @@
     </row>
     <row r="41" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2133,39 +2134,39 @@
         <v>81</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2178,10 +2179,10 @@
     </row>
     <row r="69" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2189,15 +2190,15 @@
         <v>128</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2205,15 +2206,15 @@
         <v>129</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>142</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2221,7 +2222,7 @@
         <v>140</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2229,79 +2230,79 @@
         <v>141</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix issue with gun malfunctioning not showing up right
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04FA4F07-65A1-43DB-834E-908C48F92951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{432CD0C4-FA47-408D-9E1B-0949E6C01AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -1255,9 +1255,9 @@
 There is no target that is selectable. Only enemy units that have been spotted may be selected.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The main gun may only fire at a target in the turret&amp;apos;s front sector. 
-Since that is not possible, the gun fires at no target.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll for malfunctioning gun (98, 99, or 100): &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+Since that is not possible, the gun fires at no target. Need to roll for malfunctioning gun (98, 99, or 100). 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll: &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1623,7 +1623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
check point - got gun repair working
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{432CD0C4-FA47-408D-9E1B-0949E6C01AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{469711D8-B835-4E2B-93EE-4558D62A66F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t>e001</t>
   </si>
@@ -1230,13 +1230,6 @@
     <t>e056</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e056 Repair Gun&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content=Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e055 Replace Periscopes&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1258,6 +1251,56 @@
 Since that is not possible, the gun fires at no target. Need to roll for malfunctioning gun (98, 99, or 100). 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Die Roll: &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e056a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;056 Repair Main Gun&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e056a Repair AA Machine Gun&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e056b</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e056b Repair Bow Machine Gun&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e056c</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e056c Repair Coaxial Machine Gun&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e100a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e100a Tank Retires for Today&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Due to broken gun or broken gun sight, the tank must be retired for today. &lt;LineBreak/&gt;
+An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Click image to continue to continue to Crew Rating Improvements per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                  &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1621,10 +1664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B94"/>
+  <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,7 +2257,7 @@
         <v>139</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2286,7 +2329,7 @@
         <v>183</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2294,94 +2337,126 @@
         <v>184</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="88" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>123</v>
+        <v>194</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="97" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Worked Change Load mechanics
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{469711D8-B835-4E2B-93EE-4558D62A66F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{959C023A-F75F-4B48-8E05-698560330E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
   <si>
     <t>e001</t>
   </si>
@@ -1301,6 +1301,56 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                   &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e057</t>
+  </si>
+  <si>
+    <t>e058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e057 Fire 2 Inch Mortar&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r18.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+One Smoke Marker is placed in the close zone in front of turret, and mark off one smoke grenade on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='c58LFireMortar' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e058 Throw Grenade&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r18.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+One Smoke Marker is placed your tank by a crewman throwing a grenade. Mark off one smoke grenade on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='c70ThrowSmokeGrenade' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
+  </si>
+  <si>
+    <t>e059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e059 Restock Ready Rack&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Loader restocks the ready rack from available ammo shown on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click buttons to adjust or the image when done.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+   &lt;InlineUIContainer&gt;&lt;Button Name='HeMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Name='HePlus'  Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HE Ammo&lt;LineBreak/&gt;
+   &lt;InlineUIContainer&gt;&lt;Button Name='ApMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Name='ApPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for AP Ammo&lt;LineBreak/&gt;
+   &lt;InlineUIContainer&gt;&lt;Button Name='WpMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Name='WpPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for WP Ammo&lt;LineBreak/&gt;
+   &lt;InlineUIContainer&gt;&lt;Button Name='HcbiMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Name='HcbiPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HCBI Ammo&lt;LineBreak/&gt;
+   &lt;InlineUIContainer&gt;&lt;Button Name='HvapMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Name='HvapPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HVAP Ammo&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='c60LRestockReadyRack' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
   </si>
 </sst>
 </file>
@@ -1664,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B98"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2364,99 +2414,123 @@
         <v>193</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="92" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="97" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="98" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+    <row r="100" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+    <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Many fixes to combat
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{959C023A-F75F-4B48-8E05-698560330E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D79BFCB-B206-4038-967F-36F1C18C4D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -191,14 +192,6 @@
     <t>e015</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e013 Gun Load&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Mark the type of round you want loaded in the main gun before any action begins by clicking the highlighted box on the Tank Card in the correct ammo type box. Click image below to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c17GunLoad'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e012 Hatches&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -530,16 +523,6 @@
   </si>
   <si>
     <t>e037</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e037 Smoke Depletion Phase&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.71' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Deplete smoke in each zone by converting one white full strength Smoke marker to a gray 1/2 strength Smoke marker. Alternatively, remove 1/2 strength Smoke marker. Refer to 
-&lt;InlineUIContainer&gt;&lt;Button Content='r18.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for the smoke rules. Click image to continue with 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                              &lt;InlineUIContainer&gt;&lt;Image Name='c111Smoke1' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>e038</t>
@@ -1351,6 +1334,24 @@
 &lt;InlineUIContainer&gt;&lt;Button Name='HvapPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HVAP Ammo&lt;LineBreak/&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='c60LRestockReadyRack' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e037 Smoke Depletion Phase&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.71' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Deplete smoke in each zone by converting one white full strength Smoke marker to a gray 1/2 strength Smoke marker. Alternatively, remove 1/2 strength Smoke marker. Refer to 
+&lt;InlineUIContainer&gt;&lt;Button Content='r18.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for the smoke rules. Click image to continue with 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                    &lt;InlineUIContainer&gt;&lt;Image Name='c108Smoke1' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e013 Gun Load&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Mark the type of round you want loaded in the main gun before any action begins by clicking the highlighted box on the Tank Card in the correct ammo type box. If you do not want to load the gun or have finished selecting the gun load, click image below to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c17GunLoad'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1716,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,7 +1780,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1787,7 +1788,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1795,7 +1796,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1803,7 +1804,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1811,7 +1812,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1819,7 +1820,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1827,23 +1828,23 @@
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1851,7 +1852,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1859,639 +1860,639 @@
         <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>83</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working ready rack loading
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D79BFCB-B206-4038-967F-36F1C18C4D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0F26698-FF18-4D21-B5C3-50F332E0C6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1063,28 +1062,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e052a Pivot Turret&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If you want the turret to face a different sector, select buttons here: 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                             &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
-&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e052 Pivot Tank&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If you want the Sherman to face a different sector, select buttons here:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                           &lt;InlineUIContainer&gt;&lt;Button Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;      
-&lt;InlineUIContainer&gt;&lt;Button Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>e050a</t>
   </si>
   <si>
@@ -1313,6 +1290,46 @@
   </si>
   <si>
     <t>e059</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e037 Smoke Depletion Phase&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.71' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Deplete smoke in each zone by converting one white full strength Smoke marker to a gray 1/2 strength Smoke marker. Alternatively, remove 1/2 strength Smoke marker. Refer to 
+&lt;InlineUIContainer&gt;&lt;Button Content='r18.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for the smoke rules. Click image to continue with 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                    &lt;InlineUIContainer&gt;&lt;Image Name='c108Smoke1' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e013 Gun Load&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Mark the type of round you want loaded in the main gun before any action begins by clicking the highlighted box on the Tank Card in the correct ammo type box. If you do not want to load the gun or have finished selecting the gun load, click image below to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c17GunLoad'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e052a Pivot Turret&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you want the turret to face a different sector, select buttons here: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                             &lt;InlineUIContainer&gt;&lt;Button Name='ButtonPivotTurretLeft' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
+&lt;InlineUIContainer&gt;&lt;Button Name='ButtonPivotTurretRight' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e052 Pivot Tank&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you want the Sherman to face a different sector, select buttons here:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                           &lt;InlineUIContainer&gt;&lt;Button Name='ButtonPivotHullLeft' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;      
+&lt;InlineUIContainer&gt;&lt;Button Name='ButtonPivotHullRight' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;Bold&gt;e059 Restock Ready Rack&lt;/Bold&gt; 
@@ -1329,29 +1346,11 @@
    &lt;InlineUIContainer&gt;&lt;Button Name='WpMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Name='WpPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for WP Ammo&lt;LineBreak/&gt;
    &lt;InlineUIContainer&gt;&lt;Button Name='HcbiMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Name='HcbiPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HCBI Ammo&lt;LineBreak/&gt;
-   &lt;InlineUIContainer&gt;&lt;Button Name='HvapMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Name='HbciPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HBCI Ammo&lt;LineBreak/&gt;
+   &lt;InlineUIContainer&gt;&lt;Button Name='' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Name='HvapPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HVAP Ammo&lt;LineBreak/&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='c60LRestockReadyRack' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e037 Smoke Depletion Phase&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.71' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Deplete smoke in each zone by converting one white full strength Smoke marker to a gray 1/2 strength Smoke marker. Alternatively, remove 1/2 strength Smoke marker. Refer to 
-&lt;InlineUIContainer&gt;&lt;Button Content='r18.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for the smoke rules. Click image to continue with 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                    &lt;InlineUIContainer&gt;&lt;Image Name='c108Smoke1' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e013 Gun Load&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Mark the type of round you want loaded in the main gun before any action begins by clicking the highlighted box on the Tank Card in the correct ammo type box. If you do not want to load the gun or have finished selecting the gun load, click image below to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c17GunLoad'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1717,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,15 +1835,15 @@
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1852,7 +1851,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2036,7 +2035,7 @@
         <v>81</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2228,39 +2227,39 @@
         <v>80</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2284,7 +2283,7 @@
         <v>126</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2292,7 +2291,7 @@
         <v>143</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>161</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2308,7 +2307,7 @@
         <v>137</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2340,15 +2339,15 @@
         <v>142</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2369,74 +2368,74 @@
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2444,7 +2443,7 @@
         <v>149</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2457,10 +2456,10 @@
     </row>
     <row r="92" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working ready rack reset
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D79BFCB-B206-4038-967F-36F1C18C4D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{60BB64CA-43C9-461A-A0DF-4D3220356114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1315,6 +1314,24 @@
     <t>e059</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;e037 Smoke Depletion Phase&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.71' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Deplete smoke in each zone by converting one white full strength Smoke marker to a gray 1/2 strength Smoke marker. Alternatively, remove 1/2 strength Smoke marker. Refer to 
+&lt;InlineUIContainer&gt;&lt;Button Content='r18.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for the smoke rules. Click image to continue with 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                    &lt;InlineUIContainer&gt;&lt;Image Name='c108Smoke1' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e013 Gun Load&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Mark the type of round you want loaded in the main gun before any action begins by clicking the highlighted box on the Tank Card in the correct ammo type box. If you do not want to load the gun or have finished selecting the gun load, click image below to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c17GunLoad'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;Bold&gt;e059 Restock Ready Rack&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r16.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
@@ -1322,36 +1339,18 @@
 Loader restocks the ready rack from available ammo shown on the After Action Report 
 &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click buttons to adjust or the image when done.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-   &lt;InlineUIContainer&gt;&lt;Button Name='HeMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Name='HePlus'  Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HE Ammo&lt;LineBreak/&gt;
-   &lt;InlineUIContainer&gt;&lt;Button Name='ApMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Name='ApPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for AP Ammo&lt;LineBreak/&gt;
-   &lt;InlineUIContainer&gt;&lt;Button Name='WpMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Name='WpPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for WP Ammo&lt;LineBreak/&gt;
-   &lt;InlineUIContainer&gt;&lt;Button Name='HcbiMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Name='HcbiPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HCBI Ammo&lt;LineBreak/&gt;
+   &lt;InlineUIContainer&gt;&lt;Button Name='HeMinus' Content='   -   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Name='HePlus'  Content='   +   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HE Ammo&lt;LineBreak/&gt;
+   &lt;InlineUIContainer&gt;&lt;Button Name='ApMinus' Content='   -   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Name='ApPlus' Content='   +   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for AP Ammo&lt;LineBreak/&gt;
+   &lt;InlineUIContainer&gt;&lt;Button Name='WpMinus' Content='   -   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Name='WpPlus' Content='   +   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for WP Ammo&lt;LineBreak/&gt;
+   &lt;InlineUIContainer&gt;&lt;Button Name='HbciMinus' Content='   -   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Name='HbciPlus' Content='   +   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HCBI Ammo&lt;LineBreak/&gt;
    &lt;InlineUIContainer&gt;&lt;Button Name='HvapMinus' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Name='HvapPlus' Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HVAP Ammo&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Name='HvapPlus' Content='   +   '  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for HVAP Ammo&lt;LineBreak/&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='c60LRestockReadyRack' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e037 Smoke Depletion Phase&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.71' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Deplete smoke in each zone by converting one white full strength Smoke marker to a gray 1/2 strength Smoke marker. Alternatively, remove 1/2 strength Smoke marker. Refer to 
-&lt;InlineUIContainer&gt;&lt;Button Content='r18.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for the smoke rules. Click image to continue with 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                    &lt;InlineUIContainer&gt;&lt;Image Name='c108Smoke1' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e013 Gun Load&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Mark the type of round you want loaded in the main gun before any action begins by clicking the highlighted box on the Tank Card in the correct ammo type box. If you do not want to load the gun or have finished selecting the gun load, click image below to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c17GunLoad'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1717,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,7 +1835,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2036,7 +2035,7 @@
         <v>81</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2436,7 +2435,7 @@
         <v>198</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added ellipse display. fixed many issues
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D06FBA9B-3779-44F8-A633-017444252CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AC4B2E1-CB3D-4DA5-BD21-9DA333904254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -1157,16 +1157,6 @@
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue13a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e014 Tank &amp;amp; Turret Orientation&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The Sherman tank counter is placed at the center of the battle board. If you want the turret to face a different sector, select buttons here: 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                             &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
-&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>e054b</t>
   </si>
   <si>
@@ -1350,6 +1340,16 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                              &lt;InlineUIContainer&gt;&lt;Button Name='ButtonPivotTurretLeft'  Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
 &lt;InlineUIContainer&gt;&lt;Button Name='ButtonPivotTurretRight'   Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e014 Tank &amp;amp; Turret Orientation&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Sherman tank counter is placed at the center of the battle board. If you want the turret to face a different sector, select buttons here: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                             &lt;InlineUIContainer&gt;&lt;Button Name='ButtonPivotTurretLeft' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
+&lt;InlineUIContainer&gt;&lt;Button Name='ButtonPivotTurretRight'  Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -1716,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1835,7 +1835,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1851,7 +1851,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2035,7 +2035,7 @@
         <v>81</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2283,7 +2283,7 @@
         <v>126</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2291,7 +2291,7 @@
         <v>143</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
         <v>137</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2368,74 +2368,74 @@
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2456,10 +2456,10 @@
     </row>
     <row r="92" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
final checks for retreat and advance
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AC4B2E1-CB3D-4DA5-BD21-9DA333904254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{447BB872-B256-4C6D-8E80-2CEC4187B054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
   <si>
     <t>e001</t>
   </si>
@@ -1292,14 +1292,6 @@
                                     &lt;InlineUIContainer&gt;&lt;Image Name='c108Smoke1' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e013 Gun Load&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Mark the type of round you want loaded in the main gun before any action begins by clicking the highlighted box on the Tank Card in the correct ammo type box. If you do not want to load the gun or have finished selecting the gun load, click image below to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c17GunLoad'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;Bold&gt;e059 Restock Ready Rack&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r16.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
@@ -1351,6 +1343,30 @@
                                              &lt;InlineUIContainer&gt;&lt;Button Name='ButtonPivotTurretLeft' Content='   -   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;           
 &lt;InlineUIContainer&gt;&lt;Button Name='ButtonPivotTurretRight'  Content='   +   ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e013 Gun Load&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Mark the type of round you want loaded in the main gun before any action begins by clicking the highlighted box on the Tank Card in the correct ammo type box.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Note: You must choose HE gunload if you want to use Advancing Fire when entering a new battle per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; If you do not want to load the gun or have finished selecting the gun load, click image below to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c17GunLoad'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e029a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e029a Advancing Fire Not Allowed&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Advancing fire is only allowed if there is an HE Gun Load per &lt;InlineUIContainer&gt;&lt;Button Content='r9.61' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Choose image below to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFireDeny' Height='120' Width='120'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
 </sst>
 </file>
@@ -1714,10 +1730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,12 +1846,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1851,7 +1867,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1974,563 +1990,571 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="B72" s="2" t="s">
-        <v>140</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="B90" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started adding in switching assistant with others
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{447BB872-B256-4C6D-8E80-2CEC4187B054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0E2FD0F-EEFF-4CF0-AAE3-7DD4509D716C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
   <si>
     <t>e001</t>
   </si>
@@ -1367,6 +1367,17 @@
 Advancing fire is only allowed if there is an HE Gun Load per &lt;InlineUIContainer&gt;&lt;Button Content='r9.61' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Choose image below to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFireDeny' Height='120' Width='120'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>e061</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e061 Crew Switch&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The assistant driver moves through the tank ro replace the incapacitated crewman. The assistant driver takes on the role but at half rating. Click image to  continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='CarryingMan' Height='80' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1730,10 +1741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B102"/>
+  <dimension ref="A1:B103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2470,91 +2481,99 @@
         <v>173</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+    <row r="98" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    <row r="102" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
switching out assistant driver
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0E2FD0F-EEFF-4CF0-AAE3-7DD4509D716C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EA9C71D-6A6A-440D-A597-13B584188CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -1375,9 +1375,9 @@
     <t>&lt;Bold&gt;e061 Crew Switch&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r19.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The assistant driver moves through the tank ro replace the incapacitated crewman. The assistant driver takes on the role but at half rating. Click image to  continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='CarryingMan' Height='80' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+The assistant driver moves through the tank to replace the incapacitated crewman. The assistant driver takes on the role but at half rating. Click image to  continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                                 &lt;InlineUIContainer&gt;&lt;Image Name='CarryingMan' Height='200' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1744,7 +1744,7 @@
   <dimension ref="A1:B103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A90" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added new entry in spreadsheet
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F035160-B7DB-469E-83D6-77DF40B81BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B4811C0-5367-4FC2-8578-F8122891792F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
   <si>
     <t>e001</t>
   </si>
@@ -1387,6 +1387,32 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r19.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The assistant driver moves through the tank to return back to his original position. The assistant driver returns back to his original rating. Click image to  continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                                 &lt;InlineUIContainer&gt;&lt;Image Name='CarryingMan' Height='200' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e062</t>
+  </si>
+  <si>
+    <t>e105</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e105 Crew Replacement - Knocked Out Tank&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r7.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Wounded crewmen are replaced at beginning of day when the tank is knocked out. Click image to  continue to assign new crew ratings.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e062 Crew Replacement - Battle Ends&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r7.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Wounded crewmen are replaced when battle ends or the tank withdraws. Replacing crewmen takes 30 minutes and is marked off the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to assign replacement crew ratings.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                                  &lt;InlineUIContainer&gt;&lt;Image Name='CarryingMan' Height='200' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
@@ -1752,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B104"/>
+  <dimension ref="A1:B106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2508,91 +2534,107 @@
         <v>207</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+    <row r="98" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    <row r="103" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+    <row r="104" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B104" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+    <row r="105" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+    <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented changes for injured crewman
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B4811C0-5367-4FC2-8578-F8122891792F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D0E307C-3C56-48C4-9325-C92EB3A9758C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -1397,14 +1397,6 @@
     <t>e105</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e105 Crew Replacement - Knocked Out Tank&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r7.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Wounded crewmen are replaced at beginning of day when the tank is knocked out. Click image to  continue to assign new crew ratings.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e062 Crew Replacement - Battle Ends&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r7.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
@@ -1414,7 +1406,16 @@
  &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Click image to assign replacement crew ratings.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                                 &lt;InlineUIContainer&gt;&lt;Image Name='CarryingMan' Height='200' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e105 Crew Replacement - Knocked Out Tank&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r7.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Wounded crewmen are replaced at beginning of day when the tank is knocked out. Click image to  continue to assign new crew ratings.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1780,8 +1781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,7 +2540,7 @@
         <v>208</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2590,12 +2591,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>209</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
readded stuff lost about replacing injured crewman
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D0E307C-3C56-48C4-9325-C92EB3A9758C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{02894348-FD7F-4522-90B8-B56D214E1DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -1415,7 +1415,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Wounded crewmen are replaced at beginning of day when the tank is knocked out. Click image to  continue to assign new crew ratings.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                          &lt;InlineUIContainer&gt;&lt;Image Name='AmbulanceEvening' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1781,8 +1781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes to support crew replacements
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{02894348-FD7F-4522-90B8-B56D214E1DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A22F5FE7-CD95-4B02-A917-F2AF378A3177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="218">
   <si>
     <t>e001</t>
   </si>
@@ -130,9 +130,6 @@
 #=Starting or exiting areas
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                    &lt;InlineUIContainer&gt;&lt;Image Name='MapMovement'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>e007</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e001 Fourth Armor Division Campaign&lt;/Bold&gt; 
@@ -349,21 +346,6 @@
 Click on one of the adjacent highlighted areas. Artillery Support or Air Strike Counters are moved to the battle board as a reminder. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                         &lt;InlineUIContainer&gt;&lt;Image Name='Sherman1' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e006 Combat Calendar Check&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll for possible combat today. If die &amp;lt;= probability, start morning briefing per 
-&lt;InlineUIContainer&gt;&lt;Button Content='e007' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  
-Otherwise continue with next day check.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Date from Combat Calendar: DATE&lt;LineBreak/&gt;
-Expected Resistance: RESISTANCE&lt;LineBreak/&gt;
-Probablility of Combat: PROBABILITY &amp;gt;= 
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e018 Set Start Area&lt;/Bold&gt; 
@@ -1394,7 +1376,7 @@
     <t>e062</t>
   </si>
   <si>
-    <t>e105</t>
+    <t>e062a</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e062 Crew Replacement - Battle Ends&lt;/Bold&gt; 
@@ -1406,16 +1388,68 @@
  &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Click image to assign replacement crew ratings.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e105 Crew Replacement - Knocked Out Tank&lt;/Bold&gt; 
+                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance1' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e062a Crew Replacement - Advance or Retreat&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r7.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Wounded crewmen are replaced when your Sherman Advances or Retreats. Replacing crewmen takes 30 minutes and is marked off the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to assign replacement crew ratings.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance2' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e007a</t>
+  </si>
+  <si>
+    <t>e007b</t>
+  </si>
+  <si>
+    <t>e008a</t>
+  </si>
+  <si>
+    <t>e007c</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007c Tank Replacement&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007b Returning Crewmen&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Convalenced crewmen return to your crew or leave to work another crew base on your choice. If returning to your crew, they replace the existing man. If you do not bring back the crewman, he may not rejoin later. Choose one of the options below:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007a Crew Replacement&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r7.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Wounded crewmen are replaced at beginning of day when the tank is knocked out. Click image to  continue to assign new crew ratings.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                          &lt;InlineUIContainer&gt;&lt;Image Name='AmbulanceEvening' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance3' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e006 Combat Calendar Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll for possible combat today. If die &amp;lt;= probability, start morning briefing per 
+&lt;InlineUIContainer&gt;&lt;Button Content='e007' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  
+Otherwise continue with next day check.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Date from Combat Calendar: DATE&lt;LineBreak/&gt;
+Scenario Type: SCENARIO&lt;LineBreak/&gt;
+Expected Resistance: RESISTANCE&lt;LineBreak/&gt;
+Probablility of Combat: PROBABILITY &amp;gt;= 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1779,10 +1813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B106"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1828,7 +1862,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1836,806 +1870,830 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>210</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>211</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>213</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>212</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>174</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>175</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="2" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="2" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B23" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B24" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="B43" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="B48" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="B49" s="2" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="B77" s="2" t="s">
-        <v>144</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    </row>
+    <row r="81" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    </row>
+    <row r="83" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    </row>
+    <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="B86" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B88" s="2" t="s">
+    </row>
+    <row r="92" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="B93" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    </row>
+    <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="97" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B97" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+    </row>
+    <row r="103" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+    <row r="106" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+    <row r="107" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B107" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+    <row r="108" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+    <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
major changes for finishing injuried crewman
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A22F5FE7-CD95-4B02-A917-F2AF378A3177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{381CE7DA-51CB-4440-810E-13BE5503DFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
   <si>
     <t>e001</t>
   </si>
@@ -1415,27 +1416,6 @@
     <t>e007c</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e007c Tank Replacement&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e007b Returning Crewmen&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Convalenced crewmen return to your crew or leave to work another crew base on your choice. If returning to your crew, they replace the existing man. If you do not bring back the crewman, he may not rejoin later. Choose one of the options below:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e007a Crew Replacement&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r7.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Wounded crewmen are replaced at beginning of day when the tank is knocked out. Click image to  continue to assign new crew ratings.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance3' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e006 Combat Calendar Check&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
@@ -1450,6 +1430,36 @@
 Probablility of Combat: PROBABILITY &amp;gt;= 
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e007d</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007d Tank Replacement&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007a Crew Healing&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The following crewmen are convalesing in a medical hosptial and may rejoin your crew when they are better:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007b Crew Replacement&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Wounded crewmen are replaced at beginning of day when the tank is knocked out. Click image to  continue to assign new crew ratings.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance3' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007c Returning Crewmen&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Convalenced crewmen return to your crew or leave to work another crew base on your choice. If returning to your crew, they replace the existing man. If you do not bring back the crewman, he may not rejoin later. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1813,10 +1823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B109"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,15 +1888,15 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>210</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1894,806 +1904,814 @@
         <v>211</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>213</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>215</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>202</v>
+        <v>147</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+    <row r="104" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B104" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+    <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B107" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+    <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+    <row r="109" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+    <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new tanks and mats
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B521C9C-1E66-4BD2-B7E1-5BAAD1424D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D46D5C5F-F11F-4615-AFCB-EBA181CFF7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -158,15 +158,6 @@
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue005' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e004 Tank Card&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The upper right image is the Tank Card. The game starts with the basic M4 Sherman tank, i.e., Tank Card #1. 
-The Tank Card shows the tank model and other important information regarding the tank. The use of the Tank Card is described in 
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                 &lt;InlineUIContainer&gt;&lt;Image Name='m001M4'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>e009</t>
   </si>
   <si>
@@ -1464,6 +1455,15 @@
 Consult the Tank 
 &lt;InlineUIContainer&gt;&lt;Button Content='Replacement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table after rolling two die: 
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e004 Tank Card&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The upper right image is the Tank Card. The game starts with the basic M4 Sherman tank, i.e., Tank Card #1. 
+The Tank Card shows the tank model and other important information regarding the tank. The use of the Tank Card is described in 
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                 &lt;InlineUIContainer&gt;&lt;Image Name='m01'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1829,8 +1829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1876,7 +1876,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1892,39 +1892,39 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1932,751 +1932,751 @@
         <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
HVAP ammo working on ammo load
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABB05999-567C-48A1-A719-BBFFC24C9542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90FBA2E0-F329-4F8C-A52B-1956A4B8689B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -331,6 +331,14 @@
 &lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;e028 Enter Adjacent Area&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click on one of the adjacent highlighted areas. Artillery Support or Air Strike Counters are moved to the battle board as a reminder. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                        &lt;InlineUIContainer&gt;&lt;Image Name='Sherman1' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e018 Set Start Area&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1458,14 +1466,6 @@
  In either case, consult the Tank 
 &lt;InlineUIContainer&gt;&lt;Button Content='Replacement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table after rolling two die: 
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e028 Enter Adjacent Area&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click on one of the adjacent highlighted areas. Artillery Support or Air Strike Counters are moved to the battle board as a reminder. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                        &lt;InlineUIContainer&gt;&lt;Image Name='Sherman75' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1832,7 +1832,7 @@
   <dimension ref="A1:B110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1878,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1894,39 +1894,39 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1934,15 +1934,15 @@
         <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1958,7 +1958,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1966,7 +1966,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1982,15 +1982,15 @@
         <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1998,7 +1998,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2030,7 +2030,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2038,7 +2038,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2054,7 +2054,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -2078,7 +2078,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2094,7 +2094,7 @@
         <v>46</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2102,7 +2102,7 @@
         <v>45</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2110,7 +2110,7 @@
         <v>48</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>219</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2123,10 +2123,10 @@
     </row>
     <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2134,7 +2134,7 @@
         <v>52</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2142,7 +2142,7 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2150,535 +2150,535 @@
         <v>54</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added capability for HVSS being set
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90FBA2E0-F329-4F8C-A52B-1956A4B8689B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD948C6B-D689-4CF6-8A88-033F471AEA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="222">
   <si>
     <t>e001</t>
   </si>
@@ -1466,6 +1466,18 @@
  In either case, consult the Tank 
 &lt;InlineUIContainer&gt;&lt;Button Content='Replacement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table after rolling two die: 
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e007e</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007e Horizontal Volute Spring Suspension (HVSS)&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.25' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A gyrostabilizer was attached to the main gun of the Sherman tank is to keep the gun stabilized, or steady, in the vertical axis (up-down). Even if your tank has a gyrostabilizer, it requires the crew to be trained during a refit period before it can be used. A 1D die roll is necessary to determine if you tank has HVSS installed.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll = &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1829,10 +1841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,795 +1941,803 @@
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>220</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>68</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>201</v>
+        <v>146</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+    <row r="104" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B104" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+    <row r="105" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+    <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+    <row r="109" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+    <row r="110" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+    <row r="111" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
verified HVSS is working
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD948C6B-D689-4CF6-8A88-033F471AEA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F92A37E7-6788-4518-983F-1ACEBF5BF302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -1449,15 +1449,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e007b Crew Replacement&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When you tank is knocked out, wounded crewmen are replaced in morning briefing if combat may occur this day  per 
-&lt;InlineUIContainer&gt;&lt;Button Content='e006' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to  continue to assign new crew ratings.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance3' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e007d Tank Replacement&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r24.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1475,9 +1466,20 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r5.25' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-A gyrostabilizer was attached to the main gun of the Sherman tank is to keep the gun stabilized, or steady, in the vertical axis (up-down). Even if your tank has a gyrostabilizer, it requires the crew to be trained during a refit period before it can be used. A 1D die roll is necessary to determine if you tank has HVSS installed.
+A gyrostabilizer was attached to the main gun of the Sherman tank to keep the gun stabilized, or steady, in the vertical axis (up-down). 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Even if your tank has a gyrostabilizer, it requires the crew to be trained during a refit period before it can be used. Roll 1D to determine if you tank has HVSS installed per tank card.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Die Roll = &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007b Crew Replacement&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When you tank is knocked out, wounded crewmen are replaced in morning briefing if combat may occur this day per 
+&lt;InlineUIContainer&gt;&lt;Button Content='e006' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue to assign new replacement crew.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance3' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1843,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,7 +1924,7 @@
         <v>210</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1938,15 +1940,15 @@
         <v>214</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working on harrassing fire modifier
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F92A37E7-6788-4518-983F-1ACEBF5BF302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F9CBC2B-2D54-4975-934E-52EE143E8665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -678,17 +678,6 @@
 &lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e045 Harrassing Fire&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Your tank is sprayed with small weapons fire. Roll on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Collateral' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Damage Table. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                        &lt;InlineUIContainer&gt;&lt;Image Name='CollateralDamage' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>e101</t>
   </si>
   <si>
@@ -1480,6 +1469,14 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='e006' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue to assign new replacement crew.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                           &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance3' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e045 Harrassing Fire&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Your tank is sprayed with small weapons fire.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Collateral' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Damage Table. </t>
   </si>
 </sst>
 </file>
@@ -1845,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,7 +1889,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1908,47 +1905,47 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1961,7 +1958,7 @@
     </row>
     <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>69</v>
@@ -2004,15 +2001,15 @@
         <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2020,7 +2017,7 @@
         <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2145,10 +2142,10 @@
     </row>
     <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2204,7 +2201,7 @@
         <v>70</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2212,7 +2209,7 @@
         <v>78</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2225,26 +2222,26 @@
     </row>
     <row r="47" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2252,7 +2249,7 @@
         <v>80</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2260,7 +2257,7 @@
         <v>82</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2268,7 +2265,7 @@
         <v>83</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2343,12 +2340,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>111</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2356,7 +2353,7 @@
         <v>87</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2364,7 +2361,7 @@
         <v>93</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -2372,7 +2369,7 @@
         <v>88</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2380,7 +2377,7 @@
         <v>89</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2388,7 +2385,7 @@
         <v>94</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2396,7 +2393,7 @@
         <v>90</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2404,255 +2401,255 @@
         <v>77</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2660,47 +2657,47 @@
         <v>106</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix some issues with rolling over when tank is destroyed
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F9CBC2B-2D54-4975-934E-52EE143E8665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E74229-7438-4808-A09B-19EC2C03F61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="227">
   <si>
     <t>e001</t>
   </si>
@@ -1477,6 +1477,41 @@
 Your tank is sprayed with small weapons fire.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll on the 
 &lt;InlineUIContainer&gt;&lt;Button Content='Collateral' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Damage Table. </t>
+  </si>
+  <si>
+    <t>e006a</t>
+  </si>
+  <si>
+    <t>e006b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e006a Retrofit Period&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During the periods on the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ marked Refitting, the Division is building itself back up to strength, replacing tanks, and retraining new crews. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During a refit period, you have the option of replacing your current tank per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r24.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e006b Retrofit Period - Crew Training&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Since the refit takes at least 7 days, you may attempt to improve your crew ratings per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+and train your crew to use the gyrostablilizer per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e006b Retrofit Period - Gyrostabilizer&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+When the refit takes at least 7 days, and your crew has a combined rating of 30, your crew is trained in the use of the gyrostablilizer per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.21' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Loss of the gunner losses the Horizontal Volute Spring Suspension (HVSS) capability. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c75Hvss'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1840,10 +1875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B111"/>
+  <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B12" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1908,835 +1943,859 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="15" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>210</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>170</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>171</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="28" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="29" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="35" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="41" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="47" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="48" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="50" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="51" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="52" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="53" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="66" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="71" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="72" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="73" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="75" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="76" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="77" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="78" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="79" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="80" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="81" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="82" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="88" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="89" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="90" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="91" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="96" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="97" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="98" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    <row r="99" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+    <row r="100" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+    <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    <row r="102" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    <row r="103" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    <row r="104" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B104" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+    <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+    <row r="110" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+    <row r="111" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+    <row r="112" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+    <row r="113" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+    <row r="114" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finialized transition to new day
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E74229-7438-4808-A09B-19EC2C03F61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFEAC371-56CB-4318-A8F2-FD9AA7E2F758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="228">
   <si>
     <t>e001</t>
   </si>
@@ -1485,18 +1485,6 @@
     <t>e006b</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;e006a Retrofit Period&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-During the periods on the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- marked Refitting, the Division is building itself back up to strength, replacing tanks, and retraining new crews. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-During a refit period, you have the option of replacing your current tank per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r24.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e006b Retrofit Period - Crew Training&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r27.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -1506,7 +1494,21 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e006b Retrofit Period - Gyrostabilizer&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;e006a Retrofit Period&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During the periods on the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ marked Refitting, the Division is building itself back up to strength, replacing tanks, and retraining new crews. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During a refit period, you have the option of replacing your current tank per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r24.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e006c</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e006c Retrofit Period - Gyrostabilizer&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 When the refit takes at least 7 days, and your crew has a combined rating of 30, your crew is trained in the use of the gyrostablilizer per 
 &lt;InlineUIContainer&gt;&lt;Button Content='r27.21' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Loss of the gunner losses the Horizontal Volute Spring Suspension (HVSS) capability. Click image to continue.
@@ -1877,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B11:B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,12 +1945,12 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>222</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -1956,15 +1958,15 @@
         <v>223</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
implement HVSS in retrofit
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BF58D5F-81A9-400A-9AA1-CDBAE2D1522F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{616F1122-BC7F-44A2-84D4-261B96036FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1489,31 +1488,34 @@
     <t>e006c</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;e006b Retrofit Period - Crew Training&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since the refit takes at least 7 days, you may attempt to improve your crew ratings. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue06b' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e006a Retrofit Period&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During the periods on the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ marked Refitting, the Division is building itself back up to strength, replacing tanks, and retraining crews. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During a refit period, you have the option of replacing your current tank per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r24.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e006c Retrofit Period - Gyrostabilizer&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Since the refit takes at least 7 days, and your crew has a combined rating of 30, your crew is trained in the use of the gyrostablilizer per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r27.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Loss of the gunner losses the Horizontal Volute Spring Suspension (HVSS) capability. Click image to continue.
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Loss of the gunner loses the Horizontal Volute Spring Suspension (HVSS) capability. Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                                   &lt;InlineUIContainer&gt;&lt;Image Name='c75Hvss'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e006b Retrofit Period - Crew Training&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r27.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since the refit takes at least 7 days, you may attempt to improve your crew ratings. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue06b' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e006a Retrofit Period&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-During the periods on the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- marked Refitting, the Division is building itself back up to strength, replacing tanks, and retraining crews. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-During a refit period, you have the option of replacing your current tank per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r24.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1879,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,7 +1952,7 @@
         <v>222</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1958,15 +1960,15 @@
         <v>223</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>224</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix issues with showing dialog not reappearing
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7533D82C-C5AC-4C10-87B0-256F38567855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4452B41C-2E27-4CB0-91D0-2908F6B32F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="232">
   <si>
     <t>e001</t>
   </si>
@@ -397,15 +397,6 @@
 to see if resupply occurs. If successful, you may relead your tank with ammo. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine your tank&amp;apos;s deployment from the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
@@ -1516,6 +1507,44 @@
  Table determines weather for today:  
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e011a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine your tank&amp;apos;s deployment from the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table:  Die Roll =
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e011a Deployment - Counterattack Scenario&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since this is a Counterattack scenario, your tank&amp;apos;s deployment is automatically stopped and hull down.  You must still roll for if your tank is the lead tank per the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. Die Roll =
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e032a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e032a Battle Check - Counterattack&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Time: TIME_OF_DAY   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Each 15 minutes during a counterattach scenario, battle may occur or you may choose resupply.
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Choose 
+&lt;InlineUIContainer&gt;&lt;Button Content='Resupply' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; or 
+roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to determine if combat occurs by counterattacking German forces: 
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
 </sst>
 </file>
@@ -1879,10 +1908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B114"/>
+  <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,7 +1957,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1944,71 +1973,71 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2016,15 +2045,15 @@
         <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2040,7 +2069,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2048,758 +2077,774 @@
         <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="B25" s="2" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    </row>
+    <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="B42" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="47" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="B51" s="2" t="s">
-        <v>149</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="B54" s="2" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="B58" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    </row>
+    <row r="79" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B77" s="2" t="s">
+    </row>
+    <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B78" s="2" t="s">
+      <c r="B81" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    </row>
+    <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="B88" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B90" s="2" t="s">
+    </row>
+    <row r="93" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="B93" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    </row>
+    <row r="98" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B97" s="2" t="s">
+    <row r="100" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="B100" s="2" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B101" s="2" t="s">
+    </row>
+    <row r="104" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="B104" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+    <row r="106" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B105" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+    </row>
+    <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+    <row r="113" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+    <row r="114" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+    <row r="115" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+    <row r="116" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix some of rule links
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4452B41C-2E27-4CB0-91D0-2908F6B32F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8CBBD6AE-DF70-4410-A4C9-AEF12AD6E2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -1910,8 +1910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
continuing work on counter attack
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8CBBD6AE-DF70-4410-A4C9-AEF12AD6E2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01C8B33C-F407-45C4-9133-D6B1CEFD9A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -485,18 +485,6 @@
     <t>e040</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r21.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
-Roll 1D on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. 
-The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>e041</t>
   </si>
   <si>
@@ -1521,15 +1509,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e011a Deployment - Counterattack Scenario&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since this is a Counterattack scenario, your tank&amp;apos;s deployment is automatically stopped and hull down.  You must still roll for if your tank is the lead tank per the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. Die Roll =
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>e032a</t>
   </si>
   <si>
@@ -1538,13 +1517,39 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Time: TIME_OF_DAY   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Each 15 minutes during a counterattach scenario, battle may occur or you may choose resupply.
+Each 15 minutes during a counterattack scenario, battle may occur or you may choose resupply.
  &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Choose 
 &lt;InlineUIContainer&gt;&lt;Button Content='Resupply' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; or 
 roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 Table to determine if combat occurs by counterattacking German forces: 
 Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e010 Time Check&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r21.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine sunrise and sunset for current month using the &lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
+Roll 1D on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Time Table also provides the timed used for each action take. Additionally, the same die roll is used to determine the ammo expended:  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll = 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e011a Deployment - Counterattack Scenario&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since this is a Counterattack scenario, your tank&amp;apos;s deployment is automatically stopped and hull down.  You must still roll for if your tank is the lead tank per the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1910,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1957,7 +1962,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1973,71 +1978,71 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2045,12 +2050,12 @@
         <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>67</v>
@@ -2064,12 +2069,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>79</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2077,15 +2082,15 @@
         <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2101,15 +2106,15 @@
         <v>27</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2117,7 +2122,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2242,10 +2247,10 @@
     </row>
     <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2274,10 +2279,10 @@
     </row>
     <row r="45" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2309,7 +2314,7 @@
         <v>68</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2317,7 +2322,7 @@
         <v>76</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2325,31 +2330,31 @@
         <v>77</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2357,151 +2362,151 @@
         <v>78</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2509,303 +2514,303 @@
         <v>75</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First part of counterattack working
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5E2E7BF-FDED-4A78-9EEB-CD8972AAE27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A576E91-6050-418B-AB32-56F202F9EE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="232">
   <si>
     <t>e001</t>
   </si>
@@ -1518,24 +1518,24 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine your tank&amp;apos;s deployment from the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e011a Deployment - Counterattack Scenario&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Since this is a Counterattack scenario, your tank&amp;apos;s deployment is automatically stopped and hull down.  You must still roll for if your tank is the lead tank per the 
 &lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine your tank&amp;apos;s deployment from the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =
+Die Roll = 
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
@@ -1544,24 +1544,14 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r20.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Time: TIME_OF_DAY   
+Resistance: RESISTANCE_OF_DAY&lt;LineBreak/&gt;
+Area Type: AREA_TYPE&lt;LineBreak/&gt;
  &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Choose 
 &lt;InlineUIContainer&gt;&lt;Button Content='Resupply' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; or 
 roll 1D and consult the &lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 Table to determine if combat occurs by counterattacking German forces: 
 Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-  </si>
-  <si>
-    <t>e033a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e033a No Combat - Counterattack&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Mark off 15 minutes on the After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and roll again. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue33a' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1925,10 +1915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B117"/>
+  <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,7 +2084,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2102,7 +2092,7 @@
         <v>226</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2289,7 +2279,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>227</v>
       </c>
@@ -2305,571 +2295,563 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>232</v>
+        <v>65</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>150</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>192</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>188</v>
+        <v>142</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>142</v>
+        <v>197</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>103</v>
+        <v>182</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>113</v>
+        <v>183</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>182</v>
+        <v>108</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>114</v>
+        <v>2</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B117" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final touches on counterattack scenario without combat
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A576E91-6050-418B-AB32-56F202F9EE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FB69B11-D0CF-46A1-B834-8BE91F732EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -1543,9 +1543,9 @@
     <t xml:space="preserve">&lt;Bold&gt;e032a Battle Check - Counterattack&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r20.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Time: TIME_OF_DAY   
+Time: TIME_OF_DAY   &lt;LineBreak/&gt;
 Resistance: RESISTANCE_OF_DAY&lt;LineBreak/&gt;
-Area Type: AREA_TYPE&lt;LineBreak/&gt;
+Area Type: AREA_TYPE
  &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Choose 
 &lt;InlineUIContainer&gt;&lt;Button Content='Resupply' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; or 

</xml_diff>

<commit_message>
trying to get counterattack battle results working
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{122F00D4-E3F9-40F5-8A1B-5429969B8DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5460F382-F88F-4737-B54C-36327A85AE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -132,20 +132,6 @@
                                    &lt;InlineUIContainer&gt;&lt;Image Name='MapMovement'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e001 Fourth Armor Division Campaign&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r1.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The campaign game of &lt;Bold&gt;Patton' Best&lt;/Bold&gt; recreates the actions of the 4th Armored Division from late July 1944 through April 1945. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Each day begins with a check of the Combat 
-&lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; to see what the Division was doing on that day. The four possibilities are Refitting 
-&lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, an Advance scenario &lt;InlineUIContainer&gt;&lt;Button Content='r20.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, a Battle scenario 
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, or a Counterattack scenario 
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue001' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>e008</t>
   </si>
   <si>
@@ -1529,17 +1515,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e011a Deployment - Counterattack Scenario&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since this is a Counterattack scenario, your tank&amp;apos;s deployment is automatically stopped and hull down.  You must still roll for if your tank is the lead tank per the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll = 
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;Bold&gt;e032a Battle Check - Counterattack&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r20.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1567,6 +1542,29 @@
 &lt;LineBreak/&gt;
 2.) Roll 1D/2 (rounded down) + 1 hour for elaped time.  Die Roll = 
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e001 Fourth Armor Division Campaign&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r1.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The campaign game of &lt;Bold&gt;Patton' Best&lt;/Bold&gt; recreates the actions of the 4th Armored Division from late July 1944 through April 1945. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Each day begins with a check of the Combat 
+&lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to see what the Division was doing on that day. The four possibilities are Refitting 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
+an Advance scenario &lt;InlineUIContainer&gt;&lt;Button Content='r20.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, a Battle scenario 
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, or a Counterattack scenario 
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue001' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e011a Deployment - Counterattack Scenario&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since this is a Counterattack scenario, your tank&amp;apos;s deployment is automatically stopped and hull down.  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1932,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,7 +1953,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1979,7 +1977,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1987,7 +1985,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -1995,847 +1993,847 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
counterattack working with battle. Still need to implement retreat
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5460F382-F88F-4737-B54C-36327A85AE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6086AD5B-33A4-47DD-98E2-9A58A91C2DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -1504,17 +1504,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine your tank&amp;apos;s deployment from the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;Bold&gt;e032a Battle Check - Counterattack&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r20.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1564,6 +1553,17 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Since this is a Counterattack scenario, your tank&amp;apos;s deployment is automatically stopped and hull down.  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine your tank&amp;apos;s deployment from the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll = 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -1931,7 +1931,7 @@
   <dimension ref="A1:B117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,7 +1953,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
         <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2105,7 +2105,7 @@
         <v>225</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2297,7 +2297,7 @@
         <v>226</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2334,10 +2334,10 @@
     </row>
     <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="120" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final testing of Random Event test cases when units disappear
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6086AD5B-33A4-47DD-98E2-9A58A91C2DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BBEC36F-221D-4189-A5FA-D7CEA6481DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -375,17 +375,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e027 Attempt to Resupply&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Consult the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-to see if resupply occurs. If successful, you may relead your tank with ammo. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>e033</t>
   </si>
   <si>
@@ -1564,6 +1553,17 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Die Roll = 
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e027 Attempt to Resupply&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to see if resupply occurs. If successful, you may relead your tank with ammo. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -1930,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,7 +1953,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1977,7 +1977,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1993,71 +1993,71 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2065,15 +2065,15 @@
         <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2089,7 +2089,7 @@
         <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2097,15 +2097,15 @@
         <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2121,15 +2121,15 @@
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2137,7 +2137,7 @@
         <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>44</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>62</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2262,10 +2262,10 @@
     </row>
     <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2273,7 +2273,7 @@
         <v>51</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2281,7 +2281,7 @@
         <v>52</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2289,551 +2289,551 @@
         <v>53</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implement ambush for counterattack
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BBEC36F-221D-4189-A5FA-D7CEA6481DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{77B2D5AC-3949-4514-859F-5C6EFF13DD9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -504,16 +504,6 @@
     <t>e048a</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e038 Orders Phase&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click on blue squares to open hatches. Click on Open Hatch marker to close.
- &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Right click crew member action boxes to select from a pull down to assign crew actions for each crew member.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e043a Mine Attack Ignored&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r15.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1565,6 +1555,16 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e038 Orders Phase&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+CREW ACTIONS: Right click crew member action boxes to select from a pull down to assign crew actions for each crew member.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+HATCHES: Click on blue squares to open hatches, or click on Open Hatch marker to close.
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1930,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,7 +1953,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1977,7 +1977,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1993,71 +1993,71 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2065,12 +2065,12 @@
         <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>65</v>
@@ -2089,7 +2089,7 @@
         <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2097,15 +2097,15 @@
         <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2121,15 +2121,15 @@
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2137,7 +2137,7 @@
         <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>44</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2262,10 +2262,10 @@
     </row>
     <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2294,10 +2294,10 @@
     </row>
     <row r="45" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2329,15 +2329,15 @@
         <v>66</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2345,7 +2345,7 @@
         <v>74</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2353,31 +2353,31 @@
         <v>75</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>90</v>
+        <v>233</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2385,7 +2385,7 @@
         <v>76</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2393,7 +2393,7 @@
         <v>77</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2401,7 +2401,7 @@
         <v>78</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2417,31 +2417,31 @@
         <v>86</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2449,31 +2449,31 @@
         <v>80</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2481,7 +2481,7 @@
         <v>81</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2489,7 +2489,7 @@
         <v>82</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2497,7 +2497,7 @@
         <v>88</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -2505,7 +2505,7 @@
         <v>83</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2513,7 +2513,7 @@
         <v>84</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2521,7 +2521,7 @@
         <v>89</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
         <v>85</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2537,303 +2537,303 @@
         <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added test case for etreating into enemy territory
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7BFF9F07-C782-4444-901B-02DEE71906C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B34A2E4-9546-4ADF-87A4-81CF4FD58DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="240">
   <si>
     <t>e001</t>
   </si>
@@ -1590,6 +1590,19 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r20.45' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 If you leave the engagement by advancing (moving forward) or retreating (moving backwards), you move to a new area. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                        &lt;InlineUIContainer&gt;&lt;Image Name='Sherman1' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to continue.  </t>
+  </si>
+  <si>
+    <t>e099a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e099a Retreat into a Battle&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You retreated into a battle.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                         &lt;InlineUIContainer&gt;&lt;Image Name='Sherman1' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1957,10 +1970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B119"/>
+  <dimension ref="A1:B120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2833,91 +2846,99 @@
         <v>237</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+    <row r="113" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+    <row r="114" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+    <row r="115" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B117" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+    <row r="118" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+    <row r="119" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+    <row r="120" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added hooks in for choosing path to retreat in counterattack
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B34A2E4-9546-4ADF-87A4-81CF4FD58DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E01EE2F-B78F-4F77-B516-AE96ADDE0AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
   <si>
     <t>e001</t>
   </si>
@@ -1607,6 +1607,18 @@
                         &lt;InlineUIContainer&gt;&lt;Image Name='Sherman1' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Click image to continue.  </t>
+  </si>
+  <si>
+    <t>e099b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e099b Retreat Choice in Counterattack Retreat&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.45' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Must retreat to an adjacent hex toward the start area. Since two or more choices exist, choose one of the highlighted areas on the movement board to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                        &lt;InlineUIContainer&gt;&lt;Image Name='Sherman1' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
   </si>
 </sst>
 </file>
@@ -1970,10 +1982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B120"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A108" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2856,89 +2868,97 @@
     </row>
     <row r="110" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+    <row r="114" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+    <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+    <row r="116" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+    <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+    <row r="120" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+    <row r="121" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B121" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working though showing options
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A2E1A3B-589C-44F9-9FC0-497786FD983E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8F6A8F6-E097-4441-8F77-26C1486EB245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -1559,8 +1559,18 @@
                         &lt;InlineUIContainer&gt;&lt;Image Name='Sherman1' Height='200' Width='325'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
   </si>
   <si>
+    <t>&lt;Bold&gt;e005 After Action Report (AAR)&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial5' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The events of each engagement or day of battle are recorded as they unfold on the After Action Report. At this time, you may elect to change the name of the tank or the names of your crew by clicking on the appropriate location on the form. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When ready, click image below to assign crew ratings to your new crew per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r7.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue005' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e000 Welcome to Patton's Best Solo Tank Battle Game&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial0' IsChecked='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial0' IsEnabled='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The game starts with a tutorial how to play. However, before starting, it is important to know that Active events are shown with a green background. The game may only advance when a green background is displayed. Most often, the game advances by rolling dice or clicking an image. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1568,11 +1578,12 @@
 &lt;LineBreak/&gt;
                &lt;InlineUIContainer&gt;&lt;Image Name='Tutorial0' Height='70'  Width='370'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Name='Read_Rules' Content='Read Rules' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt; or &lt;InlineUIContainer&gt;&lt;Button Name='Begin' Content='Begin Game' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
+&lt;InlineUIContainer&gt;&lt;Button Name='Read_Rules' Content='Read Rules' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt; or 
+&lt;InlineUIContainer&gt;&lt;Button Name='Begin' Content='Begin Game' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e001 Fourth Armor Division Campaign&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r1.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial1' IsChecked='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial1' IsEnabled='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The campaign game of &lt;Bold&gt;Patton' Best&lt;/Bold&gt; recreates the actions of the 4th Armored Division from late July 1944 through April 1945. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1588,7 +1599,7 @@
   </si>
   <si>
     <t>&lt;Bold&gt;e002 Movement Board&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial2' IsChecked='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial2' IsEnabled='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The movement board is a depiction fo typical European countryside and is used to show the "big picture" for the day. The movement board is divided into white lines into areas. Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1598,32 +1609,22 @@
                                    &lt;InlineUIContainer&gt;&lt;Image Name='MapMovement'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;e003 Battle Board&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial3' IsEnabled='True'  Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The battle board is an abstract display used to resolve engagements with enemy forces. Your tank is placed in the center of this display and the action of an engagement revolves around it through the use of pieces representing enemy units and other informational markers. A detailed explanation is given in &lt;InlineUIContainer&gt;&lt;Button Content='r5.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                   &lt;InlineUIContainer&gt;&lt;Image Name='MapBattle'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e004 Tank Card&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial4' IsChecked='True'  Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial4' IsEnabled='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The upper right image is the Tank Card. The game starts with the basic M4 Sherman tank, i.e., Tank Card #1. 
 The Tank Card shows the tank model and other important information regarding the tank. The use of the Tank Card is described in 
 &lt;InlineUIContainer&gt;&lt;Button Content='r5.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                  &lt;InlineUIContainer&gt;&lt;Image Name='m01'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e003 Battle Board&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial3' IsChecked='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The battle board is an abstract display used to resolve engagements with enemy forces. Your tank is placed in the center of this display and the action of an engagement revolves around it through the use of pieces representing enemy units and other informational markers. A detailed explanation is given in &lt;InlineUIContainer&gt;&lt;Button Content='r5.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                   &lt;InlineUIContainer&gt;&lt;Image Name='MapBattle'  Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e005 After Action Report (AAR)&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r2.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial5' IsChecked='True'  Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The events of each engagement or day of battle are recorded as they unfold on the After Action Report. At this time, you may elect to change the name of the tank or the names of your crew by clicking on the appropriate location on the form. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;When ready, click image below to assign crew ratings to your new crew per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r7.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue005' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1989,8 +1990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,7 +2005,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2012,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2020,7 +2021,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2036,15 +2037,15 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="210" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working option to skip ammo setup
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80BE255A-F03E-42E4-8096-302BDEC63A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{59E4B312-190E-4B54-BE25-2F5982EC4A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -268,18 +268,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Enter' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e009 Ammo Loading Limits&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r16.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-See 
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-for ammo types. See 
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-for loading ammo. The Tank Card limits the number of normal main gun ammo allowed to AMMO_NORMAL_LOAD. Extra ammo is added in a later step after assigning normal load.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;Bold&gt;-- AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
-&lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e028 Enter Adjacent Area&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1625,6 +1613,19 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e009 Ammo Loading Limits&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r16.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoRollAmmoLoad' IsEnabled='True' Content='Automatically Load Ammo' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+for ammo types. See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+for loading ammo. The Tank Card limits the number of normal main gun ammo allowed to AMMO_NORMAL_LOAD. Extra ammo is added in a later step after assigning normal load.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Bold&gt;-- AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
+&lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
   </si>
 </sst>
 </file>
@@ -1990,8 +1991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2005,7 +2006,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2013,7 +2014,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2021,7 +2022,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2029,7 +2030,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2037,7 +2038,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2045,7 +2046,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2053,79 +2054,79 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2133,23 +2134,23 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>51</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -2157,7 +2158,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2165,15 +2166,15 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2189,15 +2190,15 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2205,7 +2206,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2237,7 +2238,7 @@
         <v>31</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2245,7 +2246,7 @@
         <v>32</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2261,7 +2262,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -2285,7 +2286,7 @@
         <v>38</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2301,7 +2302,7 @@
         <v>41</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2309,7 +2310,7 @@
         <v>40</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2317,7 +2318,7 @@
         <v>43</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2330,10 +2331,10 @@
     </row>
     <row r="42" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2341,7 +2342,7 @@
         <v>47</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2349,7 +2350,7 @@
         <v>48</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2357,575 +2358,575 @@
         <v>49</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
started adding option for BattlePrep
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59E4B312-190E-4B54-BE25-2F5982EC4A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{37891AA5-A9B8-4B7F-8BD3-63D688B01F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -160,14 +160,6 @@
     <t>e017</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e017 Preparations Final&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-US Control markers are placed on sectors 1, 2, and 3. The Weather is displayed on top left of Battle Board.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue017' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>e018</t>
   </si>
   <si>
@@ -1461,17 +1453,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine your tank&amp;apos;s deployment from the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll = 
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e038 Orders Phase&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
@@ -1626,6 +1607,27 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;Bold&gt;-- AP:&lt;/Bold&gt; Unlimited&lt;LineBreak/&gt;
 &lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoPreparation' IsEnabled='False' Content='Use Setup of Previous Battle Prep' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine your tank&amp;apos;s deployment from the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll = 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e017 Preparations Final&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoPreparation' IsEnabled='False' Content='Use Setup of Previous Battle Prep' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+US Control markers are placed on sectors 1, 2, and 3. The Weather is displayed on top left of Battle Board.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue017' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1991,8 +1993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,7 +2008,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2014,7 +2016,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2022,7 +2024,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2030,7 +2032,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2038,7 +2040,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2046,7 +2048,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2054,79 +2056,79 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2134,15 +2136,15 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2150,7 +2152,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -2158,23 +2160,23 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2190,15 +2192,15 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2206,7 +2208,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2225,708 +2227,708 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>30</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added short cut for skipping battle prep
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{37891AA5-A9B8-4B7F-8BD3-63D688B01F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{79AB1972-8EB2-422B-8B89-95976FEF4F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -160,6 +160,14 @@
     <t>e017</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;e017 Preparations Final&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+US Control markers are placed on sectors 1, 2, and 3. The Weather is displayed on top left of Battle Board.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue017' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
     <t>e018</t>
   </si>
   <si>
@@ -1610,8 +1618,8 @@
   </si>
   <si>
     <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoPreparation' IsEnabled='False' Content='Use Setup of Previous Battle Prep' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoPreparation' Visibility='Hidden' Content='Use Setup of Previous Battle Prep' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Determine your tank&amp;apos;s deployment from the 
 &lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
@@ -1619,15 +1627,6 @@
 Die Roll = 
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e017 Preparations Final&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoPreparation' IsEnabled='False' Content='Use Setup of Previous Battle Prep' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-US Control markers are placed on sectors 1, 2, and 3. The Weather is displayed on top left of Battle Board.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue017' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1993,8 +1992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2008,7 +2007,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2016,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2024,7 +2023,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2032,7 +2031,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2040,7 +2039,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2048,7 +2047,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2056,79 +2055,79 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2136,15 +2135,15 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2152,7 +2151,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -2160,7 +2159,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -2168,15 +2167,15 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2192,15 +2191,15 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2208,7 +2207,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2227,708 +2226,708 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>241</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
work on Game Feats
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\happysulla\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79AB1972-8EB2-422B-8B89-95976FEF4F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D37459-D6A6-4029-A8C5-A698EFC15A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -1992,8 +1992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added more GameFeat and End Game details
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79AB1972-8EB2-422B-8B89-95976FEF4F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD97283-7154-490B-B780-C22E21D82CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -78,17 +78,6 @@
 &lt;LineBreak/&gt;   &lt;InlineUIContainer&gt;&lt;Image Name='DoorClosing'  Height='150' Width='75'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e503 End Game Statistics and Feats &lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Select 'File | New' menu option to play again.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click image to review map: 
-&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='Win' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click image to exit game:
-&lt;LineBreak/&gt;   &lt;InlineUIContainer&gt;&lt;Image Name='DoorClosing' Height='150' Width='75'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>e002</t>
   </si>
   <si>
@@ -1627,6 +1616,14 @@
 Die Roll = 
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e503 End Game Statistics and Feats &lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Select 'File | New' menu option to play again.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to exit game:
+&lt;LineBreak/&gt;   &lt;InlineUIContainer&gt;&lt;Image Name='DoorClosing' Height='150' Width='75'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1992,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2007,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2015,919 +2012,919 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2946,12 +2943,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>11</v>
+        <v>241</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add Initial Screen for setting up One Day Battle
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD97283-7154-490B-B780-C22E21D82CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B61F0CEB-46F3-4289-AB2D-EBC2B5F0B49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -1524,19 +1524,6 @@
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue005' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e000 Welcome to Patton's Best Solo Tank Battle Game&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial0' IsEnabled='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The game starts with a tutorial how to play. However, before starting, it is important to know that Active events are shown with a green background. The game may only advance when a green background is displayed. Most often, the game advances by rolling dice or clicking an image. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You can explore what may happen by showing inactive events. Inactive events have a gray background. To return to the current active event, select the active event button in the status bar per the image.
-&lt;LineBreak/&gt;
-               &lt;InlineUIContainer&gt;&lt;Image Name='Tutorial0' Height='70'  Width='370'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Name='Read_Rules' Content='Read Rules' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt; or 
-&lt;InlineUIContainer&gt;&lt;Button Name='Begin' Content='Begin Game' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e001 Fourth Armor Division Campaign&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r1.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial1' IsEnabled='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1624,6 +1611,25 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Click image to exit game:
 &lt;LineBreak/&gt;   &lt;InlineUIContainer&gt;&lt;Image Name='DoorClosing' Height='150' Width='75'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e000 Welcome to Patton's Best Solo Tank Battle Game&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial0' IsEnabled='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The game starts with a tutorial how to play. However, before starting, it is important to know that Active events are shown with a green background. The game may only advance when a green background is displayed. Most often, the game advances by rolling dice or clicking an image. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You can explore what may happen by showing inactive events. Inactive events have a gray background. To return to the current active event, select the active event button in the status bar per the image.
+&lt;LineBreak/&gt;
+               &lt;InlineUIContainer&gt;&lt;Image Name='Tutorial0' Height='70'  Width='370'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;
+Choose a button to begin:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Name='Read_Rules' Content='   Read Rules  ' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ - Can skip as rules are presented as needed &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Name='BeginCampaign' Content=' Begin Campaign' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ - Campaign from 07/44 to 04/45 &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Name='BeginSingleDay' Content=' Begin One Day ' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ - Choose tank and day of operations&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1989,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,12 +2005,12 @@
     <col min="2" max="2" width="175.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2012,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2020,7 +2026,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2028,7 +2034,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2036,7 +2042,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2148,7 +2154,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -2164,7 +2170,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2308,7 +2314,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2948,7 +2954,7 @@
         <v>6</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Got single day working
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B61F0CEB-46F3-4289-AB2D-EBC2B5F0B49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4D45D20-4C50-447D-8A5B-1F7DC593B40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
   <si>
     <t>e001</t>
   </si>
@@ -1630,6 +1630,19 @@
  - Campaign from 07/44 to 04/45 &lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Name='BeginSingleDay' Content=' Begin One Day ' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;
  - Choose tank and day of operations&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e005a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e005a Single Day of Battle&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You elected to only fight one day of battle. The game is won or lost based on victory points at end of day per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r6.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click buttons to get day and tank you want. The tank choice is limited by date shown on 
+&lt;InlineUIContainer&gt;&lt;Button Content='Replacement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Click image when ready to begin.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1993,10 +2006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2053,923 +2066,931 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>183</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>188</v>
+        <v>133</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+    <row r="110" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+    <row r="115" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+    <row r="116" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+    <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B117" s="2" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+    <row r="120" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+    <row r="121" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B121" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+    <row r="122" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on game ending and game stats
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32772E51-3660-48D4-950D-BACDA893C635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A39A8A4E-117D-4A86-B66C-F5A0234F9DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -986,20 +986,6 @@
     <t>e054b</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e054b MG Firing - Advancing Fire&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Advancing fire attacks infantry targets that move into the zone. It also help protect against Panzerfaust attacks. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 2D for ammo expected:&lt;LineBreak/&gt;
-01 - 30 = 1 box expended&lt;LineBreak/&gt;
-31 - 97 = no effect&lt;LineBreak/&gt;
-98 - 100 = MG malfunctions
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll = &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>e055</t>
   </si>
   <si>
@@ -1634,6 +1620,19 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Replacement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.  Hint: Click the date's minus sign button to rollover and show all possible tanks. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Click image when ready to begin.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e054b MG Firing - Advancing Fire&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Advancing fire attacks infantry targets that move into the zone. It also help protect against Panzerfaust attacks. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 2D for ammo expected:&lt;LineBreak/&gt;
+01 - 30 = 1 box expended&lt;LineBreak/&gt;
+31 - 97 = no effect&lt;LineBreak/&gt;
+98 - 100 = MG malfunctions
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -2000,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2015,7 +2014,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2023,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2031,7 +2030,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2039,7 +2038,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2047,7 +2046,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2055,15 +2054,15 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2071,79 +2070,79 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2151,12 +2150,12 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>57</v>
@@ -2167,7 +2166,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -2175,7 +2174,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -2183,15 +2182,15 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2207,7 +2206,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2223,7 +2222,7 @@
         <v>20</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2327,7 +2326,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2348,10 +2347,10 @@
     </row>
     <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2380,10 +2379,10 @@
     </row>
     <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2420,10 +2419,10 @@
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2431,7 +2430,7 @@
         <v>66</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2439,7 +2438,7 @@
         <v>67</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -2567,7 +2566,7 @@
         <v>73</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2679,7 +2678,7 @@
         <v>108</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2687,7 +2686,7 @@
         <v>125</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2703,7 +2702,7 @@
         <v>119</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2762,76 +2761,76 @@
         <v>132</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>159</v>
+        <v>241</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2844,58 +2843,58 @@
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2908,10 +2907,10 @@
     </row>
     <row r="113" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2967,7 +2966,7 @@
         <v>6</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
minor changes to statusbar
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\happysulla\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE65C156-CE78-4C84-84A9-BE54279DF2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0DC84D-EF0F-4017-B5FE-BE06C6EA24BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -1613,9 +1613,21 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;e101 Evening Debriefing - Victory Point Total&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.92' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+updated to reflect victory points for both your tank and friendly forces. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e054b MG Firing - Advancing Fire&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
+&lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoRollBowMgFire' IsEnabled='True' Content='Autoroll Bow MG Fire in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Advancing fire attacks infantry targets that move into the zone. It also help protect against Panzerfaust attacks. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1623,16 +1635,6 @@
 01 - 30 = 1 box expended&lt;LineBreak/&gt;
 31 - 97 = no effect&lt;LineBreak/&gt;
 98 - 100 = MG malfunctions
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e101 Evening Debriefing - Victory Point Total&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.92' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-updated to reflect victory points for both your tank and friendly forces. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -1999,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2761,12 +2763,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2918,7 +2920,7 @@
         <v>97</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="165" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
checkpointing - working our hourly check for weather
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0DC84D-EF0F-4017-B5FE-BE06C6EA24BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920A0358-EA60-4B38-B1E5-1C14F1F98606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
   <si>
     <t>e001</t>
   </si>
@@ -1635,6 +1635,14 @@
 01 - 30 = 1 box expended&lt;LineBreak/&gt;
 31 - 97 = no effect&lt;LineBreak/&gt;
 98 - 100 = MG malfunctions
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e022a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e022a Rain Roll&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -1999,10 +2007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2291,691 +2299,699 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+    <row r="104" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B104" s="2" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>184</v>
+        <v>130</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B107" s="2" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+    <row r="111" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+    <row r="116" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+    <row r="117" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B117" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+    <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+    <row r="121" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B121" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+    <row r="122" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rain and snow checks
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\happysulla\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920A0358-EA60-4B38-B1E5-1C14F1F98606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C85A915B-FAAC-4E9D-B111-20CAC8E64947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -2009,7 +2009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Solved issue with time. Added gun repair attempt between battles.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\happysulla\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C85A915B-FAAC-4E9D-B111-20CAC8E64947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A5E8241-6B96-4CA1-86B7-DBB8280ABC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="252">
   <si>
     <t>e001</t>
   </si>
@@ -1641,8 +1641,48 @@
     <t>e022a</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e022a Rain Roll&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;e022a Rain Roll&lt;/Bold&gt;    
 &lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e056d</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;056d Repair Main Gun - End of Battle Repair Attempt&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Any result other than broken repairs the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e056e</t>
+  </si>
+  <si>
+    <t>e056f</t>
+  </si>
+  <si>
+    <t>e056g</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;056f Repair Coaxial MG - End of Battle Repair Attempt&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Any result other than broken repairs the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;056e Repair AA MG - End of Battle Repair Attempt&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Any result other than broken repairs the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;056g Repair Bow MG - End of Battle Repair Attempt&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Any result other than broken repairs the gun.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
@@ -2007,10 +2047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B122"/>
+  <dimension ref="A1:B126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2827,171 +2867,203 @@
         <v>168</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>171</v>
+        <v>244</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>172</v>
+        <v>246</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>175</v>
+        <v>247</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>177</v>
+        <v>249</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+    <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+    <row r="111" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+    <row r="112" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+    <row r="113" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+    <row r="114" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>97</v>
+        <v>224</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>98</v>
+        <v>226</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+    <row r="123" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B123" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+    <row r="124" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B124" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+    <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B125" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+    <row r="126" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B126" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates to game state
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1BAA77B-F4C7-40AA-B09E-C769A25B377C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AC3819C-FD84-4730-8C9A-45F71C9DC9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -2019,8 +2019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
readded back stuff lost in merge
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AC3819C-FD84-4730-8C9A-45F71C9DC9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{592D42EA-8B84-4E05-ABAE-8BE4CDCF62E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -1387,13 +1387,6 @@
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e011a Deployment - Counterattack Scenario&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since this is a Counterattack scenario, your tank&amp;apos;s deployment is automatically stopped and hull down.  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e038 Orders Phase&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
 &lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
@@ -1537,18 +1530,6 @@
 &lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoPreparation' Visibility='Hidden' Content='Use Setup of Previous Battle Prep' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine your tank&amp;apos;s deployment from the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll = 
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e000 Welcome to Patton's Best Solo Tank Battle Game&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial0' IsEnabled='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1654,6 +1635,28 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='Bogged Down' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
+&lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoPreparation' Visibility='Hidden' Content='Use Setup of Previous Battle Prep' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine your tank&amp;apos;s deployment from the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll = 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e011a Deployment - Counterattack Scenario&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoPreparation' Visibility='Hidden' Content='Use Setup of Previous Battle Prep' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since this is a Counterattack scenario, your tank&amp;apos;s deployment is automatically stopped and hull down.  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2019,8 +2022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,7 +2037,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2042,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2050,7 +2053,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2058,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2066,7 +2069,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2074,15 +2077,15 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2159,10 +2162,10 @@
     </row>
     <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2186,7 +2189,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -2197,20 +2200,20 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>210</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>216</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2311,18 +2314,18 @@
     </row>
     <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2362,7 +2365,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2474,7 +2477,7 @@
         <v>67</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -2706,7 +2709,7 @@
         <v>139</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2738,7 +2741,7 @@
         <v>118</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2802,7 +2805,7 @@
         <v>156</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2911,26 +2914,26 @@
     </row>
     <row r="111" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2954,7 +2957,7 @@
         <v>97</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -3002,7 +3005,7 @@
         <v>6</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lots of fixes mostly about weather, battle repairs,
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{592D42EA-8B84-4E05-ABAE-8BE4CDCF62E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{10278AE0-429A-4F33-AD16-6BEB28C5EAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="254">
   <si>
     <t>e001</t>
   </si>
@@ -1024,16 +1025,6 @@
     <t>e100a</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e100a Tank Retires for Today&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Due to broken gun or broken gun sight, the tank must be retired for today. &lt;LineBreak/&gt;
-An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-Click image to continue to continue to Crew Rating Improvements per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                  &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>e057</t>
   </si>
   <si>
@@ -1657,6 +1648,57 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Since this is a Counterattack scenario, your tank&amp;apos;s deployment is automatically stopped and hull down.  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e056d</t>
+  </si>
+  <si>
+    <t>e056e</t>
+  </si>
+  <si>
+    <t>e056f</t>
+  </si>
+  <si>
+    <t>e056g</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e056g Repair Bow Machine Gun - Between Battles&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Anything other than break repairs the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e056f Repair Coaxial Machine Gun - Between Battles&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Anything other than break repairs the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e056e Repair AA Machine Gun - Between Battles&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Anything other than break repairs the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;056d Repair Main Gun - Between Battles&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Anything other than break repairs the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e100a Tank Retires for Today&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Due to broken gun or broken gun sight, the tank must be retired for today. &lt;LineBreak/&gt;
+An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to continue to continue to Crew Rating Improvements per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                  &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -2020,10 +2062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B123"/>
+  <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2037,7 +2079,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2045,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2053,7 +2095,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2061,7 +2103,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2069,7 +2111,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2077,15 +2119,15 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2093,79 +2135,79 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2173,12 +2215,12 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>57</v>
@@ -2189,7 +2231,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -2197,7 +2239,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2205,15 +2247,15 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2229,7 +2271,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2245,7 +2287,7 @@
         <v>20</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2314,18 +2356,18 @@
     </row>
     <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2365,7 +2407,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2386,10 +2428,10 @@
     </row>
     <row r="45" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2418,10 +2460,10 @@
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2458,10 +2500,10 @@
     </row>
     <row r="54" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2469,7 +2511,7 @@
         <v>66</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2477,7 +2519,7 @@
         <v>67</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -2605,7 +2647,7 @@
         <v>73</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2709,7 +2751,7 @@
         <v>139</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2717,7 +2759,7 @@
         <v>107</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2725,7 +2767,7 @@
         <v>124</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2741,7 +2783,7 @@
         <v>118</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2805,7 +2847,7 @@
         <v>156</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2848,171 +2890,203 @@
         <v>166</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>169</v>
+        <v>245</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>170</v>
+        <v>246</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>173</v>
+        <v>247</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>175</v>
+        <v>250</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+    <row r="111" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B107" s="2" t="s">
+    </row>
+    <row r="112" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="B112" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B108" s="2" t="s">
+    </row>
+    <row r="113" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="B113" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+    <row r="115" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+      <c r="B120" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B121" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+    <row r="122" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+    <row r="123" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B123" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+    <row r="124" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B124" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+    <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B125" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+    <row r="126" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B122" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+      <c r="B126" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B127" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed MG not working due to invalid state when advance fire. Fixed choosing loader or commander spot when spotting
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B1FC7706-0769-4322-8127-381A02606623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0106B79D-49D1-4E39-9BD8-9FE052FE55D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1552,18 +1551,6 @@
      &lt;InlineUIContainer&gt;&lt;Image Name='DoorClosing' Height='150' Width='75'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e005a Single Day of Battle&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You elected to only fight one day of battle. The game is won or lost based on victory points at end of day per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r6.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click buttons to get day and tank you want. The tank choice is limited by date shown on 
-&lt;InlineUIContainer&gt;&lt;Button Content='Replacement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.  Hint: Click the date's minus sign button to rollover and show all possible tanks. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click image when ready to begin.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e101 Evening Debriefing - Victory Point Total&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.92' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -1699,6 +1686,16 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                   &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e005a Single Day of Battle&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You elected to only fight one day of battle. The game is won or lost based on victory points at end of day per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r6.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click buttons to get day and tank you want. The tank choice is limited by date shown on 
+&lt;InlineUIContainer&gt;&lt;Button Content='Replacement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.  Hint: Click the date's minus sign button to rollover and show all possible tanks. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2064,8 +2061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,12 +2119,12 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>232</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2247,7 +2244,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2255,7 +2252,7 @@
         <v>209</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2356,18 +2353,18 @@
     </row>
     <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2751,7 +2748,7 @@
         <v>139</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2783,7 +2780,7 @@
         <v>118</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2847,7 +2844,7 @@
         <v>156</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2892,34 +2889,34 @@
     </row>
     <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3023,7 +3020,7 @@
         <v>167</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3031,7 +3028,7 @@
         <v>97</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="165" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added new win images
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0106B79D-49D1-4E39-9BD8-9FE052FE55D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C62AB3F-79DC-4DE3-B781-B9A1D0F5EFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -2061,8 +2061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Attempting to fix that when button is added for switching, do not allow any other options to happen
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\happysulla\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C62AB3F-79DC-4DE3-B781-B9A1D0F5EFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D1D8039-30F4-4085-9235-8B70F43B880F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="256">
   <si>
     <t>e001</t>
   </si>
@@ -872,25 +872,10 @@
     <t>e050a</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e050a No Gun Round Loaded&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since the gun is unloaded at the start of the round, choose one of the highlighted boxes to load the gun.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>e050b</t>
   </si>
   <si>
     <t>e050c</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050b Out of Main Gun Rounds&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Main Gun is empty, and there are no rounds to load. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50b' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e050c No Gun Rounds to Load&lt;/Bold&gt; 
@@ -902,14 +887,6 @@
   </si>
   <si>
     <t>e050d</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e050c No Gun Rounds to Load&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The tank is empty of all main gun rounds. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50d' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>e053f</t>
@@ -1520,6 +1497,191 @@
 &lt;Bold&gt;-- HE:&lt;/Bold&gt; Unlimited</t>
   </si>
   <si>
+    <t>e005a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e503 End Game Statistics and Feats &lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Select 'File | New' menu option to play again.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to exit game:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='DoorClosing' Height='150' Width='75'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e101 Evening Debriefing - Victory Point Total&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.92' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+updated to reflect victory points for both your tank and friendly forces. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e054b MG Firing - Advancing Fire&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
+&lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoRollBowMgFire' IsEnabled='True' Content='Autoroll Bow MG Fire in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Advancing fire attacks infantry targets that move into the zone. It also help protect against Panzerfaust attacks. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 2D for ammo expected:&lt;LineBreak/&gt;
+01 - 30 = 1 box expended&lt;LineBreak/&gt;
+31 - 97 = no effect&lt;LineBreak/&gt;
+98 - 100 = MG malfunctions
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e022a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e022a Rain Roll&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e022b</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e022b Falling Snow Roll&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e053a Main Gun Firing - No Target Available&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+There is no target that is selectable. Only enemy units that have been spotted may be selected.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The main gun may only fire at a target in the turret&amp;apos;s front sector. 
+Since that is not possible, the gun fires at no target. Need to roll for malfunctioning gun (98, 99, or 100). Note: Spotting and Combat only allowed at close range for rain or falling snow per 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll: &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e051a Bogged Down&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A bogged down tank may not move or pivot until it has freed itself by using reverse movement on the
+ &lt;InlineUIContainer&gt;&lt;Button Content='Bogged Down' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
+&lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoPreparation' Visibility='Hidden' Content='Use Setup of Previous Battle Prep' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine your tank&amp;apos;s deployment from the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Die Roll = 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e011a Deployment - Counterattack Scenario&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoPreparation' Visibility='Hidden' Content='Use Setup of Previous Battle Prep' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since this is a Counterattack scenario, your tank&amp;apos;s deployment is automatically stopped and hull down.  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e056d</t>
+  </si>
+  <si>
+    <t>e056e</t>
+  </si>
+  <si>
+    <t>e056f</t>
+  </si>
+  <si>
+    <t>e056g</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e056g Repair Bow Machine Gun - Between Battles&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Anything other than break repairs the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e056f Repair Coaxial Machine Gun - Between Battles&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Anything other than break repairs the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e056e Repair AA Machine Gun - Between Battles&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Anything other than break repairs the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;056d Repair Main Gun - Between Battles&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Anything other than break repairs the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e005a Single Day of Battle&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You elected to only fight one day of battle. The game is won or lost based on victory points at end of day per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r6.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click buttons to get day and tank you want. The tank choice is limited by date shown on 
+&lt;InlineUIContainer&gt;&lt;Button Content='Replacement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.  Hint: Click the date's minus sign button to rollover and show all possible tanks. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e100a Tank Retires for Today&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Due to broken gun or broken gun sight, the tank must be retired for today. An evening debriefing is performed per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to continue to continue to Crew Rating Improvements per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                  &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e050e</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050d No Gun Rounds to Load&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The tank is empty of all main gun rounds. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50d' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050b End of Round - Out of Main Gun Rounds&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Main Gun is empty, and there are no rounds to load. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50b' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050a End of Round - No Gun Round Loaded&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since the gun is unloaded at the start of the round, choose one of the highlighted boxes to load the gun.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e000 Welcome to Patton's Best Solo Tank Battle Game&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='SkipTutorial0' IsEnabled='True' Content='Skip in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1531,171 +1693,20 @@
 &lt;LineBreak/&gt;
 Choose a button to begin:
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Name='Read_Rules' Content='   Read Rules  ' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;InlineUIContainer&gt;&lt;Button Name='Read_Rules' Content='   Read Rules   ' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;
  - Can skip as rules are presented as needed &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Name='BeginCampaign' Content=' Begin Campaign' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;InlineUIContainer&gt;&lt;Button Name='BeginCampaign' Content=' Begin Campaign ' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;
  - Campaign from 07/44 to 04/45 &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Name='BeginSingleDay' Content=' Begin One Day ' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;InlineUIContainer&gt;&lt;Button Name='BeginSingleDay' Content=' Begin One Day  ' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;
  - Choose tank and day of operations&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>e005a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e503 End Game Statistics and Feats &lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Select 'File | New' menu option to play again.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click image to exit game:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-     &lt;InlineUIContainer&gt;&lt;Image Name='DoorClosing' Height='150' Width='75'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e101 Evening Debriefing - Victory Point Total&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.92' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-updated to reflect victory points for both your tank and friendly forces. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e054b MG Firing - Advancing Fire&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
-&lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoRollBowMgFire' IsEnabled='True' Content='Autoroll Bow MG Fire in Future' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Advancing fire attacks infantry targets that move into the zone. It also help protect against Panzerfaust attacks. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 2D for ammo expected:&lt;LineBreak/&gt;
-01 - 30 = 1 box expended&lt;LineBreak/&gt;
-31 - 97 = no effect&lt;LineBreak/&gt;
-98 - 100 = MG malfunctions
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e022a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e022a Rain Roll&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e022b</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e022b Falling Snow Roll&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;    
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e053a Main Gun Firing - No Target Available&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-There is no target that is selectable. Only enemy units that have been spotted may be selected.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The main gun may only fire at a target in the turret&amp;apos;s front sector. 
-Since that is not possible, the gun fires at no target. Need to roll for malfunctioning gun (98, 99, or 100). Note: Spotting and Combat only allowed at close range for rain or falling snow per 
-&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll: &lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e051a Bogged Down&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r11.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-A bogged down tank may not move or pivot until it has freed itself by using reverse movement on the
- &lt;InlineUIContainer&gt;&lt;Button Content='Bogged Down' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;Underline&gt;Modifiers:&lt;/Underline&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e011 Deployment&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
-&lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoPreparation' Visibility='Hidden' Content='Use Setup of Previous Battle Prep' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine your tank&amp;apos;s deployment from the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Deployment' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Die Roll = 
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollBlue' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e011a Deployment - Counterattack Scenario&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoPreparation' Visibility='Hidden' Content='Use Setup of Previous Battle Prep' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since this is a Counterattack scenario, your tank&amp;apos;s deployment is automatically stopped and hull down.  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e056d</t>
-  </si>
-  <si>
-    <t>e056e</t>
-  </si>
-  <si>
-    <t>e056f</t>
-  </si>
-  <si>
-    <t>e056g</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e056g Repair Bow Machine Gun - Between Battles&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Anything other than break repairs the gun.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e056f Repair Coaxial Machine Gun - Between Battles&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Anything other than break repairs the gun.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e056e Repair AA Machine Gun - Between Battles&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Anything other than break repairs the gun.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;056d Repair Main Gun - Between Battles&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Attempt to repair malfunction gun by rolling on the &lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Anything other than break repairs the gun.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e100a Tank Retires for Today&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Due to broken gun or broken gun sight, the tank must be retired for today. &lt;LineBreak/&gt;
-An evening debriefing is performed per &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click image to continue to continue to Crew Rating Improvements per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.91' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                  &lt;InlineUIContainer&gt;&lt;Image Name='Debrief' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e005a Single Day of Battle&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You elected to only fight one day of battle. The game is won or lost based on victory points at end of day per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r6.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click buttons to get day and tank you want. The tank choice is limited by date shown on 
-&lt;InlineUIContainer&gt;&lt;Button Content='Replacement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.  Hint: Click the date's minus sign button to rollover and show all possible tanks. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+    <t>&lt;Bold&gt;e050c End of Round - No Load Action Taken&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The loader did not perform a Load action this turn. Therefore, unable to load gun with new ammo. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                            &lt;InlineUIContainer&gt;&lt;Image Name='Continue50f' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -2059,203 +2070,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B127"/>
+  <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="175.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.15625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="175.26171875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="259.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B14" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
@@ -2263,31 +2274,31 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
@@ -2295,7 +2306,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2303,7 +2314,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -2311,7 +2322,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -2319,7 +2330,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -2327,7 +2338,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -2335,7 +2346,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -2343,7 +2354,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -2351,23 +2362,23 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
@@ -2375,7 +2386,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -2383,7 +2394,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -2391,7 +2402,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
@@ -2399,15 +2410,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
@@ -2415,7 +2426,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
@@ -2423,15 +2434,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -2439,7 +2450,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -2447,7 +2458,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -2455,15 +2466,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -2471,7 +2482,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
@@ -2479,7 +2490,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -2487,7 +2498,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
@@ -2495,31 +2506,31 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="259.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
         <v>132</v>
       </c>
@@ -2527,7 +2538,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="259.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
         <v>133</v>
       </c>
@@ -2535,7 +2546,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="259.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
         <v>137</v>
       </c>
@@ -2543,7 +2554,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
         <v>68</v>
       </c>
@@ -2551,7 +2562,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
         <v>69</v>
       </c>
@@ -2559,7 +2570,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
         <v>70</v>
       </c>
@@ -2567,7 +2578,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
         <v>71</v>
       </c>
@@ -2575,7 +2586,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
         <v>78</v>
       </c>
@@ -2583,7 +2594,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
         <v>83</v>
       </c>
@@ -2591,7 +2602,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
         <v>84</v>
       </c>
@@ -2599,7 +2610,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
         <v>85</v>
       </c>
@@ -2607,7 +2618,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
@@ -2615,7 +2626,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
         <v>89</v>
       </c>
@@ -2623,7 +2634,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
         <v>90</v>
       </c>
@@ -2631,7 +2642,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
         <v>91</v>
       </c>
@@ -2639,15 +2650,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
         <v>74</v>
       </c>
@@ -2655,7 +2666,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
         <v>80</v>
       </c>
@@ -2663,7 +2674,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
         <v>75</v>
       </c>
@@ -2671,7 +2682,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
         <v>76</v>
       </c>
@@ -2679,7 +2690,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
         <v>81</v>
       </c>
@@ -2687,7 +2698,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
@@ -2695,395 +2706,403 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="B81" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="B83" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B82" s="2" t="s">
+    </row>
+    <row r="84" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B83" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B85" s="2" t="s">
+    <row r="96" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B93" s="2" t="s">
+      <c r="B105" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B101" s="2" t="s">
+    <row r="112" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B105" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+    <row r="121" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+      <c r="B121" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+    <row r="123" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B123" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+    <row r="124" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B124" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+    <row r="125" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B125" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
+    <row r="126" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B126" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+    <row r="127" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B126" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+      <c r="B127" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B128" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tweaks to dialog displays and which ones show up on top
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\happysulla\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5185B969-E699-4A6E-8A7D-96750D6061B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7CFA53-BE18-4C1A-98BC-AE58FB044F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -2072,8 +2072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Started working on Ammo Reload shortcut
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1F0917-F74B-4208-87B1-B6EC721081F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11F9E0AD-12DA-4099-AEBD-1783D55A3846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -907,21 +907,6 @@
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue53f' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Right click marker or one of blue boxes to show the ammo reload context menu.  Alternatively, or if no blue box is shown, right click on the Gun Load marker to show the context menu.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The context menu allows setting the Ammo Reload marker. When no ammo can be reloaded, this marker disappears.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The selection of Ready Rack Ammo Reload marker over the Ammo Reload marker supports higher chance of performing rate of fire. &lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The Gun Load marker shows the round in the main gun. The Gun Load marker changes to the Ammo Reload location when the gun is fired. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e060 Reset Round&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1707,6 +1692,22 @@
 The loader did not perform a Load action this turn. Therefore, unable to load gun with new ammo. Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue50f' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e050 Ammo Reload Order&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;CheckBox Name='AutoSetAmmoLoad' IsEnabled='True' Content='Automatically assign reload to gunload box' FontFamily='Courier New'  FontSize='12'&gt;&lt;/CheckBox&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Right click marker or one of blue boxes to show the ammo reload context menu.  Alternatively, or if no blue box is shown, right click on the Gun Load marker to show the context menu.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The context menu allows setting the Ammo Reload marker. When no ammo can be reloaded, this marker disappears.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The selection of Ready Rack Ammo Reload marker over the Ammo Reload marker supports higher chance of performing rate of fire. &lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Gun Load marker shows the round in the main gun. The Gun Load marker changes to the Ammo Reload location when the gun is fired. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2072,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2087,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -2095,7 +2096,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2103,7 +2104,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2111,7 +2112,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2119,7 +2120,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -2127,15 +2128,15 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -2143,79 +2144,79 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -2223,12 +2224,12 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>57</v>
@@ -2239,7 +2240,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -2247,7 +2248,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -2255,15 +2256,15 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2279,15 +2280,15 @@
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2295,7 +2296,7 @@
         <v>20</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -2364,18 +2365,18 @@
     </row>
     <row r="36" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -2415,7 +2416,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -2436,10 +2437,10 @@
     </row>
     <row r="45" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -2468,10 +2469,10 @@
     </row>
     <row r="49" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -2508,10 +2509,10 @@
     </row>
     <row r="54" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2519,7 +2520,7 @@
         <v>66</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2527,7 +2528,7 @@
         <v>67</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
@@ -2655,7 +2656,7 @@
         <v>73</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -2706,12 +2707,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>149</v>
+        <v>255</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -2719,7 +2720,7 @@
         <v>141</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -2727,7 +2728,7 @@
         <v>142</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -2735,7 +2736,7 @@
         <v>143</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -2748,10 +2749,10 @@
     </row>
     <row r="84" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2767,7 +2768,7 @@
         <v>139</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -2775,7 +2776,7 @@
         <v>107</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -2783,7 +2784,7 @@
         <v>124</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -2799,7 +2800,7 @@
         <v>118</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -2860,106 +2861,106 @@
     </row>
     <row r="98" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -2967,63 +2968,63 @@
         <v>130</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -3036,10 +3037,10 @@
     </row>
     <row r="120" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -3047,7 +3048,7 @@
         <v>97</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -3095,7 +3096,7 @@
         <v>6</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added difference between offboard and onboard artillery
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11F9E0AD-12DA-4099-AEBD-1783D55A3846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{103E73F6-6CBA-468E-B5A9-D15B313169C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -628,27 +628,6 @@
                                    &lt;InlineUIContainer&gt;&lt;Image Name='MilitaryWatch' Height='100' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e041 Friendly Artillery&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Friendly artillery support arrives. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                        &lt;InlineUIContainer&gt;&lt;Image Name='c39ArtillerySupport'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e042 Enemy Artillery&lt;/Bold&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Enemy artillery arrives. Roll 1D to knock out (KO) friendly units: 
-&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-1 KO for 1-6&lt;LineBreak/&gt;
-2 KO for 7-9&lt;LineBreak/&gt;
-3 KO for 10
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e046 Friendly Advance&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r15.7' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1708,6 +1687,27 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The Gun Load marker shows the round in the main gun. The Gun Load marker changes to the Ammo Reload location when the gun is fired. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e042 Enemy Artillery&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy artillery arrives. Roll 1D to knock out (KO) friendly units: 
+&lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1 KO for 1-6&lt;LineBreak/&gt;
+2 KO for 7-9&lt;LineBreak/&gt;
+3 KO for 10
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e041 Off-Board Friendly Artillery&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Offboard Friendly artillery support arrives. O.B. artillery is not affected by smoke, fog/snow, friendly losses, or controlled sectors. It adds affect LW/MG/ATG in woods. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='c39ArtillerySupport'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -2073,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="B60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2088,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -2096,7 +2096,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2104,7 +2104,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2112,7 +2112,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2120,7 +2120,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -2128,15 +2128,15 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -2144,79 +2144,79 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -2224,12 +2224,12 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>57</v>
@@ -2240,7 +2240,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -2248,7 +2248,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -2256,15 +2256,15 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2280,15 +2280,15 @@
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2296,7 +2296,7 @@
         <v>20</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -2365,18 +2365,18 @@
     </row>
     <row r="36" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -2416,7 +2416,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -2437,10 +2437,10 @@
     </row>
     <row r="45" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -2469,10 +2469,10 @@
     </row>
     <row r="49" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -2504,15 +2504,15 @@
         <v>58</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2520,7 +2520,7 @@
         <v>66</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2528,31 +2528,31 @@
         <v>67</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -2568,7 +2568,7 @@
         <v>69</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>110</v>
+        <v>255</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -2576,7 +2576,7 @@
         <v>70</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>111</v>
+        <v>254</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -2656,7 +2656,7 @@
         <v>73</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -2664,7 +2664,7 @@
         <v>74</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -2672,7 +2672,7 @@
         <v>80</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -2680,7 +2680,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -2688,7 +2688,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -2696,7 +2696,7 @@
         <v>81</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -2704,7 +2704,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -2712,47 +2712,47 @@
         <v>65</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2765,10 +2765,10 @@
     </row>
     <row r="86" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -2776,15 +2776,15 @@
         <v>107</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -2792,239 +2792,239 @@
         <v>108</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -3037,10 +3037,10 @@
     </row>
     <row r="120" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -3048,7 +3048,7 @@
         <v>97</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -3096,7 +3096,7 @@
         <v>6</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fix issue with Tank Replacement Roll in Aug
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDC004EC-1591-4EDE-9D02-04C4814865E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{43EC9000-4FD7-4347-87E6-A3E95A14FD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1188,15 +1187,6 @@
 Die Roll = &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e007b Crew Replacement&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When you tank is knocked out, wounded crewmen are replaced in morning briefing if combat may occur this day per 
-&lt;InlineUIContainer&gt;&lt;Button Content='e006' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue to assign new replacement crew.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance3' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;Bold&gt;e045 Harrassing Fire&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r15.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1706,6 +1696,15 @@
 Die Roll = 
 &lt;InlineUIContainer&gt;&lt;Image Name='DieRollWhite' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e007b Crew Replacement&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When you tank is knocked out, wounded crewmen are replaced in the first morning briefing that occurs as a result of a Combat Calender check
+&lt;InlineUIContainer&gt;&lt;Button Content='e006' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue to Combat Calender Check.  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                          &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance3' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -2071,8 +2070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2086,7 +2085,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2094,7 +2093,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2102,7 +2101,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2110,7 +2109,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2118,7 +2117,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2126,15 +2125,15 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2142,31 +2141,31 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2182,7 +2181,7 @@
         <v>184</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>193</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2211,10 +2210,10 @@
     </row>
     <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2222,7 +2221,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2238,7 +2237,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -2246,7 +2245,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2254,15 +2253,15 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2363,18 +2362,18 @@
     </row>
     <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2414,7 +2413,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2467,10 +2466,10 @@
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2507,10 +2506,10 @@
     </row>
     <row r="54" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2526,7 +2525,7 @@
         <v>67</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -2566,7 +2565,7 @@
         <v>69</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2574,7 +2573,7 @@
         <v>70</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2654,7 +2653,7 @@
         <v>73</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2710,7 +2709,7 @@
         <v>65</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2718,7 +2717,7 @@
         <v>139</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2726,7 +2725,7 @@
         <v>140</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2734,7 +2733,7 @@
         <v>141</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2747,10 +2746,10 @@
     </row>
     <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2766,7 +2765,7 @@
         <v>137</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2798,7 +2797,7 @@
         <v>116</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2862,7 +2861,7 @@
         <v>150</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2907,34 +2906,34 @@
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3003,26 +3002,26 @@
     </row>
     <row r="116" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -3038,7 +3037,7 @@
         <v>161</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3046,7 +3045,7 @@
         <v>97</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -3094,7 +3093,7 @@
         <v>6</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added campaign medals at end
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\happysulla\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43EC9000-4FD7-4347-87E6-A3E95A14FD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6867820-BBA9-421D-AAEB-1914B68E89C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -1440,15 +1440,6 @@
     <t>e005a</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e503 End Game Statistics and Feats &lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Select 'File | New' menu option to play again.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click image to exit game:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-     &lt;InlineUIContainer&gt;&lt;Image Name='DoorClosing' Height='150' Width='75'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e101 Evening Debriefing - Victory Point Total&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.92' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -1705,6 +1696,10 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='e006' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue to Combat Calender Check.  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                           &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance3' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e503 End Game Statistics and Feats &lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2070,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128:B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,7 +2080,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2133,7 +2128,7 @@
         <v>223</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2181,7 +2176,7 @@
         <v>184</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2245,7 +2240,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2253,7 +2248,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2261,7 +2256,7 @@
         <v>202</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2362,18 +2357,18 @@
     </row>
     <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2565,7 +2560,7 @@
         <v>69</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2573,7 +2568,7 @@
         <v>70</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2709,7 +2704,7 @@
         <v>65</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2717,7 +2712,7 @@
         <v>139</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2725,7 +2720,7 @@
         <v>140</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2733,7 +2728,7 @@
         <v>141</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2746,10 +2741,10 @@
     </row>
     <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2765,7 +2760,7 @@
         <v>137</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2797,7 +2792,7 @@
         <v>116</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2861,7 +2856,7 @@
         <v>150</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2906,34 +2901,34 @@
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3037,7 +3032,7 @@
         <v>161</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3045,7 +3040,7 @@
         <v>97</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -3088,12 +3083,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Return Events.xlsx back to intended
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43EC9000-4FD7-4347-87E6-A3E95A14FD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D85310C1-EF15-4853-9F7D-3042B913DB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -1440,15 +1440,6 @@
     <t>e005a</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e503 End Game Statistics and Feats &lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Select 'File | New' menu option to play again.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click image to exit game:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-     &lt;InlineUIContainer&gt;&lt;Image Name='DoorClosing' Height='150' Width='75'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e101 Evening Debriefing - Victory Point Total&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.92' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -1705,6 +1696,10 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='e006' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue to Combat Calender Check.  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                           &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance3' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e503 End Game Statistics and Feats &lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2070,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,7 +2080,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2133,7 +2128,7 @@
         <v>223</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2181,7 +2176,7 @@
         <v>184</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2245,7 +2240,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2253,7 +2248,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2261,7 +2256,7 @@
         <v>202</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2362,18 +2357,18 @@
     </row>
     <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2565,7 +2560,7 @@
         <v>69</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2573,7 +2568,7 @@
         <v>70</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2709,7 +2704,7 @@
         <v>65</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2717,7 +2712,7 @@
         <v>139</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2725,7 +2720,7 @@
         <v>140</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2733,7 +2728,7 @@
         <v>141</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2746,10 +2741,10 @@
     </row>
     <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2765,7 +2760,7 @@
         <v>137</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2797,7 +2792,7 @@
         <v>116</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2861,7 +2856,7 @@
         <v>150</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2906,34 +2901,34 @@
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3037,7 +3032,7 @@
         <v>161</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3045,7 +3040,7 @@
         <v>97</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -3088,12 +3083,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed switching crew members. Tested save and open with switched crew member.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D85310C1-EF15-4853-9F7D-3042B913DB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01200BA6-05B3-4410-8366-8D235D45B459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-22830" yWindow="2910" windowWidth="21600" windowHeight="11835" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -1084,14 +1084,6 @@
     <t>e061</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e061 Crew Switch&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The assistant driver moves through the tank to replace the incapacitated crewman. The assistant driver takes on the role but at half rating. Click image to  continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                                 &lt;InlineUIContainer&gt;&lt;Image Name='CarryingMan' Height='200' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>e061a</t>
   </si>
   <si>
@@ -1700,6 +1692,14 @@
   <si>
     <t>&lt;Bold&gt;e503 End Game Statistics and Feats &lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e061 Crew Switch&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The assistant driver moves through the tank to replace the incapacitated crewman. The assistant driver takes on the role but at half rating unless switching with Driver. Click image to  continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                                 &lt;InlineUIContainer&gt;&lt;Image Name='CarryingMan' Height='200' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -2065,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,7 +2080,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2096,7 +2096,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2104,7 +2104,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2112,7 +2112,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2120,15 +2120,15 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2136,79 +2136,79 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2216,12 +2216,12 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>57</v>
@@ -2232,7 +2232,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -2240,7 +2240,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2248,15 +2248,15 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2357,18 +2357,18 @@
     </row>
     <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2408,7 +2408,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2461,10 +2461,10 @@
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2501,10 +2501,10 @@
     </row>
     <row r="54" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2520,7 +2520,7 @@
         <v>67</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -2560,7 +2560,7 @@
         <v>69</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2568,7 +2568,7 @@
         <v>70</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2648,7 +2648,7 @@
         <v>73</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2704,7 +2704,7 @@
         <v>65</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2712,7 +2712,7 @@
         <v>139</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2720,7 +2720,7 @@
         <v>140</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2728,7 +2728,7 @@
         <v>141</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2741,10 +2741,10 @@
     </row>
     <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2760,7 +2760,7 @@
         <v>137</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2792,7 +2792,7 @@
         <v>116</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2856,7 +2856,7 @@
         <v>150</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2901,34 +2901,34 @@
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2968,55 +2968,55 @@
         <v>175</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>176</v>
+        <v>255</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -3032,7 +3032,7 @@
         <v>161</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3040,7 +3040,7 @@
         <v>97</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -3088,7 +3088,7 @@
         <v>6</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix problem with name set in AAR Dialog
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01200BA6-05B3-4410-8366-8D235D45B459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B930F5DE-59BD-4931-8162-FDDD3F5F9B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22830" yWindow="2910" windowWidth="21600" windowHeight="11835" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -584,19 +585,6 @@
 Click image to continue.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e102 Evening Debriefing - Promotions&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.93' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r25.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You are promoted when promotion points reach these values. However, cannot be promoted faster than once per month:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-100 = Staff Sergeant&lt;LineBreak/&gt;
-200 = 2nd Lieutenant&lt;LineBreak/&gt;
-300 = 1st Lieutenant&lt;LineBreak/&gt;
-400 = Captian
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>e051</t>
   </si>
   <si>
@@ -1681,25 +1669,38 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;e503 End Game Statistics and Feats &lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e061 Crew Switch&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The assistant driver moves through the tank to replace the incapacitated crewman. The assistant driver takes on the role but at half rating unless switching with Driver. Click image to  continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                                 &lt;InlineUIContainer&gt;&lt;Image Name='CarryingMan' Height='200' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e102 Evening Debriefing - Promotions&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.93' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r25.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You are promoted when promotion points reach these values. However, cannot be promoted faster than once per month:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+100 = Staff Sergeant&lt;LineBreak/&gt;
+200 = 2nd Lieutenant&lt;LineBreak/&gt;
+300 = 1st Lieutenant&lt;LineBreak/&gt;
+400 = Captain
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e007b Crew Replacement&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;     
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When you tank is knocked out, wounded crewmen are replaced in the first morning briefing that occurs as a result of a Combat Calender check
-&lt;InlineUIContainer&gt;&lt;Button Content='e006' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue to Combat Calender Check.  
+When you tank is knocked out, wounded crewmen are replaced automatically on the next After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='e006' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue.  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                           &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance3' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e503 End Game Statistics and Feats &lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e061 Crew Switch&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The assistant driver moves through the tank to replace the incapacitated crewman. The assistant driver takes on the role but at half rating unless switching with Driver. Click image to  continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                                 &lt;InlineUIContainer&gt;&lt;Image Name='CarryingMan' Height='200' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -2065,8 +2066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,7 +2081,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2088,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2096,7 +2097,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2104,7 +2105,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2112,7 +2113,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2120,15 +2121,15 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2136,79 +2137,79 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2216,12 +2217,12 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>57</v>
@@ -2232,7 +2233,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -2240,7 +2241,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2248,15 +2249,15 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2272,15 +2273,15 @@
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2288,7 +2289,7 @@
         <v>20</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2357,18 +2358,18 @@
     </row>
     <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2408,7 +2409,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2429,10 +2430,10 @@
     </row>
     <row r="45" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2461,10 +2462,10 @@
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2496,15 +2497,15 @@
         <v>58</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2512,7 +2513,7 @@
         <v>66</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2520,31 +2521,31 @@
         <v>67</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2552,7 +2553,7 @@
         <v>68</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2560,7 +2561,7 @@
         <v>69</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2568,7 +2569,7 @@
         <v>70</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2648,7 +2649,7 @@
         <v>73</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2656,7 +2657,7 @@
         <v>74</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2664,7 +2665,7 @@
         <v>80</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -2672,7 +2673,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2680,7 +2681,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2688,7 +2689,7 @@
         <v>81</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2696,7 +2697,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -2704,319 +2705,319 @@
         <v>65</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -3029,10 +3030,10 @@
     </row>
     <row r="120" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3040,7 +3041,7 @@
         <v>97</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -3048,7 +3049,7 @@
         <v>98</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>104</v>
+        <v>254</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -3088,7 +3089,7 @@
         <v>6</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removed automatic refeuling at end of battle.  Fix problem with MarderIII being counted as MarderII. Fix some problems in Combat Calender.  Show Historical Battle on e006
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B930F5DE-59BD-4931-8162-FDDD3F5F9B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF501CA9-D572-42F3-8020-A4A4840A1892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1192,17 +1191,6 @@
                                             &lt;InlineUIContainer&gt;&lt;Image Name='Continue06b' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e006a Retrofit Period&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-During the periods on the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- marked Refitting, the Division is building itself back up to strength, replacing tanks, and retraining crews. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-During a refit period, you have the option of replacing your current tank per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r24.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e006c Retrofit Period - Gyrostabilizer&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1701,6 +1689,18 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='e006' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue.  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                           &lt;InlineUIContainer&gt;&lt;Image Name='Ambulance3' Height='160' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e006a Retrofit Period&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During the periods on the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ marked Refitting, the Division is building itself back up to strength, replacing tanks, and retraining crews. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During a refit period, you have the option of replacing your current tank per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r24.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+If the refit period is over 7 days, the crew goes through additional training resulting in possilbe crew rating improvements.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2066,8 +2066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2081,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2105,7 +2105,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2113,7 +2113,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2121,15 +2121,15 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2137,15 +2137,15 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>192</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>196</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2161,7 +2161,7 @@
         <v>194</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2177,7 +2177,7 @@
         <v>182</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2206,10 +2206,10 @@
     </row>
     <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2217,7 +2217,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2233,7 +2233,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2249,15 +2249,15 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2358,18 +2358,18 @@
     </row>
     <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2409,7 +2409,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2462,10 +2462,10 @@
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2502,10 +2502,10 @@
     </row>
     <row r="54" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2521,7 +2521,7 @@
         <v>67</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -2561,7 +2561,7 @@
         <v>69</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2569,7 +2569,7 @@
         <v>70</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2705,7 +2705,7 @@
         <v>65</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2713,7 +2713,7 @@
         <v>138</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2721,7 +2721,7 @@
         <v>139</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2729,7 +2729,7 @@
         <v>140</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2742,10 +2742,10 @@
     </row>
     <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2761,7 +2761,7 @@
         <v>136</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2793,7 +2793,7 @@
         <v>115</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -2857,7 +2857,7 @@
         <v>149</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -2902,34 +2902,34 @@
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2969,7 +2969,7 @@
         <v>174</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2998,26 +2998,26 @@
     </row>
     <row r="116" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -3033,7 +3033,7 @@
         <v>160</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3041,7 +3041,7 @@
         <v>97</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
         <v>98</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -3089,7 +3089,7 @@
         <v>6</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix error with weather deep snow
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF501CA9-D572-42F3-8020-A4A4840A1892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF6F3BC5-243D-4D75-9C94-3BA5939C7C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -1408,16 +1408,6 @@
     <t>e005a</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e101 Evening Debriefing - Victory Point Total&lt;/Bold&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.92' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-&lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-updated to reflect victory points for both your tank and friendly forces. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e054b MG Firing - Advancing Fire&lt;/Bold&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   
 &lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -1701,6 +1691,15 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r24.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
 If the refit period is over 7 days, the crew goes through additional training resulting in possilbe crew rating improvements.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e101 Evening Debriefing - Victory Point Total&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.92' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+updated to reflect victory points for both your tank and friendly forces. </t>
   </si>
 </sst>
 </file>
@@ -2066,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2080,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -2129,7 +2128,7 @@
         <v>220</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -2145,7 +2144,7 @@
         <v>192</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2177,7 +2176,7 @@
         <v>182</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2241,7 +2240,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2249,7 +2248,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2257,7 +2256,7 @@
         <v>199</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2358,18 +2357,18 @@
     </row>
     <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -2561,7 +2560,7 @@
         <v>69</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -2569,7 +2568,7 @@
         <v>70</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2705,7 +2704,7 @@
         <v>65</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -2713,7 +2712,7 @@
         <v>138</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2721,7 +2720,7 @@
         <v>139</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2729,7 +2728,7 @@
         <v>140</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2742,10 +2741,10 @@
     </row>
     <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="120" x14ac: